<commit_message>
Updated code on timestamp:   23-05-2021 - 15:14:05.07
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -1909,9 +1909,6 @@
     <t>wrong code update it</t>
   </si>
   <si>
-    <t>if you used stack , then it will be used for depth traversal</t>
-  </si>
-  <si>
     <t>This can be done using stack 
 stack- add fist element 
 RPA
@@ -1923,12 +1920,6 @@
   <si>
     <t>[root ]- (children…..)
 we are giving preference to children</t>
-  </si>
-  <si>
-    <t>queue - add first 
-RPA
-we are giving preference to siblings
-it display in single line</t>
   </si>
   <si>
     <t>CP/TraversalInGenericTree.java at main · spartan4cs/CP (github.com)</t>
@@ -2036,6 +2027,37 @@
 You can find height of tree using this appraoch3)
 aur ek level pe jyada freedom and ocntrol he</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">queue - add first 
+RPA
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>we are giving preference to siblings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+it display in single line</t>
+    </r>
+  </si>
+  <si>
+    <t>if you used stack , then it will be used for depth traversal, ans we rill give more prefrerence to children</t>
   </si>
 </sst>
 </file>
@@ -2683,9 +2705,6 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="14" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2693,9 +2712,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -2739,6 +2755,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3098,14 +3120,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="124" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="107"/>
-      <c r="J2" s="108" t="s">
+      <c r="G2" s="124"/>
+      <c r="J2" s="106" t="s">
         <v>328</v>
       </c>
-      <c r="K2" s="108"/>
+      <c r="K2" s="106"/>
     </row>
     <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -6626,15 +6648,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="125" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7396,7 +7418,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="103" t="s">
         <v>546</v>
       </c>
       <c r="E1" s="5">
@@ -7406,32 +7428,32 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="104" t="s">
         <v>547</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="104" t="s">
         <v>548</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="D3" s="104"/>
+      <c r="D3" s="103"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="D4" s="104"/>
+      <c r="D4" s="103"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="D5" s="104"/>
+      <c r="D5" s="103"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="D6" s="104"/>
+      <c r="D6" s="103"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7687,7 +7709,7 @@
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="102" t="s">
+      <c r="D19" s="101" t="s">
         <v>251</v>
       </c>
       <c r="E19" t="s">
@@ -7729,7 +7751,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>13</v>
       </c>
@@ -7880,7 +7902,7 @@
       <c r="G27" s="5">
         <v>1</v>
       </c>
-      <c r="H27" s="112" t="s">
+      <c r="H27" s="110" t="s">
         <v>562</v>
       </c>
       <c r="K27" s="16" t="s">
@@ -7931,7 +7953,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="110" t="s">
+      <c r="D30" s="108" t="s">
         <v>261</v>
       </c>
       <c r="E30" t="s">
@@ -7954,7 +7976,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="109" t="s">
+      <c r="D31" s="107" t="s">
         <v>262</v>
       </c>
       <c r="E31" t="s">
@@ -7983,7 +8005,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="107" t="s">
         <v>263</v>
       </c>
       <c r="E32" t="s">
@@ -8009,7 +8031,7 @@
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="111" t="s">
+      <c r="D33" s="109" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -8035,7 +8057,7 @@
       <c r="C34" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="102" t="s">
         <v>540</v>
       </c>
       <c r="E34" t="s">
@@ -8250,7 +8272,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8307,13 +8329,13 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="108" t="s">
-        <v>572</v>
-      </c>
-      <c r="C4" s="116" t="s">
+      <c r="B4" s="106" t="s">
+        <v>570</v>
+      </c>
+      <c r="C4" s="114" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="106"/>
+      <c r="F4" s="105"/>
       <c r="J4" s="16" t="s">
         <v>557</v>
       </c>
@@ -8322,13 +8344,13 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="108" t="s">
-        <v>572</v>
-      </c>
-      <c r="C5" s="117" t="s">
+      <c r="B5" s="106" t="s">
+        <v>570</v>
+      </c>
+      <c r="C5" s="115" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="106"/>
+      <c r="F5" s="105"/>
       <c r="J5" s="16" t="s">
         <v>557</v>
       </c>
@@ -8337,23 +8359,23 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="116" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="105">
         <v>2</v>
       </c>
-      <c r="G6" s="113" t="s">
+      <c r="G6" s="111" t="s">
+        <v>564</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>566</v>
-      </c>
       <c r="I6" s="10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>557</v>
@@ -8363,13 +8385,13 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="116" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F7" s="105">
         <v>2</v>
       </c>
       <c r="G7" t="s">
@@ -8386,13 +8408,13 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="118" t="s">
+      <c r="C8" s="116" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F8" s="105">
         <v>2</v>
       </c>
       <c r="G8" t="s">
@@ -8409,13 +8431,13 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="116" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="105">
         <v>2</v>
       </c>
       <c r="G9" t="s">
@@ -8438,46 +8460,46 @@
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="105">
         <v>2</v>
       </c>
-      <c r="G10" s="115" t="s">
+      <c r="G10" s="113" t="s">
         <v>497</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>561</v>
       </c>
       <c r="I10" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="116" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="105">
         <v>2</v>
       </c>
-      <c r="G11" s="114" t="s">
-        <v>573</v>
+      <c r="G11" s="112" t="s">
+        <v>571</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="J11" s="16" t="s">
         <v>567</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>563</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -8487,39 +8509,39 @@
       <c r="B12" t="s">
         <v>543</v>
       </c>
-      <c r="C12" s="118" t="s">
+      <c r="C12" s="116" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="106">
+      <c r="F12" s="105">
         <v>2</v>
       </c>
       <c r="G12" t="s">
+        <v>572</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>576</v>
-      </c>
       <c r="I12" s="10" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="118" t="s">
+      <c r="C13" s="116" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="106">
+      <c r="F13" s="105">
         <v>2</v>
       </c>
       <c r="G13" t="s">
@@ -8529,17 +8551,17 @@
         <v>561</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="108" t="s">
-        <v>572</v>
-      </c>
-      <c r="C14" s="119" t="s">
+      <c r="B14" s="106" t="s">
+        <v>570</v>
+      </c>
+      <c r="C14" s="117" t="s">
         <v>221</v>
       </c>
       <c r="G14" s="18"/>
@@ -8548,7 +8570,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="120" t="s">
+      <c r="C15" s="118" t="s">
         <v>222</v>
       </c>
     </row>
@@ -8556,7 +8578,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="119" t="s">
         <v>223</v>
       </c>
     </row>
@@ -8564,7 +8586,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="119" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8572,7 +8594,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="121" t="s">
+      <c r="C18" s="119" t="s">
         <v>225</v>
       </c>
     </row>
@@ -8580,7 +8602,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="121" t="s">
+      <c r="C19" s="119" t="s">
         <v>226</v>
       </c>
     </row>
@@ -8588,7 +8610,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="121" t="s">
+      <c r="C20" s="119" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8596,7 +8618,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="119" t="s">
         <v>228</v>
       </c>
     </row>
@@ -8604,7 +8626,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="121" t="s">
+      <c r="C22" s="119" t="s">
         <v>229</v>
       </c>
     </row>
@@ -8612,7 +8634,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="120" t="s">
         <v>230</v>
       </c>
     </row>
@@ -8620,7 +8642,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="121" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8628,7 +8650,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="124" t="s">
+      <c r="C25" s="122" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8636,7 +8658,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="124" t="s">
+      <c r="C26" s="122" t="s">
         <v>233</v>
       </c>
     </row>
@@ -8644,7 +8666,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="124" t="s">
+      <c r="C27" s="122" t="s">
         <v>234</v>
       </c>
     </row>
@@ -8652,7 +8674,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="124" t="s">
+      <c r="C28" s="122" t="s">
         <v>235</v>
       </c>
     </row>
@@ -8660,7 +8682,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="124" t="s">
+      <c r="C29" s="122" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8668,7 +8690,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="124" t="s">
+      <c r="C30" s="122" t="s">
         <v>237</v>
       </c>
     </row>
@@ -8676,7 +8698,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="124" t="s">
+      <c r="C31" s="122" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8684,7 +8706,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="124" t="s">
+      <c r="C32" s="122" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8692,7 +8714,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="C33" s="125" t="s">
+      <c r="C33" s="123" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 15:48:26.29
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -8271,8 +8271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 16:17:21.42
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -1904,9 +1904,6 @@
   </si>
   <si>
     <t>level-option</t>
-  </si>
-  <si>
-    <t>wrong code update it</t>
   </si>
   <si>
     <t>This can be done using stack 
@@ -2058,6 +2055,9 @@
   </si>
   <si>
     <t>if you used stack , then it will be used for depth traversal, ans we rill give more prefrerence to children</t>
+  </si>
+  <si>
+    <t>can be done using pointer appro0ch check the leetcode solution</t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2421,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2718,7 +2718,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2762,6 +2761,8 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3120,10 +3121,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="123" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="124"/>
+      <c r="G2" s="123"/>
       <c r="J2" s="106" t="s">
         <v>328</v>
       </c>
@@ -3980,7 +3981,7 @@
   <dimension ref="A4:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5192,7 +5193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -5723,7 +5724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6648,15 +6649,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="124" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7398,8 +7399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7774,7 +7775,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>14</v>
       </c>
@@ -7797,11 +7798,11 @@
         <v>520</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="101" t="s">
         <v>255</v>
       </c>
       <c r="E23" t="s">
@@ -7818,6 +7819,9 @@
       </c>
       <c r="I23" t="s">
         <v>501</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>577</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>500</v>
@@ -7902,9 +7906,7 @@
       <c r="G27" s="5">
         <v>1</v>
       </c>
-      <c r="H27" s="110" t="s">
-        <v>562</v>
-      </c>
+      <c r="H27" s="125"/>
       <c r="K27" s="16" t="s">
         <v>523</v>
       </c>
@@ -7933,7 +7935,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="126" t="s">
         <v>260</v>
       </c>
       <c r="E29" t="s">
@@ -8271,8 +8273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8330,9 +8332,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>570</v>
-      </c>
-      <c r="C4" s="114" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="113" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="105"/>
@@ -8345,9 +8347,9 @@
         <v>2</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>570</v>
-      </c>
-      <c r="C5" s="115" t="s">
+        <v>569</v>
+      </c>
+      <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="105"/>
@@ -8359,7 +8361,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="115" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
@@ -8368,14 +8370,14 @@
       <c r="F6" s="105">
         <v>2</v>
       </c>
-      <c r="G6" s="111" t="s">
+      <c r="G6" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>565</v>
-      </c>
       <c r="I6" s="10" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>557</v>
@@ -8385,7 +8387,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="115" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
@@ -8408,7 +8410,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="115" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
@@ -8431,7 +8433,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="115" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
@@ -8463,24 +8465,24 @@
       <c r="F10" s="105">
         <v>2</v>
       </c>
-      <c r="G10" s="113" t="s">
+      <c r="G10" s="112" t="s">
         <v>497</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>561</v>
       </c>
       <c r="I10" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="115" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
@@ -8489,17 +8491,17 @@
       <c r="F11" s="105">
         <v>2</v>
       </c>
-      <c r="G11" s="112" t="s">
-        <v>571</v>
+      <c r="G11" s="111" t="s">
+        <v>570</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>576</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>577</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -8509,7 +8511,7 @@
       <c r="B12" t="s">
         <v>543</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="115" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
@@ -8519,23 +8521,23 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>575</v>
-      </c>
       <c r="J12" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="115" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
@@ -8551,7 +8553,7 @@
         <v>561</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8559,9 +8561,9 @@
         <v>11</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>570</v>
-      </c>
-      <c r="C14" s="117" t="s">
+        <v>569</v>
+      </c>
+      <c r="C14" s="116" t="s">
         <v>221</v>
       </c>
       <c r="G14" s="18"/>
@@ -8570,7 +8572,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="117" t="s">
         <v>222</v>
       </c>
     </row>
@@ -8578,7 +8580,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="118" t="s">
         <v>223</v>
       </c>
     </row>
@@ -8586,7 +8588,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="119" t="s">
+      <c r="C17" s="118" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8594,7 +8596,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="118" t="s">
         <v>225</v>
       </c>
     </row>
@@ -8602,7 +8604,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="119" t="s">
+      <c r="C19" s="118" t="s">
         <v>226</v>
       </c>
     </row>
@@ -8610,7 +8612,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C20" s="118" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8618,7 +8620,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="119" t="s">
+      <c r="C21" s="118" t="s">
         <v>228</v>
       </c>
     </row>
@@ -8626,7 +8628,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="119" t="s">
+      <c r="C22" s="118" t="s">
         <v>229</v>
       </c>
     </row>
@@ -8634,7 +8636,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="120" t="s">
+      <c r="C23" s="119" t="s">
         <v>230</v>
       </c>
     </row>
@@ -8642,7 +8644,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="121" t="s">
+      <c r="C24" s="120" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8650,7 +8652,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="122" t="s">
+      <c r="C25" s="121" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8658,7 +8660,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="121" t="s">
         <v>233</v>
       </c>
     </row>
@@ -8666,7 +8668,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="122" t="s">
+      <c r="C27" s="121" t="s">
         <v>234</v>
       </c>
     </row>
@@ -8674,7 +8676,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="122" t="s">
+      <c r="C28" s="121" t="s">
         <v>235</v>
       </c>
     </row>
@@ -8682,7 +8684,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="122" t="s">
+      <c r="C29" s="121" t="s">
         <v>236</v>
       </c>
     </row>
@@ -8690,7 +8692,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="122" t="s">
+      <c r="C30" s="121" t="s">
         <v>237</v>
       </c>
     </row>
@@ -8698,7 +8700,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="122" t="s">
+      <c r="C31" s="121" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8706,7 +8708,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="122" t="s">
+      <c r="C32" s="121" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8714,7 +8716,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="C33" s="123" t="s">
+      <c r="C33" s="122" t="s">
         <v>240</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 16:28:39.85
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="579">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2058,6 +2058,9 @@
   </si>
   <si>
     <t>can be done using pointer appro0ch check the leetcode solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If j loop is dependent on I then there is high possiblity that we can use stack </t>
   </si>
 </sst>
 </file>
@@ -2421,7 +2424,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2763,6 +2766,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -5722,10 +5728,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5754,80 +5760,63 @@
       </c>
       <c r="I1"/>
     </row>
-    <row r="2" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2" s="127" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="38" t="s">
         <v>349</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="33"/>
-    </row>
-    <row r="3" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="5" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B5" s="56" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>33</v>
@@ -5839,21 +5828,21 @@
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>3</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>336</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>33</v>
@@ -5865,21 +5854,21 @@
         <v>5</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>4</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>336</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -5890,22 +5879,22 @@
       <c r="E7" s="2">
         <v>5</v>
       </c>
+      <c r="F7" s="10" t="s">
+        <v>337</v>
+      </c>
       <c r="G7" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>398</v>
+        <v>338</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>33</v>
@@ -5917,70 +5906,67 @@
         <v>5</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+    <row r="10" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B10" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="70">
+      <c r="C10" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="70">
         <v>5</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I10" s="16" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B11" s="61" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>8</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>33</v>
@@ -5992,21 +5978,24 @@
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>399</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>33</v>
@@ -6018,73 +6007,73 @@
         <v>3</v>
       </c>
       <c r="F12" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>9</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I13" s="16" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+    <row r="14" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B14" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="70">
+      <c r="C14" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="70">
         <v>3</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I14" s="16" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B15" s="63" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>12</v>
-      </c>
-      <c r="B15" s="63" t="s">
-        <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>33</v>
@@ -6095,19 +6084,22 @@
       <c r="E15" s="2">
         <v>3</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>402</v>
+      <c r="G15" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>401</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>33</v>
@@ -6118,19 +6110,19 @@
       <c r="E16" s="2">
         <v>3</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>403</v>
+      <c r="F16" s="10" t="s">
+        <v>402</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>14</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>52</v>
+        <v>13</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>33</v>
@@ -6141,19 +6133,19 @@
       <c r="E17" s="2">
         <v>3</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>404</v>
+      <c r="G17" s="10" t="s">
+        <v>403</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>33</v>
@@ -6164,16 +6156,19 @@
       <c r="E18" s="2">
         <v>3</v>
       </c>
+      <c r="F18" s="10" t="s">
+        <v>404</v>
+      </c>
       <c r="I18" s="16" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>33</v>
@@ -6184,44 +6179,61 @@
       <c r="E19" s="2">
         <v>3</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="I19" s="16" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>16</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H20" s="16" t="s">
         <v>371</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B21" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="67">
+      <c r="C21" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="67">
         <v>3</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G21" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I21" s="16" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
@@ -6229,46 +6241,28 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
     </row>
-    <row r="32" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="38" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="33"/>
+    </row>
+    <row r="34" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
         <v>1</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B34" s="31" t="s">
         <v>346</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>2</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>348</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>208</v>
@@ -6280,22 +6274,19 @@
         <v>0</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="I34" s="31"/>
     </row>
-    <row r="35" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>34</v>
@@ -6304,19 +6295,22 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>347</v>
+        <v>353</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>354</v>
       </c>
       <c r="I35" s="31"/>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>356</v>
+        <v>33</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>34</v>
@@ -6325,17 +6319,13 @@
         <v>0</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="H36" s="59"/>
+        <v>347</v>
+      </c>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>355</v>
@@ -6350,17 +6340,20 @@
         <v>0</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>377</v>
       </c>
       <c r="H37" s="59"/>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>356</v>
@@ -6372,22 +6365,20 @@
         <v>0</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>361</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="H38" s="59"/>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>7</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>373</v>
+        <v>6</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>359</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>208</v>
+        <v>356</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>34</v>
@@ -6396,19 +6387,22 @@
         <v>0</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>375</v>
+        <v>360</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>361</v>
       </c>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>356</v>
+        <v>208</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>34</v>
@@ -6417,19 +6411,16 @@
         <v>0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I40" s="31"/>
     </row>
-    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>356</v>
@@ -6441,22 +6432,22 @@
         <v>0</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="I41" s="31"/>
     </row>
     <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>208</v>
+        <v>356</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>34</v>
@@ -6465,19 +6456,19 @@
         <v>0</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="I42" s="31"/>
     </row>
-    <row r="43" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>208</v>
@@ -6489,22 +6480,19 @@
         <v>0</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>208</v>
@@ -6516,25 +6504,25 @@
         <v>0</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="H44" s="25" t="s">
-        <v>388</v>
-      </c>
-      <c r="I44" s="21"/>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>13</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>393</v>
+        <v>12</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>389</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>34</v>
@@ -6543,78 +6531,105 @@
         <v>0</v>
       </c>
       <c r="F45" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="I45" s="21"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>13</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G46" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="I45" s="16"/>
-    </row>
-    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="I46" s="16"/>
+    </row>
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>14</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B47" s="16" t="s">
         <v>396</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H47" s="10" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+    <row r="48" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
         <v>414</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="16" t="s">
         <v>510</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf"/>
-    <hyperlink ref="B33" r:id="rId2" display="https://leetcode.com/problems/daily-temperatures/"/>
-    <hyperlink ref="B34" r:id="rId3" display="https://leetcode.com/problems/next-greater-element-ii/"/>
-    <hyperlink ref="B35" r:id="rId4" display="https://leetcode.com/problems/next-greater-element-i/"/>
-    <hyperlink ref="B36" r:id="rId5" display="https://leetcode.com/problems/maximal-rectangle/"/>
-    <hyperlink ref="B37" r:id="rId6" display="https://leetcode.com/problems/maximal-rectangle/"/>
-    <hyperlink ref="B38" r:id="rId7" display="https://leetcode.com/problems/sliding-window-maximum/submissions/"/>
-    <hyperlink ref="B40" r:id="rId8" display="https://leetcode.com/problems/basic-calculator/"/>
-    <hyperlink ref="B39" r:id="rId9" display="https://leetcode.com/problems/basic-calculator-ii/"/>
-    <hyperlink ref="B41" r:id="rId10" display="https://leetcode.com/problems/longest-valid-parentheses/"/>
-    <hyperlink ref="B42" r:id="rId11" display="https://leetcode.com/problems/container-with-most-water/"/>
-    <hyperlink ref="B43" r:id="rId12" display="https://leetcode.com/problems/simplify-path/"/>
-    <hyperlink ref="B44" r:id="rId13" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string-ii/"/>
-    <hyperlink ref="B45" r:id="rId14" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/"/>
-    <hyperlink ref="B46" r:id="rId15" display="https://leetcode.com/problems/maximum-frequency-stack/"/>
-    <hyperlink ref="H19" r:id="rId16" display="https://leetcode.com/problems/min-stack/"/>
-    <hyperlink ref="B47" r:id="rId17" display="https://leetcode.com/problems/trapping-rain-water/"/>
-    <hyperlink ref="B48" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/"/>
+    <hyperlink ref="B34" r:id="rId2" display="https://leetcode.com/problems/daily-temperatures/"/>
+    <hyperlink ref="B35" r:id="rId3" display="https://leetcode.com/problems/next-greater-element-ii/"/>
+    <hyperlink ref="B36" r:id="rId4" display="https://leetcode.com/problems/next-greater-element-i/"/>
+    <hyperlink ref="B37" r:id="rId5" display="https://leetcode.com/problems/maximal-rectangle/"/>
+    <hyperlink ref="B38" r:id="rId6" display="https://leetcode.com/problems/maximal-rectangle/"/>
+    <hyperlink ref="B39" r:id="rId7" display="https://leetcode.com/problems/sliding-window-maximum/submissions/"/>
+    <hyperlink ref="B41" r:id="rId8" display="https://leetcode.com/problems/basic-calculator/"/>
+    <hyperlink ref="B40" r:id="rId9" display="https://leetcode.com/problems/basic-calculator-ii/"/>
+    <hyperlink ref="B42" r:id="rId10" display="https://leetcode.com/problems/longest-valid-parentheses/"/>
+    <hyperlink ref="B43" r:id="rId11" display="https://leetcode.com/problems/container-with-most-water/"/>
+    <hyperlink ref="B44" r:id="rId12" display="https://leetcode.com/problems/simplify-path/"/>
+    <hyperlink ref="B45" r:id="rId13" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string-ii/"/>
+    <hyperlink ref="B46" r:id="rId14" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/"/>
+    <hyperlink ref="B47" r:id="rId15" display="https://leetcode.com/problems/maximum-frequency-stack/"/>
+    <hyperlink ref="H20" r:id="rId16" display="https://leetcode.com/problems/min-stack/"/>
+    <hyperlink ref="B48" r:id="rId17" display="https://leetcode.com/problems/trapping-rain-water/"/>
+    <hyperlink ref="B49" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/"/>
     <hyperlink ref="G1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues"/>
-    <hyperlink ref="I4" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java"/>
-    <hyperlink ref="I7" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java"/>
-    <hyperlink ref="I8" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java"/>
-    <hyperlink ref="I9" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java"/>
-    <hyperlink ref="I5" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java"/>
-    <hyperlink ref="I14" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java"/>
-    <hyperlink ref="I15" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java"/>
-    <hyperlink ref="I12" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java"/>
-    <hyperlink ref="I13" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java"/>
-    <hyperlink ref="I10" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java"/>
-    <hyperlink ref="I11" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java"/>
-    <hyperlink ref="I16" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java"/>
-    <hyperlink ref="I17" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java"/>
-    <hyperlink ref="I18" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
-    <hyperlink ref="I19" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
-    <hyperlink ref="I20" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
-    <hyperlink ref="B49" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/"/>
-    <hyperlink ref="I6" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
+    <hyperlink ref="I5" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java"/>
+    <hyperlink ref="I8" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java"/>
+    <hyperlink ref="I9" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java"/>
+    <hyperlink ref="I10" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java"/>
+    <hyperlink ref="I6" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java"/>
+    <hyperlink ref="I15" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java"/>
+    <hyperlink ref="I16" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java"/>
+    <hyperlink ref="I13" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java"/>
+    <hyperlink ref="I14" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java"/>
+    <hyperlink ref="I11" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java"/>
+    <hyperlink ref="I12" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java"/>
+    <hyperlink ref="I17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java"/>
+    <hyperlink ref="I18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java"/>
+    <hyperlink ref="I19" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
+    <hyperlink ref="I20" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
+    <hyperlink ref="I21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
+    <hyperlink ref="B50" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/"/>
+    <hyperlink ref="I7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>
@@ -7399,7 +7414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 17:00:32.65
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2424,7 +2424,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2764,7 +2764,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3110,7 +3109,7 @@
   <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,8 +5729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5762,7 +5761,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="126" t="s">
         <v>578</v>
       </c>
       <c r="C2" s="16"/>
@@ -7414,8 +7413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7827,7 +7826,7 @@
         <v>34</v>
       </c>
       <c r="G23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>499</v>
@@ -7856,7 +7855,7 @@
         <v>34</v>
       </c>
       <c r="G24" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>502</v>
@@ -7876,7 +7875,7 @@
         <v>34</v>
       </c>
       <c r="G25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>503</v>
@@ -7899,7 +7898,7 @@
         <v>34</v>
       </c>
       <c r="G26" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>515</v>
@@ -7919,9 +7918,8 @@
         <v>34</v>
       </c>
       <c r="G27" s="5">
-        <v>1</v>
-      </c>
-      <c r="H27" s="125"/>
+        <v>2</v>
+      </c>
       <c r="K27" s="16" t="s">
         <v>523</v>
       </c>
@@ -7940,7 +7938,7 @@
         <v>34</v>
       </c>
       <c r="G28" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>534</v>
@@ -7950,7 +7948,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="126" t="s">
+      <c r="D29" s="125" t="s">
         <v>260</v>
       </c>
       <c r="E29" t="s">
@@ -7960,7 +7958,7 @@
         <v>34</v>
       </c>
       <c r="G29" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>535</v>
@@ -7980,7 +7978,7 @@
         <v>34</v>
       </c>
       <c r="G30" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>524</v>
@@ -8003,7 +8001,7 @@
         <v>34</v>
       </c>
       <c r="G31" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>537</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   23-05-2021 - 20:59:04.26
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -1886,9 +1886,6 @@
   </si>
   <si>
     <t>CP/CopyLLwithRandomnumbers.java at main · spartan4cs/CP (github.com)</t>
-  </si>
-  <si>
-    <t>concept</t>
   </si>
   <si>
     <t>CP/GenericTreeDemo.java at main · spartan4cs/CP (github.com)</t>
@@ -2061,6 +2058,9 @@
   </si>
   <si>
     <t xml:space="preserve">If j loop is dependent on I then there is high possiblity that we can use stack </t>
+  </si>
+  <si>
+    <t>require 2 stack</t>
   </si>
 </sst>
 </file>
@@ -5762,7 +5762,7 @@
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="126" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C2" s="16"/>
       <c r="G2" s="16"/>
@@ -7413,8 +7413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7835,7 +7835,7 @@
         <v>501</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>500</v>
@@ -8286,8 +8286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8345,14 +8345,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C4" s="113" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="105"/>
       <c r="J4" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8360,14 +8360,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="105"/>
       <c r="J5" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8384,16 +8384,16 @@
         <v>2</v>
       </c>
       <c r="G6" s="110" t="s">
+        <v>562</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>564</v>
-      </c>
       <c r="I6" s="10" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8413,10 +8413,10 @@
         <v>497</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8436,10 +8436,10 @@
         <v>497</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8459,10 +8459,10 @@
         <v>497</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8482,13 +8482,13 @@
         <v>497</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I10" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8505,16 +8505,16 @@
         <v>2</v>
       </c>
       <c r="G11" s="111" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>576</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -8534,16 +8534,16 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>574</v>
-      </c>
       <c r="J12" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -8560,13 +8560,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>556</v>
+        <v>578</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8574,7 +8574,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>221</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   24-05-2021 -  2:55:12.13
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="580">
   <si>
     <t>TOPIC</t>
   </si>
@@ -826,9 +826,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Linearize A Generic Tree - Efficient Approach</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Find In Generic Tree </t>
   </si>
   <si>
     <t xml:space="preserve"> Node To Root Path In Generic Tree </t>
@@ -2062,12 +2059,18 @@
   <si>
     <t>require 2 stack</t>
   </si>
+  <si>
+    <t>Leet code</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Find element In Generic Tree </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2154,6 +2157,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2424,7 +2434,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2767,6 +2777,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3131,7 +3148,7 @@
       </c>
       <c r="G2" s="123"/>
       <c r="J2" s="106" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K2" s="106"/>
     </row>
@@ -3149,15 +3166,15 @@
         <v>48</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>527</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>528</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>529</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -3165,7 +3182,7 @@
     </row>
     <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -3177,12 +3194,12 @@
         <v>97</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>124</v>
@@ -3201,7 +3218,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
@@ -3270,7 +3287,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3290,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3298,7 +3315,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3306,7 +3323,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3314,7 +3331,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3322,7 +3339,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3330,7 +3347,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3338,7 +3355,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3346,7 +3363,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="95" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3354,7 +3371,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3362,7 +3379,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="95" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3370,7 +3387,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3378,7 +3395,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3386,7 +3403,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="82" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3394,7 +3411,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,7 +3419,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,7 +3427,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,7 +3435,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="82" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,7 +3443,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3434,7 +3451,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3442,7 +3459,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3494,7 +3511,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3514,7 +3531,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="96" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3522,7 +3539,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="96" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3530,7 +3547,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="96" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3538,7 +3555,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="96" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3546,7 +3563,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="96" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3554,7 +3571,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3562,7 +3579,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="96" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3570,7 +3587,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3578,7 +3595,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="96" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3586,7 +3603,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="96" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3638,7 +3655,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3658,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3666,7 +3683,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3674,7 +3691,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3682,7 +3699,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3690,7 +3707,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3698,7 +3715,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3706,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="95" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3714,7 +3731,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="95" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3722,7 +3739,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3730,7 +3747,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="95" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3738,7 +3755,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3746,7 +3763,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3754,7 +3771,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="82" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3762,7 +3779,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -3817,7 +3834,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -3837,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3845,7 +3862,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3853,7 +3870,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3861,7 +3878,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3869,7 +3886,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3877,7 +3894,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="95" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3885,7 +3902,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="95" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3893,7 +3910,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="95" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3901,7 +3918,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="95" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3909,7 +3926,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="95" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3917,7 +3934,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3925,7 +3942,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3933,7 +3950,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="82" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3941,7 +3958,7 @@
         <v>14</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,7 +3966,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,7 +3974,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3965,7 +3982,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="82" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3973,7 +3990,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -4004,16 +4021,16 @@
         <v>51</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -4030,13 +4047,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4044,21 +4061,21 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J6" s="10"/>
     </row>
@@ -4067,11 +4084,11 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -4080,7 +4097,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="10"/>
       <c r="I7" s="16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -4089,24 +4106,24 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="79" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>476</v>
-      </c>
       <c r="I8" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J8" s="10"/>
     </row>
@@ -4115,56 +4132,56 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G9" s="90" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="G10" t="s">
         <v>496</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" s="16" t="s">
         <v>497</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C11" t="s">
         <v>208</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="F11" t="s">
         <v>530</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" s="16" t="s">
         <v>531</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4288,7 +4305,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>38</v>
@@ -4616,10 +4633,10 @@
         <v>100</v>
       </c>
       <c r="I14" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>434</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>435</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>98</v>
@@ -4648,7 +4665,7 @@
         <v>100</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4674,7 +4691,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4700,10 +4717,10 @@
         <v>100</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5222,7 +5239,7 @@
         <v>116</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -5256,7 +5273,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -5273,7 +5290,7 @@
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D4" s="25" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K4" s="16"/>
     </row>
@@ -5300,7 +5317,7 @@
         <v>105</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5326,7 +5343,7 @@
         <v>71</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -5346,7 +5363,7 @@
         <v>67</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -5369,7 +5386,7 @@
         <v>146</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5403,10 +5420,10 @@
         <v>2</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -5426,7 +5443,7 @@
         <v>145</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -5443,7 +5460,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>148</v>
@@ -5452,7 +5469,7 @@
         <v>147</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -5475,10 +5492,10 @@
         <v>169</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5486,7 +5503,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="80" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D15" s="81" t="s">
         <v>151</v>
@@ -5498,16 +5515,16 @@
         <v>2</v>
       </c>
       <c r="H15" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="I15" s="15" t="s">
         <v>477</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>478</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>152</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -5530,7 +5547,7 @@
         <v>155</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -5553,7 +5570,7 @@
         <v>165</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="195" x14ac:dyDescent="0.25">
@@ -5576,7 +5593,7 @@
         <v>158</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -5599,7 +5616,7 @@
         <v>171</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5619,7 +5636,7 @@
         <v>164</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5639,7 +5656,7 @@
         <v>167</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5659,7 +5676,7 @@
         <v>173</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -5670,7 +5687,7 @@
         <v>174</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -5752,17 +5769,17 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="126" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C2" s="16"/>
       <c r="G2" s="16"/>
@@ -5771,7 +5788,7 @@
     <row r="3" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
       <c r="B3" s="38" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -5795,7 +5812,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -5827,13 +5844,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -5853,13 +5870,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -5867,7 +5884,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -5879,13 +5896,13 @@
         <v>5</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>338</v>
-      </c>
       <c r="I7" s="16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -5905,13 +5922,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>339</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5931,10 +5948,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>341</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5954,10 +5971,10 @@
         <v>5</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>350</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -5977,16 +5994,16 @@
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6006,13 +6023,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6032,13 +6049,13 @@
         <v>3</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6058,13 +6075,13 @@
         <v>3</v>
       </c>
       <c r="F14" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>369</v>
-      </c>
       <c r="I14" s="16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -6084,13 +6101,13 @@
         <v>3</v>
       </c>
       <c r="G15" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>401</v>
-      </c>
       <c r="I15" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6110,10 +6127,10 @@
         <v>3</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6133,10 +6150,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6156,10 +6173,10 @@
         <v>3</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -6179,7 +6196,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6199,16 +6216,16 @@
         <v>3</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6228,10 +6245,10 @@
         <v>3</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -6246,7 +6263,7 @@
     <row r="33" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -6261,7 +6278,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>208</v>
@@ -6273,7 +6290,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I34" s="31"/>
     </row>
@@ -6282,7 +6299,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>208</v>
@@ -6294,10 +6311,10 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="G35" s="10" t="s">
         <v>353</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>354</v>
       </c>
       <c r="I35" s="31"/>
     </row>
@@ -6306,7 +6323,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>33</v>
@@ -6318,7 +6335,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I36" s="31"/>
     </row>
@@ -6327,10 +6344,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>356</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>34</v>
@@ -6339,10 +6356,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H37" s="59"/>
       <c r="I37" s="31"/>
@@ -6352,10 +6369,10 @@
         <v>5</v>
       </c>
       <c r="B38" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>356</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>34</v>
@@ -6364,7 +6381,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H38" s="59"/>
       <c r="I38" s="31"/>
@@ -6374,10 +6391,10 @@
         <v>6</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>34</v>
@@ -6386,10 +6403,10 @@
         <v>0</v>
       </c>
       <c r="F39" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>360</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>361</v>
       </c>
       <c r="I39" s="31"/>
     </row>
@@ -6398,7 +6415,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>208</v>
@@ -6410,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I40" s="31"/>
     </row>
@@ -6419,10 +6436,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>34</v>
@@ -6431,10 +6448,10 @@
         <v>0</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I41" s="31"/>
     </row>
@@ -6443,10 +6460,10 @@
         <v>9</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>34</v>
@@ -6455,10 +6472,10 @@
         <v>0</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I42" s="31"/>
     </row>
@@ -6467,7 +6484,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>208</v>
@@ -6479,10 +6496,10 @@
         <v>0</v>
       </c>
       <c r="F43" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>382</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>383</v>
       </c>
       <c r="I43" s="31"/>
     </row>
@@ -6491,7 +6508,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>208</v>
@@ -6503,13 +6520,13 @@
         <v>0</v>
       </c>
       <c r="F44" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="G44" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="G44" s="10" t="s">
-        <v>387</v>
-      </c>
       <c r="H44" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I44" s="31"/>
     </row>
@@ -6518,7 +6535,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>208</v>
@@ -6530,13 +6547,13 @@
         <v>0</v>
       </c>
       <c r="F45" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="G45" s="10" t="s">
-        <v>391</v>
-      </c>
       <c r="H45" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I45" s="21"/>
     </row>
@@ -6545,7 +6562,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>33</v>
@@ -6557,10 +6574,10 @@
         <v>0</v>
       </c>
       <c r="F46" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>394</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>395</v>
       </c>
       <c r="I46" s="16"/>
     </row>
@@ -6569,25 +6586,25 @@
         <v>14</v>
       </c>
       <c r="B47" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="H47" s="10" t="s">
         <v>396</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -6658,13 +6675,13 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A2" s="124" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B2" s="124"/>
       <c r="C2" s="124"/>
@@ -6688,7 +6705,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -6708,7 +6725,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -6720,12 +6737,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
       <c r="I4" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -6742,7 +6759,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
       <c r="I5" s="16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -6765,7 +6782,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6788,7 +6805,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6811,7 +6828,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
       <c r="I8" s="16" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -6834,7 +6851,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
       <c r="I9" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6855,11 +6872,11 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="77" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6867,36 +6884,36 @@
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>407</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>408</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="74" t="s">
+        <v>408</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>410</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -6967,7 +6984,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -7398,7 +7415,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -7434,7 +7451,7 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="103" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E1" s="5">
         <v>0</v>
@@ -7444,10 +7461,10 @@
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="104" t="s">
+        <v>546</v>
+      </c>
+      <c r="E2" s="104" t="s">
         <v>547</v>
-      </c>
-      <c r="E2" s="104" t="s">
-        <v>548</v>
       </c>
       <c r="G2"/>
     </row>
@@ -7491,7 +7508,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>38</v>
@@ -7508,7 +7525,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -7516,7 +7533,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -7528,7 +7545,7 @@
         <v>2</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -7536,7 +7553,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="98" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E10" t="s">
         <v>33</v>
@@ -7548,7 +7565,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7556,7 +7573,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="98" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -7568,7 +7585,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -7576,7 +7593,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="98" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -7588,7 +7605,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -7596,7 +7613,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="98" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -7608,7 +7625,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -7616,7 +7633,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="98" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -7628,7 +7645,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7636,7 +7653,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -7648,7 +7665,7 @@
         <v>2</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -7656,7 +7673,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="98" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -7668,7 +7685,7 @@
         <v>2</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -7676,7 +7693,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="98" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -7688,13 +7705,13 @@
         <v>2</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7702,7 +7719,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="99" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E18" t="s">
         <v>33</v>
@@ -7714,10 +7731,10 @@
         <v>2</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7725,7 +7742,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="101" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
@@ -7737,10 +7754,10 @@
         <v>2</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -7748,7 +7765,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
@@ -7760,10 +7777,10 @@
         <v>2</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -7771,7 +7788,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -7783,10 +7800,10 @@
         <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7794,7 +7811,7 @@
         <v>14</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -7806,10 +7823,10 @@
         <v>2</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7817,7 +7834,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="101" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -7829,16 +7846,16 @@
         <v>2</v>
       </c>
       <c r="H23" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="I23" t="s">
+        <v>500</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>575</v>
+      </c>
+      <c r="K23" s="16" t="s">
         <v>499</v>
-      </c>
-      <c r="I23" t="s">
-        <v>501</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>576</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -7846,7 +7863,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -7858,7 +7875,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -7866,7 +7883,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -7878,10 +7895,10 @@
         <v>2</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -7901,7 +7918,7 @@
         <v>2</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -7909,7 +7926,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -7921,7 +7938,7 @@
         <v>2</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -7929,7 +7946,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
@@ -7941,7 +7958,7 @@
         <v>2</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7949,7 +7966,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="125" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
@@ -7961,7 +7978,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -7969,7 +7986,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="108" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E30" t="s">
         <v>33</v>
@@ -7981,10 +7998,10 @@
         <v>2</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -7992,7 +8009,7 @@
         <v>23</v>
       </c>
       <c r="D31" s="107" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" t="s">
         <v>33</v>
@@ -8004,16 +8021,16 @@
         <v>2</v>
       </c>
       <c r="H31" s="18" t="s">
+        <v>536</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="J31" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="K31" s="16" t="s">
         <v>537</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>526</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -8021,7 +8038,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="107" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
@@ -8033,13 +8050,13 @@
         <v>2</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I32" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>549</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8059,10 +8076,10 @@
         <v>2</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8070,10 +8087,10 @@
         <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D34" s="102" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
@@ -8085,10 +8102,10 @@
         <v>2</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -8097,13 +8114,13 @@
     <row r="36" spans="1:11" s="92" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A36" s="91"/>
       <c r="D36" s="93" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G36" s="94"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
@@ -8114,12 +8131,12 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F40" t="s">
         <v>34</v>
@@ -8130,7 +8147,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
@@ -8141,7 +8158,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D42" s="16" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F42" t="s">
         <v>34</v>
@@ -8152,7 +8169,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D43" s="16" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F43" t="s">
         <v>34</v>
@@ -8161,13 +8178,13 @@
         <v>0</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K43" s="16"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D44" s="16" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F44" t="s">
         <v>34</v>
@@ -8178,7 +8195,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D45" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F45" t="s">
         <v>34</v>
@@ -8189,7 +8206,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D46" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F46" t="s">
         <v>34</v>
@@ -8200,10 +8217,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G47" s="5">
         <v>0</v>
@@ -8211,7 +8228,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D48" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -8222,7 +8239,7 @@
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" s="16" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -8284,10 +8301,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8325,7 +8342,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>38</v>
@@ -8345,14 +8362,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C4" s="113" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="105"/>
       <c r="J4" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8360,14 +8377,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="105"/>
       <c r="J5" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8384,16 +8401,16 @@
         <v>2</v>
       </c>
       <c r="G6" s="110" t="s">
+        <v>561</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>563</v>
-      </c>
       <c r="I6" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8410,13 +8427,13 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8433,13 +8450,13 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8456,13 +8473,13 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8479,16 +8496,16 @@
         <v>2</v>
       </c>
       <c r="G10" s="112" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I10" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8505,16 +8522,16 @@
         <v>2</v>
       </c>
       <c r="G11" s="111" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>575</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -8522,7 +8539,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C12" s="115" t="s">
         <v>219</v>
@@ -8534,16 +8551,16 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>571</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>572</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>573</v>
-      </c>
       <c r="J12" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -8560,13 +8577,13 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8574,7 +8591,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>221</v>
@@ -8618,7 +8635,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="118" t="s">
-        <v>226</v>
+        <v>579</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8626,7 +8643,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="118" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -8634,7 +8651,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8642,7 +8659,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="118" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8650,7 +8667,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="119" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -8658,7 +8675,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="120" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -8666,7 +8683,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="121" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -8674,7 +8691,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="121" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -8682,7 +8699,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="121" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -8690,7 +8707,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="121" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -8698,7 +8715,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="121" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -8706,7 +8723,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="121" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -8714,7 +8731,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="121" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -8722,7 +8739,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="121" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8730,7 +8747,13 @@
         <v>30</v>
       </c>
       <c r="C33" s="122" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="128" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="127"/>
+      <c r="C45" s="129" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   25-05-2021 -  3:07:07.75
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="587">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2064,6 +2064,30 @@
   </si>
   <si>
     <t xml:space="preserve"> Find element In Generic Tree </t>
+  </si>
+  <si>
+    <t>check no of children and appy recursion on xhild</t>
+  </si>
+  <si>
+    <t>no of children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">khudki hi mirror image he </t>
+  </si>
+  <si>
+    <t>travel and change strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we will use state 0 1 2 
+</t>
+  </si>
+  <si>
+    <t>state 0 me jo aakri visit hua that - that is predessor
+state 1 me jo  aakhri visit hua tha- this is successor</t>
+  </si>
+  <si>
+    <t>ceil -smallest among larges
+floow- largest among smallest</t>
   </si>
 </sst>
 </file>
@@ -2434,7 +2458,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2757,9 +2781,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="5" xfId="14" applyBorder="1" applyAlignment="1">
@@ -3143,10 +3164,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="123" t="s">
+      <c r="F2" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="123"/>
+      <c r="G2" s="122"/>
       <c r="J2" s="106" t="s">
         <v>327</v>
       </c>
@@ -5778,7 +5799,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="125" t="s">
         <v>576</v>
       </c>
       <c r="C2" s="16"/>
@@ -6680,15 +6701,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="123" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7965,7 +7986,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="125" t="s">
+      <c r="D29" s="124" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -8304,7 +8325,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8614,7 +8635,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -8622,7 +8643,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>15</v>
       </c>
@@ -8630,7 +8651,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -8638,7 +8659,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -8646,7 +8667,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -8654,7 +8675,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -8662,83 +8683,104 @@
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="119" t="s">
+      <c r="C23" s="118" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="120" t="s">
+      <c r="C24" s="118" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="121" t="s">
+      <c r="C25" s="119" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="121" t="s">
+      <c r="C26" s="120" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="121" t="s">
+      <c r="C27" s="120" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G27" s="18" t="s">
+        <v>584</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="121" t="s">
+      <c r="C28" s="120" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G28" s="18" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="121" t="s">
+      <c r="C29" s="120" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="121" t="s">
+      <c r="C30" s="120" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="121" t="s">
+      <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="120" t="s">
         <v>238</v>
       </c>
     </row>
@@ -8746,13 +8788,13 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="C33" s="122" t="s">
+      <c r="C33" s="121" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="128" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="127"/>
-      <c r="C45" s="129" t="s">
+    <row r="45" spans="1:3" s="127" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="126"/>
+      <c r="C45" s="128" t="s">
         <v>578</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   25-05-2021 - 23:20:33.73
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="598">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2088,6 +2088,70 @@
   <si>
     <t>ceil -smallest among larges
 floow- largest among smallest</t>
+  </si>
+  <si>
+    <t>use floor k times</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">this is type of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>problem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+where hum return kuch aur kar rhe he aur 
+calculate hum kuch aur bana rhe he </t>
+    </r>
+  </si>
+  <si>
+    <t>returen max height in recursion and 
+based on that we will calculate the diameter</t>
+  </si>
+  <si>
+    <t>visulaize how state is gettig managed
+managed
+we are using pair{ data and state}
+and stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agar st.top me state =-1 - preorder
+agar st.top me state  =size of children - postorder
+else processing of children
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Validate Stack Sequences - LeetCode</t>
+  </si>
+  <si>
+    <t>N-ary Tree Level Order Traversal - LeetCode</t>
+  </si>
+  <si>
+    <t>Maximum Depth of N-ary Tree - LeetCode</t>
+  </si>
+  <si>
+    <t>N-ary Tree Preorder Traversal - LeetCode</t>
+  </si>
+  <si>
+    <t>N-ary Tree Postorder Traversal - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -5765,10 +5829,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6626,6 +6690,11 @@
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
         <v>509</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -6667,9 +6736,10 @@
     <hyperlink ref="I21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
     <hyperlink ref="B50" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/"/>
     <hyperlink ref="I7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
+    <hyperlink ref="B51" r:id="rId38" display="https://leetcode.com/problems/validate-stack-sequences/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -7451,8 +7521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8093,8 +8163,8 @@
       <c r="F33" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="5">
-        <v>2</v>
+      <c r="G33" s="5" t="s">
+        <v>592</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>550</v>
@@ -8322,10 +8392,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8759,29 +8829,44 @@
       <c r="C29" s="120" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
       <c r="C30" s="120" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="18" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
       <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G31" s="18" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
       <c r="C32" s="120" t="s">
         <v>238</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8796,6 +8881,26 @@
       <c r="A45" s="126"/>
       <c r="C45" s="128" t="s">
         <v>578</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="16" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="16" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="16" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="16" t="s">
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -8810,8 +8915,12 @@
     <hyperlink ref="J11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java"/>
     <hyperlink ref="J12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
     <hyperlink ref="J13" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java"/>
+    <hyperlink ref="C47" r:id="rId11" display="https://leetcode.com/problems/n-ary-tree-level-order-traversal/"/>
+    <hyperlink ref="C48" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-n-ary-tree/"/>
+    <hyperlink ref="C49" r:id="rId13" display="https://leetcode.com/problems/n-ary-tree-preorder-traversal/"/>
+    <hyperlink ref="C50" r:id="rId14" display="https://leetcode.com/problems/n-ary-tree-postorder-traversal/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   26-05-2021 -  2:15:33.05
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="598">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2158,7 +2158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2252,6 +2252,13 @@
     <font>
       <sz val="16"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2850,9 +2857,6 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="5" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2868,6 +2872,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3228,10 +3235,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="122" t="s">
+      <c r="F2" s="121" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="122"/>
+      <c r="G2" s="121"/>
       <c r="J2" s="106" t="s">
         <v>327</v>
       </c>
@@ -5863,7 +5870,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="124" t="s">
         <v>576</v>
       </c>
       <c r="C2" s="16"/>
@@ -6771,15 +6778,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="122" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8056,7 +8063,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="123" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -8394,8 +8401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8873,13 +8880,16 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="C33" s="121" t="s">
+      <c r="B33" s="106" t="s">
+        <v>567</v>
+      </c>
+      <c r="C33" s="128" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="127" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="126"/>
-      <c r="C45" s="128" t="s">
+    <row r="45" spans="1:3" s="126" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="125"/>
+      <c r="C45" s="127" t="s">
         <v>578</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   27-05-2021 -  1:40:45.62
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="599">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2152,6 +2152,9 @@
   </si>
   <si>
     <t>N-ary Tree Postorder Traversal - LeetCode</t>
+  </si>
+  <si>
+    <t>need to update notes for 9 and 10</t>
   </si>
 </sst>
 </file>
@@ -2529,7 +2532,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2875,6 +2878,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4346,8 +4361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD38"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,7 +5322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -5838,7 +5853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -7528,7 +7543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -8401,8 +8416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8415,9 +8430,12 @@
     <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1"/>
+      <c r="F1" s="18" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
@@ -8496,7 +8514,7 @@
         <v>34</v>
       </c>
       <c r="F6" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="110" t="s">
         <v>561</v>
@@ -8522,7 +8540,7 @@
         <v>34</v>
       </c>
       <c r="F7" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
         <v>496</v>
@@ -8545,7 +8563,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
         <v>496</v>
@@ -8568,7 +8586,7 @@
         <v>34</v>
       </c>
       <c r="F9" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
         <v>496</v>
@@ -8591,7 +8609,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="112" t="s">
         <v>496</v>
@@ -8617,7 +8635,7 @@
         <v>34</v>
       </c>
       <c r="F11" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="111" t="s">
         <v>568</v>
@@ -8646,7 +8664,7 @@
         <v>34</v>
       </c>
       <c r="F12" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
         <v>569</v>
@@ -8672,7 +8690,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
         <v>577</v>
@@ -8703,6 +8721,9 @@
       <c r="C15" s="117" t="s">
         <v>222</v>
       </c>
+      <c r="F15" s="129">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -8711,6 +8732,9 @@
       <c r="C16" s="118" t="s">
         <v>223</v>
       </c>
+      <c r="F16" s="129">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
@@ -8719,45 +8743,63 @@
       <c r="C17" s="118" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
       <c r="C18" s="118" t="s">
         <v>225</v>
+      </c>
+      <c r="F18" s="129">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="131" t="s">
         <v>579</v>
+      </c>
+      <c r="F19" s="129">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="118" t="s">
+      <c r="C20" s="130" t="s">
         <v>226</v>
+      </c>
+      <c r="F20" s="129">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="130" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="132" t="s">
         <v>228</v>
+      </c>
+      <c r="F22" s="129">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -8767,6 +8809,9 @@
       <c r="C23" s="118" t="s">
         <v>229</v>
       </c>
+      <c r="F23" s="129">
+        <v>1</v>
+      </c>
       <c r="G23" t="s">
         <v>580</v>
       </c>
@@ -8778,6 +8823,9 @@
       <c r="C24" s="118" t="s">
         <v>230</v>
       </c>
+      <c r="F24" s="129">
+        <v>1</v>
+      </c>
       <c r="G24" t="s">
         <v>581</v>
       </c>
@@ -8789,6 +8837,9 @@
       <c r="C25" s="119" t="s">
         <v>231</v>
       </c>
+      <c r="F25" s="129">
+        <v>1</v>
+      </c>
       <c r="G25" t="s">
         <v>582</v>
       </c>
@@ -8800,6 +8851,9 @@
       <c r="C26" s="120" t="s">
         <v>232</v>
       </c>
+      <c r="F26" s="129">
+        <v>1</v>
+      </c>
       <c r="G26" t="s">
         <v>583</v>
       </c>
@@ -8811,6 +8865,9 @@
       <c r="C27" s="120" t="s">
         <v>233</v>
       </c>
+      <c r="F27" s="129">
+        <v>1</v>
+      </c>
       <c r="G27" s="18" t="s">
         <v>584</v>
       </c>
@@ -8825,6 +8882,9 @@
       <c r="C28" s="120" t="s">
         <v>234</v>
       </c>
+      <c r="F28" s="129">
+        <v>1</v>
+      </c>
       <c r="G28" s="18" t="s">
         <v>586</v>
       </c>
@@ -8836,6 +8896,9 @@
       <c r="C29" s="120" t="s">
         <v>235</v>
       </c>
+      <c r="F29" s="129">
+        <v>1</v>
+      </c>
       <c r="G29" t="s">
         <v>587</v>
       </c>
@@ -8847,6 +8910,9 @@
       <c r="C30" s="120" t="s">
         <v>236</v>
       </c>
+      <c r="F30" s="129">
+        <v>1</v>
+      </c>
       <c r="G30" s="18" t="s">
         <v>588</v>
       </c>
@@ -8858,6 +8924,9 @@
       <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
+      <c r="F31" s="129">
+        <v>1</v>
+      </c>
       <c r="G31" s="18" t="s">
         <v>589</v>
       </c>
@@ -8868,6 +8937,9 @@
       </c>
       <c r="C32" s="120" t="s">
         <v>238</v>
+      </c>
+      <c r="F32" s="129">
+        <v>1</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>590</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   27-05-2021 - 23:32:25.99
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="600">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2155,6 +2155,9 @@
   </si>
   <si>
     <t>need to update notes for 9 and 10</t>
+  </si>
+  <si>
+    <t>theory</t>
   </si>
 </sst>
 </file>
@@ -3352,8 +3355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,6 +3416,9 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
+      <c r="C4" s="106" t="s">
+        <v>599</v>
+      </c>
       <c r="D4" s="95" t="s">
         <v>263</v>
       </c>
@@ -3421,6 +3427,9 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
+      <c r="C5" s="106" t="s">
+        <v>599</v>
+      </c>
       <c r="D5" s="95" t="s">
         <v>264</v>
       </c>
@@ -3428,6 +3437,9 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
+      </c>
+      <c r="C6" s="106" t="s">
+        <v>599</v>
       </c>
       <c r="D6" s="95" t="s">
         <v>265</v>
@@ -8416,8 +8428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8897,7 +8909,7 @@
         <v>235</v>
       </c>
       <c r="F29" s="129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" t="s">
         <v>587</v>
@@ -8911,7 +8923,7 @@
         <v>236</v>
       </c>
       <c r="F30" s="129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>588</v>
@@ -8925,7 +8937,7 @@
         <v>237</v>
       </c>
       <c r="F31" s="129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>589</v>
@@ -8939,7 +8951,7 @@
         <v>238</v>
       </c>
       <c r="F32" s="129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>590</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   29-05-2021 - 13:04:04.63
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="607">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2158,6 +2158,27 @@
   </si>
   <si>
     <t>theory</t>
+  </si>
+  <si>
+    <t>think in terms of recursion stack state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar to 16 </t>
+  </si>
+  <si>
+    <t>similar to 17</t>
+  </si>
+  <si>
+    <t>similar to 18</t>
+  </si>
+  <si>
+    <t>find size,max,min,height -suing global variable preorder</t>
+  </si>
+  <si>
+    <t>counting ki kitne element bache he from intersection point</t>
+  </si>
+  <si>
+    <t>2 tree will superimpose</t>
   </si>
 </sst>
 </file>
@@ -3355,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8428,8 +8449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8733,8 +8754,11 @@
       <c r="C15" s="117" t="s">
         <v>222</v>
       </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="129">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -8744,8 +8768,11 @@
       <c r="C16" s="118" t="s">
         <v>223</v>
       </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
       <c r="F16" s="129">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -8755,6 +8782,9 @@
       <c r="C17" s="118" t="s">
         <v>224</v>
       </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" s="129">
         <v>1</v>
       </c>
@@ -8766,6 +8796,9 @@
       <c r="C18" s="118" t="s">
         <v>225</v>
       </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
       <c r="F18" s="129">
         <v>1</v>
       </c>
@@ -8777,8 +8810,14 @@
       <c r="C19" s="131" t="s">
         <v>579</v>
       </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
       <c r="F19" s="129">
         <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -8788,8 +8827,14 @@
       <c r="C20" s="130" t="s">
         <v>226</v>
       </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="129">
         <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -8799,19 +8844,34 @@
       <c r="C21" s="130" t="s">
         <v>227</v>
       </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="129">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
       <c r="C22" s="132" t="s">
         <v>228</v>
       </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
       <c r="F22" s="129">
         <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>603</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -8827,6 +8887,9 @@
       <c r="G23" t="s">
         <v>580</v>
       </c>
+      <c r="H23" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
@@ -8868,6 +8931,9 @@
       </c>
       <c r="G26" t="s">
         <v>583</v>
+      </c>
+      <c r="H26" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   29-05-2021 - 13:22:56.78
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -2178,7 +2178,8 @@
     <t>counting ki kitne element bache he from intersection point</t>
   </si>
   <si>
-    <t>2 tree will superimpose</t>
+    <t>2 tree will superimpose
+can also be done using iterative queue level wise</t>
   </si>
 </sst>
 </file>
@@ -8450,7 +8451,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8874,7 +8875,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -8887,7 +8888,7 @@
       <c r="G23" t="s">
         <v>580</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="18" t="s">
         <v>606</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   30-05-2021 - 11:24:26.35
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="617">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1781,9 +1781,6 @@
   </si>
   <si>
     <t>check video how to manage tail using prev rather than using loop of n</t>
-  </si>
-  <si>
-    <t>number to char(letter)</t>
   </si>
   <si>
     <t>number to char(number)</t>
@@ -2181,12 +2178,57 @@
     <t>2 tree will superimpose
 can also be done using iterative queue level wise</t>
   </si>
+  <si>
+    <t xml:space="preserve"> 2^31-1 = 2147483647</t>
+  </si>
+  <si>
+    <t>number to char(letter) mapping</t>
+  </si>
+  <si>
+    <r>
+      <t> -</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF111111"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2^31 = -2147483648</t>
+    </r>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>resume creation</t>
+  </si>
+  <si>
+    <t>react projects</t>
+  </si>
+  <si>
+    <t>microservices</t>
+  </si>
+  <si>
+    <t>aws</t>
+  </si>
+  <si>
+    <t>docker &amp; kubernetes</t>
+  </si>
+  <si>
+    <t>todos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2290,6 +2332,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -2557,7 +2612,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2885,12 +2940,6 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="5" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2917,6 +2966,13 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -2961,8 +3017,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>33651</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>186051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3255,10 +3311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K18"/>
+  <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3268,23 +3324,23 @@
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>119</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="121" t="s">
+      <c r="F2" s="131" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="121"/>
+      <c r="G2" s="131"/>
       <c r="J2" s="106" t="s">
         <v>327</v>
       </c>
       <c r="K2" s="106"/>
     </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>121</v>
       </c>
@@ -3301,20 +3357,20 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>526</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>527</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>528</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="J4" s="16"/>
     </row>
-    <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>526</v>
+        <v>607</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -3329,7 +3385,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>391</v>
       </c>
@@ -3340,7 +3396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F7" s="5" t="s">
         <v>125</v>
       </c>
@@ -3348,16 +3404,62 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B12" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>610</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E18" s="12"/>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N31" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>615</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3439,7 +3541,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="106" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>263</v>
@@ -3450,7 +3552,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D5" s="95" t="s">
         <v>264</v>
@@ -3461,7 +3563,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D6" s="95" t="s">
         <v>265</v>
@@ -4310,19 +4412,19 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C11" t="s">
         <v>208</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="F11" t="s">
         <v>529</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" s="16" t="s">
         <v>530</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5919,8 +6021,8 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="124" t="s">
-        <v>576</v>
+      <c r="B2" s="122" t="s">
+        <v>575</v>
       </c>
       <c r="C2" s="16"/>
       <c r="G2" s="16"/>
@@ -6043,7 +6145,7 @@
         <v>337</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6750,7 +6852,7 @@
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -6827,15 +6929,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7598,7 +7700,7 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="103" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E1" s="5">
         <v>0</v>
@@ -7608,10 +7710,10 @@
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="104" t="s">
+        <v>545</v>
+      </c>
+      <c r="E2" s="104" t="s">
         <v>546</v>
-      </c>
-      <c r="E2" s="104" t="s">
-        <v>547</v>
       </c>
       <c r="G2"/>
     </row>
@@ -7999,7 +8101,7 @@
         <v>500</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>499</v>
@@ -8105,14 +8207,14 @@
         <v>2</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="123" t="s">
+      <c r="D29" s="121" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -8125,7 +8227,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -8148,7 +8250,7 @@
         <v>523</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -8168,7 +8270,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>524</v>
@@ -8177,7 +8279,7 @@
         <v>525</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -8197,13 +8299,13 @@
         <v>2</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I32" s="18" t="s">
+        <v>547</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>548</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8220,13 +8322,13 @@
         <v>34</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8234,10 +8336,10 @@
         <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D34" s="102" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
@@ -8249,10 +8351,10 @@
         <v>2</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -8278,7 +8380,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -8375,7 +8477,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D48" s="16" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -8386,7 +8488,7 @@
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" s="16" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -8450,7 +8552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -8468,7 +8570,7 @@
       <c r="A1"/>
       <c r="C1"/>
       <c r="F1" s="18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -8512,14 +8614,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C4" s="113" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="105"/>
       <c r="J4" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8527,14 +8629,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C5" s="114" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="105"/>
       <c r="J5" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8551,16 +8653,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="110" t="s">
+        <v>560</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>561</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>562</v>
-      </c>
       <c r="I6" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8580,10 +8682,10 @@
         <v>496</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -8603,10 +8705,10 @@
         <v>496</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8626,10 +8728,10 @@
         <v>496</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8649,13 +8751,13 @@
         <v>496</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8672,16 +8774,16 @@
         <v>3</v>
       </c>
       <c r="G11" s="111" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H11" s="10" t="s">
+        <v>572</v>
+      </c>
+      <c r="I11" s="10" t="s">
         <v>573</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>574</v>
-      </c>
       <c r="J11" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -8689,7 +8791,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C12" s="115" t="s">
         <v>219</v>
@@ -8701,16 +8803,16 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H12" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>572</v>
-      </c>
       <c r="J12" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -8727,13 +8829,13 @@
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8741,7 +8843,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C14" s="116" t="s">
         <v>221</v>
@@ -8758,7 +8860,7 @@
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="129">
+      <c r="F15" s="127">
         <v>2</v>
       </c>
     </row>
@@ -8772,7 +8874,7 @@
       <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="129">
+      <c r="F16" s="127">
         <v>2</v>
       </c>
     </row>
@@ -8786,7 +8888,7 @@
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="129">
+      <c r="F17" s="127">
         <v>1</v>
       </c>
     </row>
@@ -8800,7 +8902,7 @@
       <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="129">
+      <c r="F18" s="127">
         <v>1</v>
       </c>
     </row>
@@ -8808,71 +8910,71 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="131" t="s">
-        <v>579</v>
+      <c r="C19" s="129" t="s">
+        <v>578</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="129">
+      <c r="F19" s="127">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="130" t="s">
+      <c r="C20" s="128" t="s">
         <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="129">
+      <c r="F20" s="127">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="128" t="s">
         <v>227</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="129">
+      <c r="F21" s="127">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="132" t="s">
+      <c r="C22" s="130" t="s">
         <v>228</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="129">
+      <c r="F22" s="127">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8882,14 +8984,14 @@
       <c r="C23" s="118" t="s">
         <v>229</v>
       </c>
-      <c r="F23" s="129">
+      <c r="F23" s="127">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -8899,11 +9001,11 @@
       <c r="C24" s="118" t="s">
         <v>230</v>
       </c>
-      <c r="F24" s="129">
+      <c r="F24" s="127">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8913,11 +9015,11 @@
       <c r="C25" s="119" t="s">
         <v>231</v>
       </c>
-      <c r="F25" s="129">
+      <c r="F25" s="127">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -8927,14 +9029,14 @@
       <c r="C26" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="F26" s="129">
+      <c r="F26" s="127">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H26" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8944,14 +9046,14 @@
       <c r="C27" s="120" t="s">
         <v>233</v>
       </c>
-      <c r="F27" s="129">
+      <c r="F27" s="127">
         <v>1</v>
       </c>
       <c r="G27" s="18" t="s">
+        <v>583</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>584</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8961,11 +9063,11 @@
       <c r="C28" s="120" t="s">
         <v>234</v>
       </c>
-      <c r="F28" s="129">
+      <c r="F28" s="127">
         <v>1</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -8975,11 +9077,11 @@
       <c r="C29" s="120" t="s">
         <v>235</v>
       </c>
-      <c r="F29" s="129">
+      <c r="F29" s="127">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -8989,11 +9091,11 @@
       <c r="C30" s="120" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="129">
+      <c r="F30" s="127">
         <v>0</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9003,11 +9105,11 @@
       <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
-      <c r="F31" s="129">
+      <c r="F31" s="127">
         <v>0</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -9017,14 +9119,14 @@
       <c r="C32" s="120" t="s">
         <v>238</v>
       </c>
-      <c r="F32" s="129">
+      <c r="F32" s="127">
         <v>0</v>
       </c>
       <c r="G32" s="18" t="s">
+        <v>589</v>
+      </c>
+      <c r="H32" s="18" t="s">
         <v>590</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9032,36 +9134,36 @@
         <v>30</v>
       </c>
       <c r="B33" s="106" t="s">
-        <v>567</v>
-      </c>
-      <c r="C33" s="128" t="s">
+        <v>566</v>
+      </c>
+      <c r="C33" s="126" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="126" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="125"/>
-      <c r="C45" s="127" t="s">
-        <v>578</v>
+    <row r="45" spans="1:3" s="124" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="123"/>
+      <c r="C45" s="125" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   30-05-2021 - 21:32:17.03
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="617">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2612,7 +2612,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2973,6 +2973,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3477,31 +3478,31 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="4" max="4" width="55.140625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="9" width="39" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" customWidth="1"/>
-    <col min="11" max="11" width="52.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="8" width="39" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" customWidth="1"/>
+    <col min="10" max="10" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
@@ -3515,28 +3516,25 @@
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -3547,7 +3545,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -3569,23 +3567,29 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="D7" s="95" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
+      <c r="C8" s="134" t="s">
+        <v>598</v>
+      </c>
       <c r="D8" s="95" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -3593,7 +3597,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -3601,7 +3605,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -3609,7 +3613,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -3625,7 +3629,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -3633,7 +3637,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -3641,7 +3645,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -8552,8 +8556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8984,6 +8988,9 @@
       <c r="C23" s="118" t="s">
         <v>229</v>
       </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
       <c r="F23" s="127">
         <v>1</v>
       </c>
@@ -9000,6 +9007,9 @@
       </c>
       <c r="C24" s="118" t="s">
         <v>230</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
       </c>
       <c r="F24" s="127">
         <v>1</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   30-05-2021 - 22:02:46.62
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="617">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3481,7 +3481,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,6 +3595,9 @@
       </c>
       <c r="D9" s="95" t="s">
         <v>268</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated code on timestamp:   31-05-2021 -  1:26:22.17
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="617">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2133,9 +2133,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Validate Stack Sequences - LeetCode</t>
   </si>
   <si>
@@ -2222,6 +2219,10 @@
   </si>
   <si>
     <t>todos</t>
+  </si>
+  <si>
+    <t>need to do the iteratve solution for recursiotn which was done in last lec
+for both return type and void vale recursion</t>
   </si>
 </sst>
 </file>
@@ -2966,14 +2967,14 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3332,10 +3333,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="131" t="s">
+      <c r="F2" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="131"/>
+      <c r="G2" s="133"/>
       <c r="J2" s="106" t="s">
         <v>327</v>
       </c>
@@ -3371,7 +3372,7 @@
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -3412,18 +3413,18 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>610</v>
-      </c>
-      <c r="B13" s="133" t="s">
-        <v>608</v>
+        <v>609</v>
+      </c>
+      <c r="B13" s="131" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.25">
@@ -3434,32 +3435,32 @@
     </row>
     <row r="30" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="31" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="32" spans="5:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -3480,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3502,7 +3503,7 @@
       <c r="A2"/>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
@@ -3539,10 +3540,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="106" t="s">
-        <v>598</v>
-      </c>
-      <c r="D4" s="95" t="s">
+        <v>597</v>
+      </c>
+      <c r="D4" s="129" t="s">
         <v>263</v>
+      </c>
+      <c r="G4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3550,10 +3554,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="106" t="s">
-        <v>598</v>
-      </c>
-      <c r="D5" s="95" t="s">
+        <v>597</v>
+      </c>
+      <c r="D5" s="128" t="s">
         <v>264</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3561,51 +3568,66 @@
         <v>3</v>
       </c>
       <c r="C6" s="106" t="s">
-        <v>598</v>
-      </c>
-      <c r="D6" s="95" t="s">
+        <v>597</v>
+      </c>
+      <c r="D6" s="128" t="s">
         <v>265</v>
+      </c>
+      <c r="G6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="128" t="s">
         <v>266</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="134" t="s">
-        <v>598</v>
-      </c>
-      <c r="D8" s="95" t="s">
+      <c r="C8" s="132" t="s">
+        <v>597</v>
+      </c>
+      <c r="D8" s="128" t="s">
         <v>267</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="128" t="s">
         <v>268</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="130" t="s">
         <v>269</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -4504,7 +4526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -5466,7 +5488,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D15" sqref="D15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6859,7 +6881,7 @@
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -6936,15 +6958,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="134" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7686,8 +7708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7798,7 +7820,7 @@
         <v>34</v>
       </c>
       <c r="G9" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>449</v>
@@ -7818,7 +7840,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>449</v>
@@ -7838,7 +7860,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>449</v>
@@ -7858,7 +7880,7 @@
         <v>34</v>
       </c>
       <c r="G12" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>449</v>
@@ -7878,7 +7900,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>449</v>
@@ -7898,7 +7920,7 @@
         <v>34</v>
       </c>
       <c r="G14" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>449</v>
@@ -7918,7 +7940,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>449</v>
@@ -7938,7 +7960,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>449</v>
@@ -7958,7 +7980,7 @@
         <v>34</v>
       </c>
       <c r="G17" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>466</v>
@@ -7984,7 +8006,7 @@
         <v>34</v>
       </c>
       <c r="G18" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>469</v>
@@ -8007,7 +8029,7 @@
         <v>34</v>
       </c>
       <c r="G19" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>467</v>
@@ -8030,7 +8052,7 @@
         <v>34</v>
       </c>
       <c r="G20" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20" s="18" t="s">
         <v>468</v>
@@ -8053,7 +8075,7 @@
         <v>34</v>
       </c>
       <c r="G21" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H21" s="18" t="s">
         <v>471</v>
@@ -8076,7 +8098,7 @@
         <v>34</v>
       </c>
       <c r="G22" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="18" t="s">
         <v>470</v>
@@ -8099,7 +8121,7 @@
         <v>34</v>
       </c>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>498</v>
@@ -8128,7 +8150,7 @@
         <v>34</v>
       </c>
       <c r="G24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24" s="16" t="s">
         <v>501</v>
@@ -8148,7 +8170,7 @@
         <v>34</v>
       </c>
       <c r="G25" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>502</v>
@@ -8171,7 +8193,7 @@
         <v>34</v>
       </c>
       <c r="G26" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" s="16" t="s">
         <v>514</v>
@@ -8191,7 +8213,7 @@
         <v>34</v>
       </c>
       <c r="G27" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" s="16" t="s">
         <v>522</v>
@@ -8211,7 +8233,7 @@
         <v>34</v>
       </c>
       <c r="G28" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>532</v>
@@ -8231,7 +8253,7 @@
         <v>34</v>
       </c>
       <c r="G29" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K29" s="16" t="s">
         <v>533</v>
@@ -8251,7 +8273,7 @@
         <v>34</v>
       </c>
       <c r="G30" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>523</v>
@@ -8274,7 +8296,7 @@
         <v>34</v>
       </c>
       <c r="G31" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>535</v>
@@ -8303,7 +8325,7 @@
         <v>34</v>
       </c>
       <c r="G32" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H32" s="18" t="s">
         <v>542</v>
@@ -8328,8 +8350,8 @@
       <c r="F33" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>591</v>
+      <c r="G33" s="5">
+        <v>3</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>549</v>
@@ -8355,7 +8377,7 @@
         <v>34</v>
       </c>
       <c r="G34" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H34" s="18" t="s">
         <v>550</v>
@@ -8559,8 +8581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8573,16 +8595,19 @@
     <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1"/>
-      <c r="F1" s="18" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G1" s="106" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="C2"/>
+      <c r="G2" s="18" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
@@ -8927,7 +8952,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -8944,7 +8969,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -8961,7 +8986,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8978,10 +9003,10 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9001,7 +9026,7 @@
         <v>579</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -9049,7 +9074,7 @@
         <v>582</v>
       </c>
       <c r="H26" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -9161,22 +9186,22 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   01-06-2021 - 22:34:00.47
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="619">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2223,6 +2223,15 @@
   <si>
     <t>need to do the iteratve solution for recursiotn which was done in last lec
 for both return type and void vale recursion</t>
+  </si>
+  <si>
+    <t>can be askes as - 
+max distance between 2 nodes
+2 server k bich me max distances
+max edge between 2 nodes</t>
+  </si>
+  <si>
+    <t>you will learn how to use klevel down and node to root parth</t>
   </si>
 </sst>
 </file>
@@ -2613,7 +2622,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2974,6 +2983,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3481,8 +3493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,6 +3649,9 @@
       <c r="D11" s="95" t="s">
         <v>270</v>
       </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -3645,13 +3660,19 @@
       <c r="D12" s="95" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="135" t="s">
         <v>272</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6018,7 +6039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
@@ -8581,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8910,7 +8931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -8921,10 +8942,10 @@
         <v>34</v>
       </c>
       <c r="F17" s="127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
@@ -8935,10 +8956,10 @@
         <v>34</v>
       </c>
       <c r="F18" s="127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -8949,13 +8970,13 @@
         <v>34</v>
       </c>
       <c r="F19" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -8966,13 +8987,13 @@
         <v>34</v>
       </c>
       <c r="F20" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -8983,13 +9004,13 @@
         <v>34</v>
       </c>
       <c r="F21" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -9000,7 +9021,7 @@
         <v>34</v>
       </c>
       <c r="F22" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
         <v>601</v>
@@ -9009,7 +9030,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -9020,7 +9041,7 @@
         <v>34</v>
       </c>
       <c r="F23" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
         <v>579</v>
@@ -9029,7 +9050,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
@@ -9040,35 +9061,41 @@
         <v>34</v>
       </c>
       <c r="F24" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
       <c r="C25" s="119" t="s">
         <v>231</v>
       </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
       <c r="F25" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
       <c r="C26" s="120" t="s">
         <v>232</v>
       </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
       <c r="F26" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
         <v>582</v>
@@ -9077,15 +9104,18 @@
         <v>602</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
       <c r="C27" s="120" t="s">
         <v>233</v>
       </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
       <c r="F27" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>583</v>
@@ -9094,71 +9124,89 @@
         <v>584</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
       <c r="C28" s="120" t="s">
         <v>234</v>
       </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
       <c r="F28" s="127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
       <c r="C29" s="120" t="s">
         <v>235</v>
       </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
       <c r="F29" s="127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
       <c r="C30" s="120" t="s">
         <v>236</v>
       </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
       <c r="F30" s="127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
       <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
       <c r="F31" s="127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I31" s="18" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
       <c r="C32" s="120" t="s">
         <v>238</v>
       </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
       <c r="F32" s="127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>589</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   01-06-2021 - 23:13:26.19
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="620">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2233,12 +2233,15 @@
   <si>
     <t>you will learn how to use klevel down and node to root parth</t>
   </si>
+  <si>
+    <t>All Nodes Distance K in Binary Tree - LeetCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2355,6 +2358,13 @@
       <color rgb="FF111111"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="18">
@@ -2622,7 +2632,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2985,6 +2995,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3491,10 +3508,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3755,8 +3772,23 @@
         <v>282</v>
       </c>
     </row>
+    <row r="37" spans="1:4" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="136"/>
+      <c r="D37" s="138" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="16" t="s">
+        <v>619</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  0:23:16.93
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="640">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2235,6 +2235,66 @@
   </si>
   <si>
     <t>All Nodes Distance K in Binary Tree - LeetCode</t>
+  </si>
+  <si>
+    <t>CP/MirrorAGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PredessorAndSuccessorElement.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/CeilAndFloor.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KthLargestInGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/DiameterGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Multisolver.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/MaxSumSubtree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IterativePreorderPostorderGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/AreTreeSymmetric.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/AreTreesMirror.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/AreTreesSimilarInShape.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Distancebetween2Nodes.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LowestCommonAncestor.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/NodeToRootPath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/FindElementInGenericTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/RemoveLeavesInGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LinearizeGT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>diameter approach 2 pending</t>
+  </si>
+  <si>
+    <t>peding</t>
+  </si>
+  <si>
+    <t>not done</t>
   </si>
 </sst>
 </file>
@@ -3510,8 +3570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8635,7 +8695,7 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8934,6 +8994,9 @@
         <v>221</v>
       </c>
       <c r="G14" s="18"/>
+      <c r="J14" s="16" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
@@ -8948,6 +9011,9 @@
       <c r="F15" s="127">
         <v>2</v>
       </c>
+      <c r="J15" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -8962,8 +9028,11 @@
       <c r="F16" s="127">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="16" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -8976,8 +9045,11 @@
       <c r="F17" s="127">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" s="16" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <v>15</v>
       </c>
@@ -8990,8 +9062,11 @@
       <c r="F18" s="127">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="16" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -9007,8 +9082,11 @@
       <c r="G19" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="16" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -9024,8 +9102,11 @@
       <c r="G20" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="16" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -9041,8 +9122,11 @@
       <c r="G21" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="16" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29">
         <v>19</v>
       </c>
@@ -9061,8 +9145,11 @@
       <c r="H22" s="18" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J22" s="16" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>20</v>
       </c>
@@ -9081,8 +9168,11 @@
       <c r="H23" s="18" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="16" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>21</v>
       </c>
@@ -9098,8 +9188,11 @@
       <c r="G24" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="16" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29">
         <v>22</v>
       </c>
@@ -9115,8 +9208,11 @@
       <c r="G25" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="16" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>23</v>
       </c>
@@ -9124,7 +9220,7 @@
         <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>639</v>
       </c>
       <c r="F26" s="127">
         <v>2</v>
@@ -9135,8 +9231,11 @@
       <c r="H26" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" s="16" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>24</v>
       </c>
@@ -9155,8 +9254,11 @@
       <c r="H27" s="18" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J27" s="16" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>25</v>
       </c>
@@ -9172,8 +9274,11 @@
       <c r="G28" s="18" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="16" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>26</v>
       </c>
@@ -9189,8 +9294,11 @@
       <c r="G29" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J29" s="16" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
       </c>
@@ -9206,16 +9314,19 @@
       <c r="G30" s="18" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J30" s="16" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>28</v>
       </c>
       <c r="C31" s="120" t="s">
         <v>237</v>
       </c>
-      <c r="E31" t="s">
-        <v>34</v>
+      <c r="E31" s="18" t="s">
+        <v>637</v>
       </c>
       <c r="F31" s="127">
         <v>2</v>
@@ -9226,8 +9337,11 @@
       <c r="I31" s="18" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J31" s="16" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>29</v>
       </c>
@@ -9235,7 +9349,7 @@
         <v>238</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>638</v>
       </c>
       <c r="F32" s="127">
         <v>2</v>
@@ -9245,6 +9359,9 @@
       </c>
       <c r="H32" s="18" t="s">
         <v>590</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9300,8 +9417,27 @@
     <hyperlink ref="C48" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-n-ary-tree/"/>
     <hyperlink ref="C49" r:id="rId13" display="https://leetcode.com/problems/n-ary-tree-preorder-traversal/"/>
     <hyperlink ref="C50" r:id="rId14" display="https://leetcode.com/problems/n-ary-tree-postorder-traversal/"/>
+    <hyperlink ref="J15" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MirrorAGT.java"/>
+    <hyperlink ref="J27" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/PredessorAndSuccessorElement.java"/>
+    <hyperlink ref="J28" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/CeilAndFloor.java"/>
+    <hyperlink ref="J29" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/KthLargestInGT.java"/>
+    <hyperlink ref="J31" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/DiameterGT.java"/>
+    <hyperlink ref="J26" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Multisolver.java"/>
+    <hyperlink ref="J30" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxSumSubtree.java"/>
+    <hyperlink ref="J32" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/IterativePreorderPostorderGT.java"/>
+    <hyperlink ref="J25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreeSymmetric.java"/>
+    <hyperlink ref="J24" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java"/>
+    <hyperlink ref="J23" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesSimilarInShape.java"/>
+    <hyperlink ref="J22" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Distancebetween2Nodes.java"/>
+    <hyperlink ref="J21" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LowestCommonAncestor.java"/>
+    <hyperlink ref="J20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/NodeToRootPath.java"/>
+    <hyperlink ref="J19" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/FindElementInGenericTree.java"/>
+    <hyperlink ref="J16" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/RemoveLeavesInGT.java"/>
+    <hyperlink ref="J17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java"/>
+    <hyperlink ref="J18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java"/>
+    <hyperlink ref="J14" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  0:37:12.59
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="643">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2295,6 +2295,15 @@
   </si>
   <si>
     <t>not done</t>
+  </si>
+  <si>
+    <t>CP/BinaryTreeConstruction.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/SizeMinMaxHgt.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Traversal.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3568,287 +3577,308 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="4" max="4" width="55.140625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="8" width="39" customWidth="1"/>
-    <col min="9" max="9" width="36.85546875" customWidth="1"/>
-    <col min="10" max="10" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="7" width="39" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:9" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="F3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="B4" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="D4" s="129" t="s">
+      <c r="C4" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="16" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="B5" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="D5" s="128" t="s">
+      <c r="C5" s="128" t="s">
         <v>264</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="16" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="106" t="s">
+      <c r="B6" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="D6" s="128" t="s">
+      <c r="C6" s="128" t="s">
         <v>265</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="16" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="128" t="s">
+      <c r="C7" s="128" t="s">
         <v>266</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="16" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="132" t="s">
+      <c r="B8" s="132" t="s">
         <v>597</v>
       </c>
-      <c r="D8" s="128" t="s">
+      <c r="C8" s="128" t="s">
         <v>267</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="16" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="128" t="s">
+      <c r="C9" s="128" t="s">
         <v>268</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="16" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="130" t="s">
+      <c r="C10" s="130" t="s">
         <v>269</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="C11" s="95" t="s">
         <v>270</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="C12" s="95" t="s">
         <v>271</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="135" t="s">
+      <c r="C13" s="135" t="s">
         <v>272</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="18" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="C14" s="82" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="C15" s="82" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="C16" s="82" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="C17" s="82" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="C18" s="82" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="C19" s="82" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="D20" s="82" t="s">
+      <c r="C20" s="82" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="C21" s="82" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="C22" s="82" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="C23" s="82" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="136"/>
-      <c r="D37" s="138" t="s">
+      <c r="C37" s="138" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="16" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="16" t="s">
         <v>619</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/"/>
+    <hyperlink ref="C38" r:id="rId1" display="https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
+    <hyperlink ref="I6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
+    <hyperlink ref="I5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java"/>
+    <hyperlink ref="I9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  0:52:09.65
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="644">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2304,6 +2304,9 @@
   </si>
   <si>
     <t>CP/Traversal.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IterativePrePostInOrderinBT.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3580,7 +3583,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,6 +3745,9 @@
       <c r="F10" t="s">
         <v>100</v>
       </c>
+      <c r="I10" s="16" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -3876,9 +3882,10 @@
     <hyperlink ref="I7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java"/>
     <hyperlink ref="I9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java"/>
     <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java"/>
+    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  0:57:11.03
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="644">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3583,7 +3583,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,6 +3759,9 @@
       <c r="F11" t="s">
         <v>100</v>
       </c>
+      <c r="I11" s="16" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -3883,9 +3886,10 @@
     <hyperlink ref="I9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java"/>
     <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java"/>
     <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
+    <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  1:14:31.17
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="645">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2307,6 +2307,9 @@
   </si>
   <si>
     <t>CP/IterativePrePostInOrderinBT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintKlevelDown.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3583,7 +3586,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,6 +3776,9 @@
       <c r="F12" t="s">
         <v>100</v>
       </c>
+      <c r="I12" s="16" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -3887,9 +3893,10 @@
     <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java"/>
     <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
     <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java"/>
+    <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  1:17:22.32
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="647">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2310,6 +2310,12 @@
   </si>
   <si>
     <t>CP/PrintKlevelDown.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>standart recursion</t>
+  </si>
+  <si>
+    <t>CP/RootToleafPathSumInRange.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3586,7 +3592,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,6 +3796,9 @@
       <c r="F13" s="18" t="s">
         <v>618</v>
       </c>
+      <c r="I13" s="16" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -3797,6 +3806,12 @@
       </c>
       <c r="C14" s="82" t="s">
         <v>273</v>
+      </c>
+      <c r="F14" t="s">
+        <v>645</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3894,9 +3909,11 @@
     <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
     <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java"/>
     <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
+    <hyperlink ref="I13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
+    <hyperlink ref="I14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   02-06-2021 -  1:37:53.73
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -3591,7 +3591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -8759,8 +8759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-06-2021 -  1:05:24.02
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -2713,7 +2713,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3054,9 +3054,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3443,10 +3440,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="133" t="s">
+      <c r="F2" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="133"/>
+      <c r="G2" s="132"/>
       <c r="J2" s="106" t="s">
         <v>327</v>
       </c>
@@ -3533,7 +3530,7 @@
       <c r="A13" t="s">
         <v>609</v>
       </c>
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="130" t="s">
         <v>607</v>
       </c>
     </row>
@@ -3649,7 +3646,7 @@
       <c r="B4" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="128" t="s">
         <v>263</v>
       </c>
       <c r="F4" t="s">
@@ -3666,7 +3663,7 @@
       <c r="B5" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="C5" s="128" t="s">
+      <c r="C5" s="127" t="s">
         <v>264</v>
       </c>
       <c r="F5" t="s">
@@ -3683,7 +3680,7 @@
       <c r="B6" s="106" t="s">
         <v>597</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="127" t="s">
         <v>265</v>
       </c>
       <c r="F6" t="s">
@@ -3697,7 +3694,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="128" t="s">
+      <c r="C7" s="127" t="s">
         <v>266</v>
       </c>
       <c r="D7" t="s">
@@ -3714,10 +3711,10 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="131" t="s">
         <v>597</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="127" t="s">
         <v>267</v>
       </c>
       <c r="F8" t="s">
@@ -3731,7 +3728,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="128" t="s">
+      <c r="C9" s="127" t="s">
         <v>268</v>
       </c>
       <c r="D9" t="s">
@@ -3748,7 +3745,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="129" t="s">
         <v>269</v>
       </c>
       <c r="F10" t="s">
@@ -3790,7 +3787,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="134" t="s">
         <v>272</v>
       </c>
       <c r="F13" s="18" t="s">
@@ -3886,9 +3883,9 @@
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="136"/>
-      <c r="C37" s="138" t="s">
+    <row r="37" spans="1:3" s="136" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="135"/>
+      <c r="C37" s="137" t="s">
         <v>507</v>
       </c>
     </row>
@@ -7136,15 +7133,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="133" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8759,8 +8756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9058,6 +9055,9 @@
       <c r="C14" s="116" t="s">
         <v>221</v>
       </c>
+      <c r="F14" s="105">
+        <v>3</v>
+      </c>
       <c r="G14" s="18"/>
       <c r="J14" s="16" t="s">
         <v>564</v>
@@ -9073,8 +9073,8 @@
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="127">
-        <v>2</v>
+      <c r="F15" s="105">
+        <v>3</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>620</v>
@@ -9090,8 +9090,8 @@
       <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="127">
-        <v>2</v>
+      <c r="F16" s="105">
+        <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>635</v>
@@ -9107,8 +9107,8 @@
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="127">
-        <v>2</v>
+      <c r="F17" s="105">
+        <v>3</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>636</v>
@@ -9124,8 +9124,8 @@
       <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="127">
-        <v>2</v>
+      <c r="F18" s="105">
+        <v>3</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>636</v>
@@ -9135,14 +9135,14 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="128" t="s">
         <v>578</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="127">
-        <v>2</v>
+      <c r="F19" s="105">
+        <v>3</v>
       </c>
       <c r="G19" t="s">
         <v>598</v>
@@ -9155,14 +9155,14 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="128" t="s">
+      <c r="C20" s="127" t="s">
         <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="127">
-        <v>2</v>
+      <c r="F20" s="105">
+        <v>3</v>
       </c>
       <c r="G20" t="s">
         <v>599</v>
@@ -9175,14 +9175,14 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="128" t="s">
+      <c r="C21" s="127" t="s">
         <v>227</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="127">
-        <v>2</v>
+      <c r="F21" s="105">
+        <v>3</v>
       </c>
       <c r="G21" t="s">
         <v>600</v>
@@ -9195,14 +9195,14 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="130" t="s">
+      <c r="C22" s="129" t="s">
         <v>228</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="127">
-        <v>2</v>
+      <c r="F22" s="105">
+        <v>3</v>
       </c>
       <c r="G22" t="s">
         <v>601</v>
@@ -9224,8 +9224,8 @@
       <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="127">
-        <v>2</v>
+      <c r="F23" s="105">
+        <v>3</v>
       </c>
       <c r="G23" t="s">
         <v>579</v>
@@ -9247,8 +9247,8 @@
       <c r="E24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="127">
-        <v>2</v>
+      <c r="F24" s="105">
+        <v>3</v>
       </c>
       <c r="G24" t="s">
         <v>580</v>
@@ -9267,8 +9267,8 @@
       <c r="E25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="127">
-        <v>2</v>
+      <c r="F25" s="105">
+        <v>3</v>
       </c>
       <c r="G25" t="s">
         <v>581</v>
@@ -9287,8 +9287,8 @@
       <c r="E26" t="s">
         <v>639</v>
       </c>
-      <c r="F26" s="127">
-        <v>2</v>
+      <c r="F26" s="105">
+        <v>3</v>
       </c>
       <c r="G26" t="s">
         <v>582</v>
@@ -9310,8 +9310,8 @@
       <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="127">
-        <v>2</v>
+      <c r="F27" s="105">
+        <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>583</v>
@@ -9333,8 +9333,8 @@
       <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="127">
-        <v>2</v>
+      <c r="F28" s="105">
+        <v>3</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>585</v>
@@ -9353,8 +9353,8 @@
       <c r="E29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="127">
-        <v>2</v>
+      <c r="F29" s="105">
+        <v>3</v>
       </c>
       <c r="G29" t="s">
         <v>586</v>
@@ -9373,8 +9373,8 @@
       <c r="E30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="127">
-        <v>2</v>
+      <c r="F30" s="105">
+        <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>587</v>
@@ -9393,8 +9393,8 @@
       <c r="E31" s="18" t="s">
         <v>637</v>
       </c>
-      <c r="F31" s="127">
-        <v>2</v>
+      <c r="F31" s="105">
+        <v>3</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>588</v>
@@ -9416,8 +9416,8 @@
       <c r="E32" t="s">
         <v>638</v>
       </c>
-      <c r="F32" s="127">
-        <v>2</v>
+      <c r="F32" s="105">
+        <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>589</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-06-2021 -  1:26:44.97
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2713,7 +2713,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3072,7 +3072,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -3080,6 +3080,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3588,8 +3591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,7 +3762,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="134" t="s">
         <v>270</v>
       </c>
       <c r="F11" t="s">
@@ -3773,7 +3776,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="115" t="s">
         <v>271</v>
       </c>
       <c r="F12" t="s">
@@ -3783,11 +3786,11 @@
         <v>644</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="138" t="s">
         <v>272</v>
       </c>
       <c r="F13" s="18" t="s">
@@ -3801,7 +3804,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="117" t="s">
         <v>273</v>
       </c>
       <c r="F14" t="s">
@@ -3815,7 +3818,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="82" t="s">
+      <c r="C15" s="118" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3823,7 +3826,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="118" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3831,7 +3834,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="118" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3839,7 +3842,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="82" t="s">
+      <c r="C18" s="118" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3847,7 +3850,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="118" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3855,7 +3858,7 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="118" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3863,7 +3866,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="118" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3871,15 +3874,15 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="118" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="119" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5662,7 +5665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D15" sqref="D15:D18"/>
     </sheetView>
   </sheetViews>
@@ -7883,8 +7886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G34"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8756,8 +8759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-06-2021 -  1:28:02.53
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -2713,7 +2713,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2947,13 +2947,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
@@ -3075,6 +3069,15 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3083,6 +3086,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3443,14 +3455,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="J2" s="106" t="s">
+      <c r="G2" s="130"/>
+      <c r="J2" s="104" t="s">
         <v>327</v>
       </c>
-      <c r="K2" s="106"/>
+      <c r="K2" s="104"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3533,7 +3545,7 @@
       <c r="A13" t="s">
         <v>609</v>
       </c>
-      <c r="B13" s="130" t="s">
+      <c r="B13" s="128" t="s">
         <v>607</v>
       </c>
     </row>
@@ -3591,7 +3603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
@@ -3646,10 +3658,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="126" t="s">
         <v>263</v>
       </c>
       <c r="F4" t="s">
@@ -3663,10 +3675,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="125" t="s">
         <v>264</v>
       </c>
       <c r="F5" t="s">
@@ -3680,10 +3692,10 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="125" t="s">
         <v>265</v>
       </c>
       <c r="F6" t="s">
@@ -3697,7 +3709,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="125" t="s">
         <v>266</v>
       </c>
       <c r="D7" t="s">
@@ -3714,10 +3726,10 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="129" t="s">
         <v>597</v>
       </c>
-      <c r="C8" s="127" t="s">
+      <c r="C8" s="125" t="s">
         <v>267</v>
       </c>
       <c r="F8" t="s">
@@ -3731,7 +3743,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="127" t="s">
+      <c r="C9" s="125" t="s">
         <v>268</v>
       </c>
       <c r="D9" t="s">
@@ -3748,7 +3760,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="127" t="s">
         <v>269</v>
       </c>
       <c r="F10" t="s">
@@ -3762,7 +3774,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="132" t="s">
         <v>270</v>
       </c>
       <c r="F11" t="s">
@@ -3776,7 +3788,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="113" t="s">
         <v>271</v>
       </c>
       <c r="F12" t="s">
@@ -3790,7 +3802,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="138" t="s">
+      <c r="C13" s="139" t="s">
         <v>272</v>
       </c>
       <c r="F13" s="18" t="s">
@@ -3804,7 +3816,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="115" t="s">
         <v>273</v>
       </c>
       <c r="F14" t="s">
@@ -3818,7 +3830,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="116" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3826,7 +3838,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="118" t="s">
+      <c r="C16" s="116" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3834,7 +3846,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="118" t="s">
+      <c r="C17" s="116" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3842,7 +3854,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="116" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3850,7 +3862,7 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="116" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3858,7 +3870,7 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="118" t="s">
+      <c r="C20" s="116" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3866,7 +3878,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="116" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3874,7 +3886,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="118" t="s">
+      <c r="C22" s="116" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3882,13 +3894,13 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="119" t="s">
+      <c r="C23" s="117" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="136" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="135"/>
-      <c r="C37" s="137" t="s">
+    <row r="37" spans="1:3" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="136"/>
+      <c r="C37" s="138" t="s">
         <v>507</v>
       </c>
     </row>
@@ -3980,7 +3992,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="94" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3988,7 +4000,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="94" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3996,7 +4008,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="94" t="s">
         <v>285</v>
       </c>
     </row>
@@ -4004,7 +4016,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="96" t="s">
+      <c r="D7" s="94" t="s">
         <v>286</v>
       </c>
     </row>
@@ -4012,7 +4024,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="94" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4020,7 +4032,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="94" t="s">
         <v>288</v>
       </c>
     </row>
@@ -4028,7 +4040,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="94" t="s">
         <v>289</v>
       </c>
     </row>
@@ -4036,7 +4048,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="94" t="s">
         <v>290</v>
       </c>
     </row>
@@ -4044,7 +4056,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="94" t="s">
         <v>291</v>
       </c>
     </row>
@@ -4052,7 +4064,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="94" t="s">
         <v>292</v>
       </c>
     </row>
@@ -4124,7 +4136,7 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="93" t="s">
         <v>293</v>
       </c>
     </row>
@@ -4132,7 +4144,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="93" t="s">
         <v>294</v>
       </c>
     </row>
@@ -4140,7 +4152,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="93" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4148,7 +4160,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="93" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4156,7 +4168,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="93" t="s">
         <v>297</v>
       </c>
     </row>
@@ -4164,7 +4176,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="93" t="s">
         <v>298</v>
       </c>
     </row>
@@ -4172,7 +4184,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="93" t="s">
         <v>299</v>
       </c>
     </row>
@@ -4180,7 +4192,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="93" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4188,7 +4200,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="93" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4196,7 +4208,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="93" t="s">
         <v>302</v>
       </c>
     </row>
@@ -4204,7 +4216,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="81" t="s">
         <v>303</v>
       </c>
     </row>
@@ -4212,7 +4224,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="81" t="s">
         <v>304</v>
       </c>
     </row>
@@ -4220,7 +4232,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="D16" s="81" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4228,7 +4240,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="81" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4303,7 +4315,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="93" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4311,7 +4323,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="93" t="s">
         <v>309</v>
       </c>
     </row>
@@ -4319,7 +4331,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="93" t="s">
         <v>310</v>
       </c>
     </row>
@@ -4327,7 +4339,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="93" t="s">
         <v>311</v>
       </c>
     </row>
@@ -4335,7 +4347,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="93" t="s">
         <v>312</v>
       </c>
     </row>
@@ -4343,7 +4355,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="93" t="s">
         <v>313</v>
       </c>
     </row>
@@ -4351,7 +4363,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="93" t="s">
         <v>314</v>
       </c>
     </row>
@@ -4359,7 +4371,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="93" t="s">
         <v>315</v>
       </c>
     </row>
@@ -4367,7 +4379,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="93" t="s">
         <v>316</v>
       </c>
     </row>
@@ -4375,7 +4387,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="93" t="s">
         <v>317</v>
       </c>
     </row>
@@ -4383,7 +4395,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="81" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4391,7 +4403,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="82" t="s">
+      <c r="D15" s="81" t="s">
         <v>319</v>
       </c>
     </row>
@@ -4399,7 +4411,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="82" t="s">
+      <c r="D16" s="81" t="s">
         <v>320</v>
       </c>
     </row>
@@ -4407,7 +4419,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="82" t="s">
+      <c r="D17" s="81" t="s">
         <v>321</v>
       </c>
     </row>
@@ -4415,7 +4427,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="D18" s="81" t="s">
         <v>322</v>
       </c>
     </row>
@@ -4423,7 +4435,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="D19" s="81" t="s">
         <v>323</v>
       </c>
     </row>
@@ -4431,7 +4443,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="82" t="s">
+      <c r="D20" s="81" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4439,7 +4451,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="81" t="s">
         <v>308</v>
       </c>
     </row>
@@ -4594,7 +4606,7 @@
       <c r="F9" s="25" t="s">
         <v>494</v>
       </c>
-      <c r="G9" s="90" t="s">
+      <c r="G9" s="88" t="s">
         <v>496</v>
       </c>
       <c r="H9" s="10"/>
@@ -5665,8 +5677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5674,13 +5686,13 @@
     <col min="1" max="1" width="9.140625" style="13"/>
     <col min="2" max="2" width="8.5703125" style="13" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="25" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="18.140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="38.5703125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="39.7109375" style="15" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="66.7109375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="57.28515625" style="15" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5744,11 +5756,12 @@
       </c>
       <c r="K4" s="16"/>
     </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="115" t="s">
         <v>64</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -5774,7 +5787,7 @@
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="116" t="s">
         <v>66</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -5796,11 +5809,11 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="117" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -5820,7 +5833,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="133" t="s">
         <v>139</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -5843,7 +5856,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="134" t="s">
         <v>139</v>
       </c>
       <c r="F10" s="23" t="s">
@@ -5860,7 +5873,7 @@
       <c r="A11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="134" t="s">
         <v>168</v>
       </c>
       <c r="F11" s="78" t="s">
@@ -5880,7 +5893,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="134" t="s">
         <v>140</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -5896,11 +5909,11 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="135" t="s">
         <v>144</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -5926,7 +5939,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="140" t="s">
         <v>149</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -5955,7 +5968,7 @@
       <c r="C15" s="80" t="s">
         <v>478</v>
       </c>
-      <c r="D15" s="81" t="s">
+      <c r="D15" s="141" t="s">
         <v>151</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -5977,11 +5990,11 @@
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="D16" s="142" t="s">
         <v>153</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -6004,7 +6017,7 @@
       <c r="A17" s="13">
         <v>12</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="133" t="s">
         <v>154</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -6027,7 +6040,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="134" t="s">
         <v>157</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -6050,7 +6063,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="134" t="s">
         <v>159</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -6073,7 +6086,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="134" t="s">
         <v>162</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -6093,7 +6106,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="134" t="s">
         <v>163</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -6109,11 +6122,11 @@
         <v>485</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="135" t="s">
         <v>166</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -6133,7 +6146,7 @@
       <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="D23" s="84" t="s">
+      <c r="D23" s="82" t="s">
         <v>174</v>
       </c>
       <c r="I23" s="15" t="s">
@@ -6144,7 +6157,7 @@
       <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="D24" s="84" t="s">
+      <c r="D24" s="82" t="s">
         <v>175</v>
       </c>
     </row>
@@ -6228,7 +6241,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="120" t="s">
         <v>575</v>
       </c>
       <c r="C2" s="16"/>
@@ -7136,15 +7149,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="131" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7459,7 +7472,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="83" t="s">
         <v>178</v>
       </c>
       <c r="E4" t="s">
@@ -7473,7 +7486,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="83" t="s">
         <v>179</v>
       </c>
       <c r="E5" t="s">
@@ -7487,7 +7500,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="85" t="s">
+      <c r="D6" s="83" t="s">
         <v>180</v>
       </c>
       <c r="E6" t="s">
@@ -7501,7 +7514,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="83" t="s">
         <v>181</v>
       </c>
       <c r="E7" t="s">
@@ -7515,7 +7528,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="85" t="s">
+      <c r="D8" s="83" t="s">
         <v>182</v>
       </c>
       <c r="E8" t="s">
@@ -7529,7 +7542,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="83" t="s">
         <v>183</v>
       </c>
       <c r="E9" t="s">
@@ -7543,7 +7556,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="84" t="s">
         <v>184</v>
       </c>
       <c r="E10" t="s">
@@ -7557,7 +7570,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="84" t="s">
         <v>185</v>
       </c>
       <c r="E11" t="s">
@@ -7571,7 +7584,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="84" t="s">
         <v>186</v>
       </c>
       <c r="E12" t="s">
@@ -7585,7 +7598,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="D13" s="84" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
@@ -7599,7 +7612,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="84" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
@@ -7613,7 +7626,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="84" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
@@ -7627,7 +7640,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="98" t="s">
         <v>190</v>
       </c>
       <c r="E16" t="s">
@@ -7641,7 +7654,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="98" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
@@ -7655,7 +7668,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D18" s="98" t="s">
         <v>192</v>
       </c>
       <c r="E18" t="s">
@@ -7669,7 +7682,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="100" t="s">
+      <c r="D19" s="98" t="s">
         <v>193</v>
       </c>
       <c r="E19" t="s">
@@ -7683,7 +7696,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="88" t="s">
+      <c r="D20" s="86" t="s">
         <v>194</v>
       </c>
       <c r="E20" t="s">
@@ -7697,7 +7710,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="88" t="s">
+      <c r="D21" s="86" t="s">
         <v>195</v>
       </c>
       <c r="E21" t="s">
@@ -7711,7 +7724,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="88" t="s">
+      <c r="D22" s="86" t="s">
         <v>196</v>
       </c>
       <c r="E22" t="s">
@@ -7725,7 +7738,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="86" t="s">
         <v>197</v>
       </c>
       <c r="E23" t="s">
@@ -7739,7 +7752,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="89" t="s">
+      <c r="D24" s="87" t="s">
         <v>198</v>
       </c>
       <c r="E24" t="s">
@@ -7753,7 +7766,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="89" t="s">
+      <c r="D25" s="87" t="s">
         <v>199</v>
       </c>
       <c r="E25" t="s">
@@ -7767,7 +7780,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="89" t="s">
+      <c r="D26" s="87" t="s">
         <v>200</v>
       </c>
       <c r="E26" t="s">
@@ -7781,7 +7794,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="89" t="s">
+      <c r="D27" s="87" t="s">
         <v>201</v>
       </c>
       <c r="E27" t="s">
@@ -7795,7 +7808,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="85" t="s">
         <v>202</v>
       </c>
       <c r="E28" t="s">
@@ -7809,7 +7822,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="87" t="s">
+      <c r="D29" s="85" t="s">
         <v>203</v>
       </c>
       <c r="E29" t="s">
@@ -7823,7 +7836,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="87" t="s">
+      <c r="D30" s="85" t="s">
         <v>204</v>
       </c>
       <c r="E30" t="s">
@@ -7837,7 +7850,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="87" t="s">
+      <c r="D31" s="85" t="s">
         <v>205</v>
       </c>
       <c r="E31" t="s">
@@ -7851,7 +7864,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="87" t="s">
+      <c r="D32" s="85" t="s">
         <v>206</v>
       </c>
       <c r="G32" s="29">
@@ -7862,7 +7875,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="85" t="s">
         <v>207</v>
       </c>
       <c r="G33" s="29">
@@ -7906,7 +7919,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="101" t="s">
         <v>544</v>
       </c>
       <c r="E1" s="5">
@@ -7916,32 +7929,32 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="102" t="s">
         <v>545</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="102" t="s">
         <v>546</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="D3" s="103"/>
+      <c r="D3" s="101"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="D4" s="103"/>
+      <c r="D4" s="101"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="D5" s="103"/>
+      <c r="D5" s="101"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="D6" s="103"/>
+      <c r="D6" s="101"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7988,7 +8001,7 @@
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="95" t="s">
         <v>240</v>
       </c>
       <c r="E9" t="s">
@@ -8008,7 +8021,7 @@
       <c r="A10" s="29">
         <v>2</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="96" t="s">
         <v>241</v>
       </c>
       <c r="E10" t="s">
@@ -8028,7 +8041,7 @@
       <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="D11" s="98" t="s">
+      <c r="D11" s="96" t="s">
         <v>242</v>
       </c>
       <c r="E11" t="s">
@@ -8048,7 +8061,7 @@
       <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="96" t="s">
         <v>243</v>
       </c>
       <c r="E12" t="s">
@@ -8068,7 +8081,7 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="96" t="s">
         <v>244</v>
       </c>
       <c r="E13" t="s">
@@ -8088,7 +8101,7 @@
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="96" t="s">
         <v>245</v>
       </c>
       <c r="E14" t="s">
@@ -8108,7 +8121,7 @@
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="96" t="s">
         <v>246</v>
       </c>
       <c r="E15" t="s">
@@ -8128,7 +8141,7 @@
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="96" t="s">
         <v>247</v>
       </c>
       <c r="E16" t="s">
@@ -8148,7 +8161,7 @@
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="D17" s="98" t="s">
+      <c r="D17" s="96" t="s">
         <v>248</v>
       </c>
       <c r="E17" t="s">
@@ -8174,7 +8187,7 @@
       <c r="A18" s="29">
         <v>10</v>
       </c>
-      <c r="D18" s="99" t="s">
+      <c r="D18" s="97" t="s">
         <v>249</v>
       </c>
       <c r="E18" t="s">
@@ -8197,7 +8210,7 @@
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="101" t="s">
+      <c r="D19" s="99" t="s">
         <v>250</v>
       </c>
       <c r="E19" t="s">
@@ -8289,7 +8302,7 @@
       <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="99" t="s">
         <v>254</v>
       </c>
       <c r="E23" t="s">
@@ -8421,7 +8434,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="121" t="s">
+      <c r="D29" s="119" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -8441,7 +8454,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D30" s="106" t="s">
         <v>260</v>
       </c>
       <c r="E30" t="s">
@@ -8464,7 +8477,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="107" t="s">
+      <c r="D31" s="105" t="s">
         <v>261</v>
       </c>
       <c r="E31" t="s">
@@ -8493,7 +8506,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="107" t="s">
+      <c r="D32" s="105" t="s">
         <v>262</v>
       </c>
       <c r="E32" t="s">
@@ -8519,7 +8532,7 @@
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="109" t="s">
+      <c r="D33" s="107" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -8545,7 +8558,7 @@
       <c r="C34" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="D34" s="102" t="s">
+      <c r="D34" s="100" t="s">
         <v>538</v>
       </c>
       <c r="E34" t="s">
@@ -8567,12 +8580,12 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:11" s="92" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A36" s="91"/>
-      <c r="D36" s="93" t="s">
+    <row r="36" spans="1:11" s="90" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="89"/>
+      <c r="D36" s="91" t="s">
         <v>507</v>
       </c>
-      <c r="G36" s="94"/>
+      <c r="G36" s="92"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
@@ -8759,7 +8772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -8776,7 +8789,7 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1"/>
-      <c r="G1" s="106" t="s">
+      <c r="G1" s="104" t="s">
         <v>596</v>
       </c>
     </row>
@@ -8823,13 +8836,13 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="104" t="s">
         <v>566</v>
       </c>
-      <c r="C4" s="113" t="s">
+      <c r="C4" s="111" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="105"/>
+      <c r="F4" s="103"/>
       <c r="J4" s="16" t="s">
         <v>554</v>
       </c>
@@ -8838,13 +8851,13 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="104" t="s">
         <v>566</v>
       </c>
-      <c r="C5" s="114" t="s">
+      <c r="C5" s="112" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="105"/>
+      <c r="F5" s="103"/>
       <c r="J5" s="16" t="s">
         <v>554</v>
       </c>
@@ -8853,16 +8866,16 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="113" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="105">
+      <c r="F6" s="103">
         <v>3</v>
       </c>
-      <c r="G6" s="110" t="s">
+      <c r="G6" s="108" t="s">
         <v>560</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -8879,13 +8892,13 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="113" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="105">
+      <c r="F7" s="103">
         <v>3</v>
       </c>
       <c r="G7" t="s">
@@ -8902,13 +8915,13 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="115" t="s">
+      <c r="C8" s="113" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="105">
+      <c r="F8" s="103">
         <v>3</v>
       </c>
       <c r="G8" t="s">
@@ -8925,13 +8938,13 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="113" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="105">
+      <c r="F9" s="103">
         <v>3</v>
       </c>
       <c r="G9" t="s">
@@ -8948,16 +8961,16 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="C10" s="98" t="s">
+      <c r="C10" s="96" t="s">
         <v>217</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="105">
+      <c r="F10" s="103">
         <v>3</v>
       </c>
-      <c r="G10" s="112" t="s">
+      <c r="G10" s="110" t="s">
         <v>496</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -8974,16 +8987,16 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="115" t="s">
+      <c r="C11" s="113" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="105">
+      <c r="F11" s="103">
         <v>3</v>
       </c>
-      <c r="G11" s="111" t="s">
+      <c r="G11" s="109" t="s">
         <v>567</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -9003,13 +9016,13 @@
       <c r="B12" t="s">
         <v>541</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="113" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="105">
+      <c r="F12" s="103">
         <v>3</v>
       </c>
       <c r="G12" t="s">
@@ -9029,13 +9042,13 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="113" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="105">
+      <c r="F13" s="103">
         <v>3</v>
       </c>
       <c r="G13" t="s">
@@ -9052,13 +9065,13 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="104" t="s">
         <v>566</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="F14" s="105">
+      <c r="F14" s="103">
         <v>3</v>
       </c>
       <c r="G14" s="18"/>
@@ -9070,13 +9083,13 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="117" t="s">
+      <c r="C15" s="115" t="s">
         <v>222</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="105">
+      <c r="F15" s="103">
         <v>3</v>
       </c>
       <c r="J15" s="16" t="s">
@@ -9087,13 +9100,13 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="118" t="s">
+      <c r="C16" s="116" t="s">
         <v>223</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="105">
+      <c r="F16" s="103">
         <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
@@ -9104,13 +9117,13 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="118" t="s">
+      <c r="C17" s="116" t="s">
         <v>224</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="105">
+      <c r="F17" s="103">
         <v>3</v>
       </c>
       <c r="J17" s="16" t="s">
@@ -9121,13 +9134,13 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="116" t="s">
         <v>225</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="105">
+      <c r="F18" s="103">
         <v>3</v>
       </c>
       <c r="J18" s="16" t="s">
@@ -9138,13 +9151,13 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="128" t="s">
+      <c r="C19" s="126" t="s">
         <v>578</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="105">
+      <c r="F19" s="103">
         <v>3</v>
       </c>
       <c r="G19" t="s">
@@ -9158,13 +9171,13 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="127" t="s">
+      <c r="C20" s="125" t="s">
         <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="105">
+      <c r="F20" s="103">
         <v>3</v>
       </c>
       <c r="G20" t="s">
@@ -9178,13 +9191,13 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="127" t="s">
+      <c r="C21" s="125" t="s">
         <v>227</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="105">
+      <c r="F21" s="103">
         <v>3</v>
       </c>
       <c r="G21" t="s">
@@ -9198,13 +9211,13 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="127" t="s">
         <v>228</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="105">
+      <c r="F22" s="103">
         <v>3</v>
       </c>
       <c r="G22" t="s">
@@ -9221,13 +9234,13 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="118" t="s">
+      <c r="C23" s="116" t="s">
         <v>229</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="105">
+      <c r="F23" s="103">
         <v>3</v>
       </c>
       <c r="G23" t="s">
@@ -9244,13 +9257,13 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="118" t="s">
+      <c r="C24" s="116" t="s">
         <v>230</v>
       </c>
       <c r="E24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="105">
+      <c r="F24" s="103">
         <v>3</v>
       </c>
       <c r="G24" t="s">
@@ -9264,13 +9277,13 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="119" t="s">
+      <c r="C25" s="117" t="s">
         <v>231</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="105">
+      <c r="F25" s="103">
         <v>3</v>
       </c>
       <c r="G25" t="s">
@@ -9284,13 +9297,13 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="120" t="s">
+      <c r="C26" s="118" t="s">
         <v>232</v>
       </c>
       <c r="E26" t="s">
         <v>639</v>
       </c>
-      <c r="F26" s="105">
+      <c r="F26" s="103">
         <v>3</v>
       </c>
       <c r="G26" t="s">
@@ -9307,13 +9320,13 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="120" t="s">
+      <c r="C27" s="118" t="s">
         <v>233</v>
       </c>
       <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="105">
+      <c r="F27" s="103">
         <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
@@ -9330,13 +9343,13 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C28" s="118" t="s">
         <v>234</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="105">
+      <c r="F28" s="103">
         <v>3</v>
       </c>
       <c r="G28" s="18" t="s">
@@ -9350,13 +9363,13 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="120" t="s">
+      <c r="C29" s="118" t="s">
         <v>235</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="105">
+      <c r="F29" s="103">
         <v>3</v>
       </c>
       <c r="G29" t="s">
@@ -9370,13 +9383,13 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="120" t="s">
+      <c r="C30" s="118" t="s">
         <v>236</v>
       </c>
       <c r="E30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="105">
+      <c r="F30" s="103">
         <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
@@ -9390,13 +9403,13 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="120" t="s">
+      <c r="C31" s="118" t="s">
         <v>237</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>637</v>
       </c>
-      <c r="F31" s="105">
+      <c r="F31" s="103">
         <v>3</v>
       </c>
       <c r="G31" s="18" t="s">
@@ -9413,13 +9426,13 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="120" t="s">
+      <c r="C32" s="118" t="s">
         <v>238</v>
       </c>
       <c r="E32" t="s">
         <v>638</v>
       </c>
-      <c r="F32" s="105">
+      <c r="F32" s="103">
         <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
@@ -9436,16 +9449,16 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="104" t="s">
         <v>566</v>
       </c>
-      <c r="C33" s="126" t="s">
+      <c r="C33" s="124" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="124" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="123"/>
-      <c r="C45" s="125" t="s">
+    <row r="45" spans="1:3" s="122" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="121"/>
+      <c r="C45" s="123" t="s">
         <v>577</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-06-2021 -  2:32:25.16
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="648">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2316,6 +2316,9 @@
   </si>
   <si>
     <t>CP/RootToleafPathSumInRange.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>look for the video for understanding cost</t>
   </si>
 </sst>
 </file>
@@ -3604,7 +3607,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C13"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,6 +3667,9 @@
       <c r="C4" s="126" t="s">
         <v>263</v>
       </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
       <c r="F4" t="s">
         <v>100</v>
       </c>
@@ -3681,6 +3687,9 @@
       <c r="C5" s="125" t="s">
         <v>264</v>
       </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
       <c r="F5" t="s">
         <v>100</v>
       </c>
@@ -3698,6 +3707,9 @@
       <c r="C6" s="125" t="s">
         <v>265</v>
       </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
       <c r="F6" t="s">
         <v>100</v>
       </c>
@@ -3715,6 +3727,9 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
       <c r="F7" t="s">
         <v>100</v>
       </c>
@@ -3732,6 +3747,9 @@
       <c r="C8" s="125" t="s">
         <v>267</v>
       </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
       <c r="F8" t="s">
         <v>100</v>
       </c>
@@ -3749,6 +3767,9 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
       <c r="F9" t="s">
         <v>100</v>
       </c>
@@ -3763,6 +3784,9 @@
       <c r="C10" s="127" t="s">
         <v>269</v>
       </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
       <c r="F10" t="s">
         <v>100</v>
       </c>
@@ -3777,6 +3801,9 @@
       <c r="C11" s="132" t="s">
         <v>270</v>
       </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
       <c r="F11" t="s">
         <v>100</v>
       </c>
@@ -3791,6 +3818,9 @@
       <c r="C12" s="113" t="s">
         <v>271</v>
       </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
       <c r="F12" t="s">
         <v>100</v>
       </c>
@@ -3805,6 +3835,9 @@
       <c r="C13" s="139" t="s">
         <v>272</v>
       </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
       <c r="F13" s="18" t="s">
         <v>618</v>
       </c>
@@ -3819,6 +3852,9 @@
       <c r="C14" s="115" t="s">
         <v>273</v>
       </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
       <c r="F14" t="s">
         <v>645</v>
       </c>
@@ -3833,6 +3869,9 @@
       <c r="C15" s="116" t="s">
         <v>274</v>
       </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -3841,61 +3880,85 @@
       <c r="C16" s="116" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
       <c r="C17" s="116" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
       <c r="C18" s="116" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>16</v>
       </c>
       <c r="C19" s="116" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
       <c r="C20" s="116" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>18</v>
       </c>
       <c r="C21" s="116" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
       <c r="C22" s="116" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>20</v>
       </c>
       <c r="C23" s="117" t="s">
         <v>282</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
@@ -4716,7 +4779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -5675,530 +5738,529 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D22"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="8.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="66.7109375" style="15" customWidth="1"/>
-    <col min="10" max="10" width="57.28515625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="66.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="57.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>342</v>
       </c>
+      <c r="E1" s="13"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D2" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="J1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="14"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="14"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>0</v>
+      <c r="C3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>488</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D4" s="25" t="s">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="115" t="s">
+      <c r="C6" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5">
         <v>2</v>
       </c>
+      <c r="G6" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="H6" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="116" t="s">
+      <c r="C7" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5">
         <v>2</v>
       </c>
+      <c r="G7" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="H7" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="D8" s="117" t="s">
+      <c r="C8" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5">
         <v>2</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="C9" s="133" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="5">
         <v>2</v>
       </c>
+      <c r="H9" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="I9" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="D10" s="134" t="s">
+      <c r="C10" s="134" t="s">
         <v>139</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="E10" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="15" t="s">
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="134" t="s">
+      <c r="B11" s="80" t="s">
+        <v>647</v>
+      </c>
+      <c r="C11" s="134" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="E11" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="5">
         <v>2</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="D12" s="134" t="s">
+      <c r="C12" s="134" t="s">
         <v>140</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="H12" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="D13" s="135" t="s">
+      <c r="C13" s="135" t="s">
         <v>144</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="5">
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="5">
         <v>2</v>
       </c>
+      <c r="G13" s="15" t="s">
+        <v>464</v>
+      </c>
       <c r="H13" s="15" t="s">
-        <v>464</v>
+        <v>148</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="J13" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="D14" s="140" t="s">
+      <c r="C14" s="140" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="5">
+      <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="5">
         <v>2</v>
       </c>
+      <c r="G14" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="H14" s="15" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="J14" s="15" t="s">
         <v>481</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>10</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="B15" s="80" t="s">
         <v>478</v>
       </c>
-      <c r="D15" s="141" t="s">
+      <c r="C15" s="141" t="s">
         <v>151</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5">
         <v>2</v>
       </c>
+      <c r="G15" s="15" t="s">
+        <v>476</v>
+      </c>
       <c r="H15" s="15" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="J15" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="J15" s="16" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="D16" s="142" t="s">
+      <c r="C16" s="142" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="5">
         <v>2</v>
       </c>
+      <c r="H16" s="15" t="s">
+        <v>156</v>
+      </c>
       <c r="I16" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="J16" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="J16" s="16" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>12</v>
       </c>
-      <c r="D17" s="133" t="s">
+      <c r="C17" s="133" t="s">
         <v>154</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="5">
+      <c r="E17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="5">
         <v>2</v>
       </c>
+      <c r="G17" s="15" t="s">
+        <v>170</v>
+      </c>
       <c r="H17" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="J17" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="D18" s="134" t="s">
+      <c r="C18" s="134" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="E18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="5">
         <v>2</v>
       </c>
+      <c r="H18" s="15" t="s">
+        <v>161</v>
+      </c>
       <c r="I18" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="J18" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="J18" s="16" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="D19" s="134" t="s">
+      <c r="C19" s="134" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="5">
+      <c r="F19" s="5">
         <v>2</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="H19" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="J19" s="16" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="D20" s="134" t="s">
+      <c r="C20" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="E20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="5">
         <v>2</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="K20" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="D21" s="134" t="s">
+      <c r="C21" s="134" t="s">
         <v>163</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="E21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="5">
         <v>2</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="J21" s="16" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="D22" s="135" t="s">
+      <c r="C22" s="135" t="s">
         <v>166</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="E22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="5">
         <v>2</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="K22" s="16" t="s">
+      <c r="J22" s="16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="C23" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="H23" s="15" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="D24" s="82" t="s">
+      <c r="C24" s="82" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="64"/>
-    </row>
-    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="64"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>20</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="C26" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>21</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="C27" s="26" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf"/>
-    <hyperlink ref="K6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java"/>
-    <hyperlink ref="K7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java"/>
-    <hyperlink ref="K8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java"/>
-    <hyperlink ref="K9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java"/>
-    <hyperlink ref="K11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java"/>
-    <hyperlink ref="K12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java"/>
-    <hyperlink ref="K13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java"/>
-    <hyperlink ref="K14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java"/>
-    <hyperlink ref="K15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java"/>
-    <hyperlink ref="K16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java"/>
-    <hyperlink ref="K17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java"/>
-    <hyperlink ref="K18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java"/>
-    <hyperlink ref="K19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java"/>
-    <hyperlink ref="K21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java"/>
-    <hyperlink ref="K22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java"/>
-    <hyperlink ref="K20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java"/>
+    <hyperlink ref="D1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf"/>
+    <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java"/>
+    <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java"/>
+    <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java"/>
+    <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java"/>
+    <hyperlink ref="J11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java"/>
+    <hyperlink ref="J12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java"/>
+    <hyperlink ref="J13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java"/>
+    <hyperlink ref="J14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java"/>
+    <hyperlink ref="J15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java"/>
+    <hyperlink ref="J16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java"/>
+    <hyperlink ref="J17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java"/>
+    <hyperlink ref="J18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java"/>
+    <hyperlink ref="J19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java"/>
+    <hyperlink ref="J21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java"/>
+    <hyperlink ref="J22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java"/>
+    <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>
@@ -7899,7 +7961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -8772,7 +8834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 17:09:04.70
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="649">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2319,6 +2319,10 @@
   </si>
   <si>
     <t>look for the video for understanding cost</t>
+  </si>
+  <si>
+    <t>when we get the element of left side we swap, when we get the element of right side we increment the iterator
+and j will be pointitng at the 1st greater to pivot</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2720,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3063,12 +3067,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3099,6 +3097,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3458,10 +3474,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="130" t="s">
+      <c r="F2" s="145" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="130"/>
+      <c r="G2" s="145"/>
       <c r="J2" s="104" t="s">
         <v>327</v>
       </c>
@@ -3606,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,7 +3814,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="130" t="s">
         <v>270</v>
       </c>
       <c r="E11" s="5">
@@ -3832,7 +3848,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="139" t="s">
+      <c r="C13" s="137" t="s">
         <v>272</v>
       </c>
       <c r="E13" s="5">
@@ -3961,9 +3977,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="137" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="136"/>
-      <c r="C37" s="138" t="s">
+    <row r="37" spans="1:3" s="135" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="134"/>
+      <c r="C37" s="136" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5740,8 +5756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5892,7 +5908,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="131" t="s">
         <v>139</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -5915,7 +5931,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="132" t="s">
         <v>139</v>
       </c>
       <c r="E10" s="23" t="s">
@@ -5935,7 +5951,7 @@
       <c r="B11" s="80" t="s">
         <v>647</v>
       </c>
-      <c r="C11" s="134" t="s">
+      <c r="C11" s="132" t="s">
         <v>168</v>
       </c>
       <c r="E11" s="78" t="s">
@@ -5951,11 +5967,11 @@
         <v>460</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="C12" s="134" t="s">
+      <c r="C12" s="132" t="s">
         <v>140</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -5963,6 +5979,9 @@
       </c>
       <c r="F12" s="5">
         <v>3</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>648</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>145</v>
@@ -5975,7 +5994,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="133" t="s">
         <v>144</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -6001,7 +6020,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="C14" s="140" t="s">
+      <c r="C14" s="138" t="s">
         <v>149</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -6030,7 +6049,7 @@
       <c r="B15" s="80" t="s">
         <v>478</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="139" t="s">
         <v>151</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -6056,7 +6075,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="140" t="s">
         <v>153</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -6076,10 +6095,10 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="144">
         <v>12</v>
       </c>
-      <c r="C17" s="133" t="s">
+      <c r="C17" s="141" t="s">
         <v>154</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -6102,7 +6121,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="C18" s="134" t="s">
+      <c r="C18" s="142" t="s">
         <v>157</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -6125,7 +6144,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="C19" s="134" t="s">
+      <c r="C19" s="142" t="s">
         <v>159</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -6148,7 +6167,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="C20" s="134" t="s">
+      <c r="C20" s="142" t="s">
         <v>162</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -6168,7 +6187,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="C21" s="134" t="s">
+      <c r="C21" s="142" t="s">
         <v>163</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -6188,7 +6207,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="C22" s="135" t="s">
+      <c r="C22" s="143" t="s">
         <v>166</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -7211,15 +7230,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="146" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 17:20:49.25
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="652">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2323,6 +2323,17 @@
   <si>
     <t>when we get the element of left side we swap, when we get the element of right side we increment the iterator
 and j will be pointitng at the 1st greater to pivot</t>
+  </si>
+  <si>
+    <t>CP/PrintSingleChildNode.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>2 app</t>
+  </si>
+  <si>
+    <t>2 approach
+1- using parent and ndoe
+2. usng node</t>
   </si>
 </sst>
 </file>
@@ -3623,7 +3634,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -3910,8 +3921,17 @@
       <c r="E17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>650</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>651</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -3922,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -3933,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -3944,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>18</v>
       </c>
@@ -3955,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -3966,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -4002,9 +4022,10 @@
     <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
     <hyperlink ref="I13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
     <hyperlink ref="I14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
+    <hyperlink ref="I17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 17:32:03.65
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="654">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2334,6 +2334,12 @@
     <t>2 approach
 1- using parent and ndoe
 2. usng node</t>
+  </si>
+  <si>
+    <t>CP/TransformNormalToLeftClone.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>preorder(without returntype) and post order approach(with returhn type</t>
   </si>
 </sst>
 </file>
@@ -3634,7 +3640,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,7 +3895,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -3898,6 +3904,12 @@
       </c>
       <c r="E15" s="5">
         <v>0</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>653</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4023,9 +4035,10 @@
     <hyperlink ref="I13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
     <hyperlink ref="I14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
     <hyperlink ref="I17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
+    <hyperlink ref="I15" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 17:39:43.52
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="655">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2340,6 +2340,9 @@
   </si>
   <si>
     <t>preorder(without returntype) and post order approach(with returhn type</t>
+  </si>
+  <si>
+    <t>CP/TransformLeftCloneToNormal.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3640,7 +3643,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,6 +3924,9 @@
       </c>
       <c r="E16" s="5">
         <v>0</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4036,9 +4042,10 @@
     <hyperlink ref="I14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
     <hyperlink ref="I17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
     <hyperlink ref="I15" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
+    <hyperlink ref="I16" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 19:59:01.66
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -3642,7 +3642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -4054,7 +4054,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D13"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4197,7 +4197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14:D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 22:03:35.73
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="657">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2343,6 +2343,12 @@
   </si>
   <si>
     <t>CP/TransformLeftCloneToNormal.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/DiameterOfBT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>similar to generic tree</t>
   </si>
 </sst>
 </file>
@@ -2740,7 +2746,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3135,6 +3141,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3642,8 +3651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,7 +3894,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="56" t="s">
         <v>273</v>
       </c>
       <c r="E14" s="5">
@@ -3902,7 +3911,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="50" t="s">
         <v>274</v>
       </c>
       <c r="E15" s="5">
@@ -3919,7 +3928,7 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="50" t="s">
         <v>275</v>
       </c>
       <c r="E16" s="5">
@@ -3933,7 +3942,7 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="50" t="s">
         <v>276</v>
       </c>
       <c r="E17" s="5">
@@ -3953,7 +3962,7 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="50" t="s">
         <v>277</v>
       </c>
       <c r="E18" s="5">
@@ -3964,18 +3973,24 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="116" t="s">
+      <c r="C19" s="50" t="s">
         <v>278</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>656</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="116" t="s">
+      <c r="C20" s="51" t="s">
         <v>279</v>
       </c>
       <c r="E20" s="5">
@@ -3986,7 +4001,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="113" t="s">
         <v>280</v>
       </c>
       <c r="E21" s="5">
@@ -3997,7 +4012,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="116" t="s">
+      <c r="C22" s="113" t="s">
         <v>281</v>
       </c>
       <c r="E22" s="5">
@@ -4008,7 +4023,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="117" t="s">
+      <c r="C23" s="147" t="s">
         <v>282</v>
       </c>
       <c r="E23" s="5">
@@ -4043,9 +4058,10 @@
     <hyperlink ref="I17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
     <hyperlink ref="I15" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
     <hyperlink ref="I16" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
+    <hyperlink ref="I19" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -4197,8 +4213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 22:07:41.04
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="659">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2349,6 +2349,12 @@
   </si>
   <si>
     <t>similar to generic tree</t>
+  </si>
+  <si>
+    <t>CP/RemoveLeaves.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/TiltABT.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3652,7 +3658,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3968,6 +3974,9 @@
       <c r="E18" s="5">
         <v>0</v>
       </c>
+      <c r="I18" s="16" t="s">
+        <v>657</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -3986,7 +3995,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -3995,6 +4004,9 @@
       </c>
       <c r="E20" s="5">
         <v>0</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4059,9 +4071,11 @@
     <hyperlink ref="I15" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
     <hyperlink ref="I16" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
     <hyperlink ref="I19" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
+    <hyperlink ref="I18" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
+    <hyperlink ref="I20" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -4852,7 +4866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   05-06-2021 - 22:11:10.60
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="676">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2355,6 +2355,57 @@
   </si>
   <si>
     <t>CP/TiltABT.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/FloodFill.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KnightTraversal.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/NQueenOptionLevelApproach.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/NQueenSubsetApproach.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/TargetSumSubset.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintEncodings.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintKPC.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintStairPath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintMazePath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintMazePathWithJumps.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintPermutation.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintSubsequences.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetMazePath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetMazepathJumps.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetStairPaths.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetSubsequence.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/kpc.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3657,7 +3708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -4866,8 +4917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,6 +5411,9 @@
       <c r="I18" s="10" t="s">
         <v>108</v>
       </c>
+      <c r="K18" s="16" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -5383,6 +5437,9 @@
       <c r="H19" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="K19" s="16" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -5406,6 +5463,9 @@
       <c r="H20" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="K20" s="16" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -5429,6 +5489,9 @@
       <c r="H21" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="K21" s="16" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
@@ -5452,6 +5515,9 @@
       <c r="H22" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="K22" s="16" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -5481,6 +5547,9 @@
       <c r="J23" s="10" t="s">
         <v>102</v>
       </c>
+      <c r="K23" s="16" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -5510,6 +5579,9 @@
       <c r="J24" s="10" t="s">
         <v>106</v>
       </c>
+      <c r="K24" s="16" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -5536,7 +5608,9 @@
       <c r="I25" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="K25" s="16"/>
+      <c r="K25" s="16" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -5563,7 +5637,9 @@
       <c r="I26" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="K26" s="16"/>
+      <c r="K26" s="16" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -5593,7 +5669,9 @@
       <c r="J27" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="K27" s="16"/>
+      <c r="K27" s="16" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -5620,7 +5698,9 @@
       <c r="I28" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K28" s="16"/>
+      <c r="K28" s="16" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
@@ -5650,7 +5730,9 @@
       <c r="J29" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="16"/>
+      <c r="K29" s="16" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -5680,7 +5762,9 @@
       <c r="J30" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="K30" s="16"/>
+      <c r="K30" s="16" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -5710,7 +5794,9 @@
       <c r="J31" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="K31" s="16"/>
+      <c r="K31" s="16" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -5740,7 +5826,9 @@
       <c r="J32" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="K32" s="16"/>
+      <c r="K32" s="16" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="53" t="s">
@@ -5752,7 +5840,9 @@
       <c r="I33" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="K33" s="16"/>
+      <c r="K33" s="16" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
@@ -5782,7 +5872,9 @@
       <c r="J34" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="K34" s="16"/>
+      <c r="K34" s="16" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D35" s="16"/>
@@ -5817,9 +5909,26 @@
     <hyperlink ref="K15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/FirstIndex.java"/>
     <hyperlink ref="K16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/LastIndex.java"/>
     <hyperlink ref="K17" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/AllIndices.java"/>
+    <hyperlink ref="K30" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/FloodFill.java"/>
+    <hyperlink ref="K34" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightTraversal.java"/>
+    <hyperlink ref="K33" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenOptionLevelApproach.java"/>
+    <hyperlink ref="K32" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenSubsetApproach.java"/>
+    <hyperlink ref="K31" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/TargetSumSubset.java"/>
+    <hyperlink ref="K29" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintEncodings.java"/>
+    <hyperlink ref="K24" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintKPC.java"/>
+    <hyperlink ref="K25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintStairPath.java"/>
+    <hyperlink ref="K26" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePath.java"/>
+    <hyperlink ref="K27" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePathWithJumps.java"/>
+    <hyperlink ref="K28" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintPermutation.java"/>
+    <hyperlink ref="K23" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintSubsequences.java"/>
+    <hyperlink ref="K21" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazePath.java"/>
+    <hyperlink ref="K22" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazepathJumps.java"/>
+    <hyperlink ref="K20" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetStairPaths.java"/>
+    <hyperlink ref="K18" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetSubsequence.java"/>
+    <hyperlink ref="K19" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/kpc.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 12:16:54.58
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="676">
   <si>
     <t>TOPIC</t>
   </si>
@@ -4917,7 +4917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -5934,10 +5934,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E7" activeCellId="1" sqref="D1:D1048576 E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5945,35 +5945,33 @@
     <col min="1" max="1" width="9.140625" style="13"/>
     <col min="2" max="2" width="16.85546875" style="13" customWidth="1"/>
     <col min="3" max="3" width="46.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="66.7109375" style="15" customWidth="1"/>
-    <col min="9" max="9" width="57.28515625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="66.7109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="57.28515625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="14"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="14"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -5984,147 +5982,144 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>488</v>
       </c>
+      <c r="F3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="J4" s="16"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:10" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="5">
         <v>2</v>
       </c>
+      <c r="F6" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="G6" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I6" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="I6" s="16" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>2</v>
       </c>
       <c r="C7" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5">
         <v>2</v>
       </c>
+      <c r="F7" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="G7" s="15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="16" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="C8" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="I8" s="16" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="C9" s="131" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5">
         <v>2</v>
       </c>
+      <c r="G9" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="H9" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>5</v>
       </c>
       <c r="C10" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="15" t="s">
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>6</v>
       </c>
@@ -6134,95 +6129,95 @@
       <c r="C11" s="132" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="D11" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="5">
         <v>2</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="H11" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>7</v>
       </c>
       <c r="C12" s="132" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5">
         <v>3</v>
       </c>
+      <c r="F12" s="15" t="s">
+        <v>648</v>
+      </c>
       <c r="G12" s="15" t="s">
-        <v>648</v>
-      </c>
-      <c r="H12" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="I12" s="16" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>8</v>
       </c>
       <c r="C13" s="133" t="s">
         <v>144</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5">
         <v>2</v>
       </c>
+      <c r="F13" s="15" t="s">
+        <v>464</v>
+      </c>
       <c r="G13" s="15" t="s">
-        <v>464</v>
+        <v>148</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="I13" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="I13" s="16" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>9</v>
       </c>
       <c r="C14" s="138" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5">
         <v>2</v>
       </c>
+      <c r="F14" s="15" t="s">
+        <v>150</v>
+      </c>
       <c r="G14" s="15" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="I14" s="15" t="s">
         <v>481</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="I14" s="16" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>10</v>
       </c>
@@ -6232,189 +6227,189 @@
       <c r="C15" s="139" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5">
         <v>2</v>
       </c>
+      <c r="F15" s="15" t="s">
+        <v>476</v>
+      </c>
       <c r="G15" s="15" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="I15" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="I15" s="16" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>11</v>
       </c>
       <c r="C16" s="140" t="s">
         <v>153</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="5">
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5">
         <v>2</v>
       </c>
+      <c r="G16" s="15" t="s">
+        <v>156</v>
+      </c>
       <c r="H16" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="I16" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="I16" s="16" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="144">
         <v>12</v>
       </c>
       <c r="C17" s="141" t="s">
         <v>154</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5">
         <v>2</v>
       </c>
+      <c r="F17" s="15" t="s">
+        <v>170</v>
+      </c>
       <c r="G17" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="H17" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="I17" s="16" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>13</v>
       </c>
       <c r="C18" s="142" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="D18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5">
         <v>2</v>
       </c>
+      <c r="G18" s="15" t="s">
+        <v>161</v>
+      </c>
       <c r="H18" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="I18" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="I18" s="16" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>14</v>
       </c>
       <c r="C19" s="142" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="F19" s="5">
+      <c r="E19" s="5">
         <v>2</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="G19" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="I19" s="16" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>15</v>
       </c>
       <c r="C20" s="142" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="5">
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="5">
         <v>2</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="G20" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="I20" s="16" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>16</v>
       </c>
       <c r="C21" s="142" t="s">
         <v>163</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="5">
+      <c r="D21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="G21" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="I21" s="16" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
       <c r="C22" s="143" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="D22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="5">
         <v>2</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="G22" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="I22" s="16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>18</v>
       </c>
       <c r="C23" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="G23" s="15" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>19</v>
       </c>
@@ -6422,10 +6417,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="64"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>20</v>
       </c>
@@ -6433,7 +6428,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>21</v>
       </c>
@@ -6443,23 +6438,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf"/>
-    <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java"/>
-    <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java"/>
-    <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java"/>
-    <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java"/>
-    <hyperlink ref="J11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java"/>
-    <hyperlink ref="J12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java"/>
-    <hyperlink ref="J13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java"/>
-    <hyperlink ref="J14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java"/>
-    <hyperlink ref="J15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java"/>
-    <hyperlink ref="J16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java"/>
-    <hyperlink ref="J17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java"/>
-    <hyperlink ref="J18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java"/>
-    <hyperlink ref="J19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java"/>
-    <hyperlink ref="J21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java"/>
-    <hyperlink ref="J22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java"/>
-    <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java"/>
+    <hyperlink ref="I8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java"/>
+    <hyperlink ref="I9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java"/>
+    <hyperlink ref="I11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java"/>
+    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java"/>
+    <hyperlink ref="I13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java"/>
+    <hyperlink ref="I14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java"/>
+    <hyperlink ref="I15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java"/>
+    <hyperlink ref="I16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java"/>
+    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java"/>
+    <hyperlink ref="I18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java"/>
+    <hyperlink ref="I19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java"/>
+    <hyperlink ref="I21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java"/>
+    <hyperlink ref="I22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java"/>
+    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 19:23:46.46
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="677">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2406,6 +2406,9 @@
   </si>
   <si>
     <t>CP/kpc.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IsBinarySearchTree.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3193,14 +3196,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3560,10 +3563,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="145" t="s">
+      <c r="F2" s="146" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="145"/>
+      <c r="G2" s="146"/>
       <c r="J2" s="104" t="s">
         <v>327</v>
       </c>
@@ -3708,8 +3711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4070,6 +4073,9 @@
       <c r="E21" s="5">
         <v>0</v>
       </c>
+      <c r="I21" s="16" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -4086,7 +4092,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="147" t="s">
+      <c r="C23" s="145" t="s">
         <v>282</v>
       </c>
       <c r="E23" s="5">
@@ -4124,9 +4130,10 @@
     <hyperlink ref="I19" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
     <hyperlink ref="I18" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
     <hyperlink ref="I20" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
+    <hyperlink ref="I21" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -5936,8 +5943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" activeCellId="1" sqref="D1:D1048576 E7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7405,15 +7412,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="147" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 19:30:24.28
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="678">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2409,6 +2409,9 @@
   </si>
   <si>
     <t>CP/IsBinarySearchTree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IsBalancesBST.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3712,7 +3715,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,6 +4089,9 @@
       </c>
       <c r="E22" s="5">
         <v>0</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4131,9 +4137,10 @@
     <hyperlink ref="I18" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
     <hyperlink ref="I20" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
     <hyperlink ref="I21" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
+    <hyperlink ref="I22" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 20:09:58.48
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="679">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2412,6 +2412,9 @@
   </si>
   <si>
     <t>CP/IsBalancesBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LargestBSTSubtree.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3715,7 +3718,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4103,6 +4106,9 @@
       </c>
       <c r="E23" s="5">
         <v>0</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="135" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
@@ -4138,9 +4144,10 @@
     <hyperlink ref="I20" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
     <hyperlink ref="I21" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
     <hyperlink ref="I22" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java"/>
+    <hyperlink ref="I23" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 22:57:31.00
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="679">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3718,7 +3718,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D7" sqref="D7:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3858,6 +3858,9 @@
       <c r="C8" s="125" t="s">
         <v>267</v>
       </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
@@ -3895,6 +3898,9 @@
       <c r="C10" s="127" t="s">
         <v>269</v>
       </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="5">
         <v>0</v>
       </c>
@@ -3912,6 +3918,9 @@
       <c r="C11" s="130" t="s">
         <v>270</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="5">
         <v>0</v>
       </c>
@@ -3929,6 +3938,9 @@
       <c r="C12" s="113" t="s">
         <v>271</v>
       </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" s="5">
         <v>0</v>
       </c>
@@ -3946,6 +3958,9 @@
       <c r="C13" s="137" t="s">
         <v>272</v>
       </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" s="5">
         <v>0</v>
       </c>
@@ -3963,6 +3978,9 @@
       <c r="C14" s="56" t="s">
         <v>273</v>
       </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="5">
         <v>0</v>
       </c>
@@ -3980,6 +3998,9 @@
       <c r="C15" s="50" t="s">
         <v>274</v>
       </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
@@ -3997,6 +4018,9 @@
       <c r="C16" s="50" t="s">
         <v>275</v>
       </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
@@ -4011,6 +4035,9 @@
       <c r="C17" s="50" t="s">
         <v>276</v>
       </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
@@ -4031,6 +4058,9 @@
       <c r="C18" s="50" t="s">
         <v>277</v>
       </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
@@ -4045,6 +4075,9 @@
       <c r="C19" s="50" t="s">
         <v>278</v>
       </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
@@ -4062,6 +4095,9 @@
       <c r="C20" s="51" t="s">
         <v>279</v>
       </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
       <c r="E20" s="5">
         <v>0</v>
       </c>
@@ -4076,6 +4112,9 @@
       <c r="C21" s="113" t="s">
         <v>280</v>
       </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
       <c r="E21" s="5">
         <v>0</v>
       </c>
@@ -4090,6 +4129,9 @@
       <c r="C22" s="113" t="s">
         <v>281</v>
       </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
       <c r="E22" s="5">
         <v>0</v>
       </c>
@@ -4103,6 +4145,9 @@
       </c>
       <c r="C23" s="145" t="s">
         <v>282</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   06-06-2021 - 23:31:53.51
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="679">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3717,7 +3717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7:D23"/>
     </sheetView>
   </sheetViews>
@@ -4198,140 +4198,143 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="41.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="47.7109375" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
-    <col min="10" max="10" width="42.42578125" customWidth="1"/>
-    <col min="11" max="11" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.85546875" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" customWidth="1"/>
+    <col min="10" max="10" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>0</v>
+      <c r="C3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="B4" s="104" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" s="94" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="94" t="s">
+      <c r="B5" s="104" t="s">
+        <v>597</v>
+      </c>
+      <c r="C5" s="94" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="94" t="s">
+      <c r="C6" s="94" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="C7" s="94" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="94" t="s">
+      <c r="C8" s="94" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="C9" s="94" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="C10" s="94" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="C11" s="94" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="94" t="s">
+      <c r="C12" s="94" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="94" t="s">
+      <c r="C13" s="94" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   07-06-2021 -  0:44:22.30
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="680">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2415,6 +2415,9 @@
   </si>
   <si>
     <t>CP/LargestBSTSubtree.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -3717,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4198,29 +4201,29 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="41.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="47.7109375" customWidth="1"/>
-    <col min="8" max="8" width="39.85546875" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="9" max="9" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
@@ -4231,39 +4234,36 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="F3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="104" t="s">
-        <v>597</v>
+        <v>679</v>
       </c>
       <c r="C4" s="94" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   08-06-2021 - 22:06:08.59
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="681">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2418,6 +2418,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CP/PrintKDistanceAwaynode.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3724,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,7 +3785,7 @@
         <v>263</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
         <v>100</v>
@@ -3802,7 +3805,7 @@
         <v>264</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
@@ -3822,7 +3825,7 @@
         <v>265</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>100</v>
@@ -3842,7 +3845,7 @@
         <v>34</v>
       </c>
       <c r="E7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
         <v>100</v>
@@ -3865,7 +3868,7 @@
         <v>34</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
         <v>100</v>
@@ -3885,7 +3888,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
         <v>100</v>
@@ -3905,7 +3908,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>100</v>
@@ -3925,7 +3928,7 @@
         <v>34</v>
       </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>100</v>
@@ -3945,7 +3948,7 @@
         <v>34</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>100</v>
@@ -3971,7 +3974,7 @@
         <v>618</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>644</v>
+        <v>680</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4182,17 +4185,17 @@
     <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
     <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java"/>
     <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
-    <hyperlink ref="I13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
-    <hyperlink ref="I14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
-    <hyperlink ref="I17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
-    <hyperlink ref="I15" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
-    <hyperlink ref="I16" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
-    <hyperlink ref="I19" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
-    <hyperlink ref="I18" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
-    <hyperlink ref="I20" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
-    <hyperlink ref="I21" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
-    <hyperlink ref="I22" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java"/>
-    <hyperlink ref="I23" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java"/>
+    <hyperlink ref="I14" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
+    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
+    <hyperlink ref="I15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
+    <hyperlink ref="I16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
+    <hyperlink ref="I19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
+    <hyperlink ref="I18" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
+    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
+    <hyperlink ref="I21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
+    <hyperlink ref="I22" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java"/>
+    <hyperlink ref="I23" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java"/>
+    <hyperlink ref="I13" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
@@ -6005,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 10:52:41.58
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="681">
   <si>
     <t>TOPIC</t>
   </si>
@@ -3723,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3968,7 +3968,7 @@
         <v>34</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>618</v>
@@ -3988,7 +3988,7 @@
         <v>34</v>
       </c>
       <c r="E14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>645</v>
@@ -4008,7 +4008,7 @@
         <v>34</v>
       </c>
       <c r="E15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>653</v>
@@ -4028,7 +4028,7 @@
         <v>34</v>
       </c>
       <c r="E16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>654</v>
@@ -4045,7 +4045,7 @@
         <v>34</v>
       </c>
       <c r="E17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>650</v>
@@ -4068,7 +4068,7 @@
         <v>34</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>657</v>
@@ -4085,7 +4085,7 @@
         <v>34</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>656</v>
@@ -4105,7 +4105,7 @@
         <v>34</v>
       </c>
       <c r="E20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>658</v>
@@ -4206,8 +4206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4265,6 +4265,9 @@
       <c r="C4" s="94" t="s">
         <v>283</v>
       </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -4276,6 +4279,9 @@
       <c r="C5" s="94" t="s">
         <v>284</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -4284,6 +4290,9 @@
       <c r="C6" s="94" t="s">
         <v>285</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -4292,6 +4301,9 @@
       <c r="C7" s="94" t="s">
         <v>286</v>
       </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -4308,6 +4320,9 @@
       <c r="C9" s="94" t="s">
         <v>288</v>
       </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -4316,6 +4331,9 @@
       <c r="C10" s="94" t="s">
         <v>289</v>
       </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -4324,6 +4342,9 @@
       <c r="C11" s="94" t="s">
         <v>290</v>
       </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -4332,6 +4353,9 @@
       <c r="C12" s="94" t="s">
         <v>291</v>
       </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -4339,6 +4363,9 @@
       </c>
       <c r="C13" s="94" t="s">
         <v>292</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 14:30:23.59
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="685">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2421,6 +2421,20 @@
   </si>
   <si>
     <t>CP/PrintKDistanceAwaynode.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>better way to find the intersection of 2 array</t>
+  </si>
+  <si>
+    <t>complexity: of recursive: call ^height</t>
+  </si>
+  <si>
+    <t>if it seems like n^ n  = n! complexity</t>
+  </si>
+  <si>
+    <t>1. get presence
+2. get startingpoint
+3. update the starting ans max length</t>
   </si>
 </sst>
 </file>
@@ -2818,7 +2832,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3216,6 +3230,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -4206,8 +4226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4375,172 +4395,181 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="4" max="4" width="41.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" customWidth="1"/>
-    <col min="9" max="9" width="57.140625" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="57.140625" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="B4" s="104" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" s="149" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="C5" s="149" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="149" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="C7" s="149" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="C8" s="149" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="18" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="B9" s="104" t="s">
+        <v>597</v>
+      </c>
+      <c r="C9" s="130" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="C10" s="113" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="C11" s="113" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="C12" s="113" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="C13" s="145" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="C14" s="115" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="D15" s="81" t="s">
+      <c r="C15" s="116" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="C16" s="116" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="C17" s="117" t="s">
         <v>306</v>
       </c>
     </row>
@@ -5016,8 +5045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5034,14 +5063,19 @@
     <col min="10" max="10" width="30" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="I1" s="148" t="s">
+        <v>682</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D2" s="8"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 18:38:12.16
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="690">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2435,6 +2435,21 @@
     <t>1. get presence
 2. get startingpoint
 3. update the starting ans max length</t>
+  </si>
+  <si>
+    <t>CP/GetCommonElements.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetCommonElements2.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/HashMapUsage.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/HighestFrequencyCharacter.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LongestConsecutiveSequenceOfElements.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4398,7 +4413,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4459,6 +4474,9 @@
       <c r="C4" s="149" t="s">
         <v>293</v>
       </c>
+      <c r="J4" s="16" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -4467,6 +4485,9 @@
       <c r="C5" s="149" t="s">
         <v>294</v>
       </c>
+      <c r="J5" s="16" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -4475,6 +4496,9 @@
       <c r="C6" s="149" t="s">
         <v>295</v>
       </c>
+      <c r="J6" s="16" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -4486,6 +4510,9 @@
       <c r="G7" t="s">
         <v>681</v>
       </c>
+      <c r="J7" s="16" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
@@ -4497,6 +4524,9 @@
       <c r="G8" s="18" t="s">
         <v>684</v>
       </c>
+      <c r="J8" s="16" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -4574,6 +4604,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java"/>
+    <hyperlink ref="J7" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java"/>
+    <hyperlink ref="J4" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java"/>
+    <hyperlink ref="J5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java"/>
+    <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 18:48:02.29
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="691">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2450,6 +2450,9 @@
   </si>
   <si>
     <t>CP/LongestConsecutiveSequenceOfElements.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KLargestElement.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4413,7 +4416,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,6 +4549,9 @@
       <c r="C10" s="113" t="s">
         <v>299</v>
       </c>
+      <c r="J10" s="16" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -4610,6 +4616,7 @@
     <hyperlink ref="J4" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java"/>
     <hyperlink ref="J5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java"/>
     <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java"/>
+    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8325,7 +8332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -9198,7 +9205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 19:02:55.77
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="692">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2453,6 +2453,9 @@
   </si>
   <si>
     <t>CP/KLargestElement.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/SortKUnSorted.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4416,7 +4419,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,7 +4545,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -4553,12 +4556,15 @@
         <v>690</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="C11" s="113" t="s">
         <v>300</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4573,7 +4579,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="145" t="s">
+      <c r="C13" s="137" t="s">
         <v>302</v>
       </c>
     </row>
@@ -4617,6 +4623,7 @@
     <hyperlink ref="J5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java"/>
     <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java"/>
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
+    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   12-06-2021 - 21:55:05.58
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="693">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2456,6 +2456,9 @@
   </si>
   <si>
     <t>CP/SortKUnSorted.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/MedianPriorityQ.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4419,7 +4422,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4574,6 +4577,9 @@
       <c r="C12" s="113" t="s">
         <v>301</v>
       </c>
+      <c r="J12" s="16" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
@@ -4624,6 +4630,7 @@
     <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java"/>
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
     <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java"/>
+    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  0:01:07.65
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -3333,6 +3333,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>372398</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5800725" y="5867400"/>
+          <a:ext cx="6611273" cy="1667108"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3601,7 +3639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
@@ -4422,7 +4460,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  0:39:42.93
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="694">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2459,6 +2459,9 @@
   </si>
   <si>
     <t>CP/MedianPriorityQ.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GenericHM.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4460,7 +4463,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,6 +4637,9 @@
       <c r="C14" s="115" t="s">
         <v>303</v>
       </c>
+      <c r="J14" s="16" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -4669,6 +4675,7 @@
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
     <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java"/>
     <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java"/>
+    <hyperlink ref="J14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9257,7 +9264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  0:51:07.50
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="698">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2462,6 +2462,18 @@
   </si>
   <si>
     <t>CP/GenericHM.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/AddNodeToBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/LcaInBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/ReplaceNodeSumOfLargerValue.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/SizeMinMaxFindSum.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4291,8 +4303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4378,6 +4390,9 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
+      <c r="I6" s="16" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -4389,6 +4404,9 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
+      <c r="I7" s="16" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -4408,6 +4426,9 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
+      <c r="I9" s="16" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -4419,6 +4440,9 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
+      <c r="I10" s="16" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -4454,6 +4478,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I7" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/AddNodeToBST.java"/>
+    <hyperlink ref="I10" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/LcaInBST.java"/>
+    <hyperlink ref="I9" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/ReplaceNodeSumOfLargerValue.java"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/SizeMinMaxFindSum.java"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4462,7 +4492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  1:00:55.49
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="698">
   <si>
     <t>TOPIC</t>
   </si>
@@ -4304,7 +4304,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4469,6 +4469,9 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
+      </c>
+      <c r="B13" s="104" t="s">
+        <v>597</v>
       </c>
       <c r="C13" s="94" t="s">
         <v>292</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  1:02:08.48
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="701">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2475,12 +2475,21 @@
   <si>
     <t>CP/SizeMinMaxFindSum.java at main · spartan4cs/CP (github.com)</t>
   </si>
+  <si>
+    <t>CP/TargetSumPairInBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintInRangeInBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/RemoveNodeFromBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2605,8 +2614,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2702,6 +2718,11 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -2853,7 +2874,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2870,8 +2891,9 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3276,8 +3298,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" xfId="16" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="9" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="11" builtinId="31"/>
@@ -3292,6 +3317,7 @@
     <cellStyle name="Bad" xfId="14" builtinId="27"/>
     <cellStyle name="Good" xfId="8" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -4303,8 +4329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,7 +4410,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="150" t="s">
         <v>285</v>
       </c>
       <c r="D6" t="s">
@@ -4398,7 +4424,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="150" t="s">
         <v>286</v>
       </c>
       <c r="D7" t="s">
@@ -4412,15 +4438,18 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="150" t="s">
         <v>287</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="150" t="s">
         <v>288</v>
       </c>
       <c r="D9" t="s">
@@ -4434,7 +4463,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="150" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
@@ -4448,22 +4477,28 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="94" t="s">
+      <c r="C11" s="150" t="s">
         <v>290</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="94" t="s">
+      <c r="C12" s="150" t="s">
         <v>291</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4486,6 +4521,9 @@
     <hyperlink ref="I10" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/LcaInBST.java"/>
     <hyperlink ref="I9" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/ReplaceNodeSumOfLargerValue.java"/>
     <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/SizeMinMaxFindSum.java"/>
+    <hyperlink ref="I12" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/TargetSumPairInBST.java"/>
+    <hyperlink ref="I11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/PrintInRangeInBST.java"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/RemoveNodeFromBST.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4495,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4655,7 +4693,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 -  1:21:20.25
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="700">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2474,9 +2474,6 @@
   </si>
   <si>
     <t>CP/SizeMinMaxFindSum.java at main · spartan4cs/CP (github.com)</t>
-  </si>
-  <si>
-    <t>CP/TargetSumPairInBST.java at main · spartan4cs/CP (github.com)</t>
   </si>
   <si>
     <t>CP/PrintInRangeInBST.java at main · spartan4cs/CP (github.com)</t>
@@ -4329,8 +4326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4442,7 +4439,7 @@
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4484,7 +4481,7 @@
         <v>34</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4498,7 +4495,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>698</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4521,9 +4518,9 @@
     <hyperlink ref="I10" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/LcaInBST.java"/>
     <hyperlink ref="I9" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/ReplaceNodeSumOfLargerValue.java"/>
     <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/SizeMinMaxFindSum.java"/>
-    <hyperlink ref="I12" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/TargetSumPairInBST.java"/>
-    <hyperlink ref="I11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/PrintInRangeInBST.java"/>
-    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/RemoveNodeFromBST.java"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/PrintInRangeInBST.java"/>
+    <hyperlink ref="I8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/RemoveNodeFromBST.java"/>
+    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/TargetSumPair.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4533,8 +4530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated code on timestamp:   13-06-2021 - 12:06:21.72
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -3284,19 +3284,19 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" xfId="16" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" xfId="16" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3695,10 +3695,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="149" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="146"/>
+      <c r="G2" s="149"/>
       <c r="J2" s="104" t="s">
         <v>327</v>
       </c>
@@ -4326,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -4407,7 +4407,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="150" t="s">
+      <c r="C6" s="148" t="s">
         <v>285</v>
       </c>
       <c r="D6" t="s">
@@ -4421,7 +4421,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="150" t="s">
+      <c r="C7" s="148" t="s">
         <v>286</v>
       </c>
       <c r="D7" t="s">
@@ -4435,7 +4435,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="150" t="s">
+      <c r="C8" s="148" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -4446,7 +4446,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="150" t="s">
+      <c r="C9" s="148" t="s">
         <v>288</v>
       </c>
       <c r="D9" t="s">
@@ -4460,7 +4460,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="150" t="s">
+      <c r="C10" s="148" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
@@ -4474,7 +4474,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="150" t="s">
+      <c r="C11" s="148" t="s">
         <v>290</v>
       </c>
       <c r="D11" t="s">
@@ -4488,7 +4488,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="150" t="s">
+      <c r="C12" s="148" t="s">
         <v>291</v>
       </c>
       <c r="D12" t="s">
@@ -4530,8 +4530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,7 +4589,7 @@
       <c r="B4" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="147" t="s">
         <v>293</v>
       </c>
       <c r="J4" s="16" t="s">
@@ -4600,7 +4600,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="149" t="s">
+      <c r="C5" s="147" t="s">
         <v>294</v>
       </c>
       <c r="J5" s="16" t="s">
@@ -4611,7 +4611,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="149" t="s">
+      <c r="C6" s="147" t="s">
         <v>295</v>
       </c>
       <c r="J6" s="16" t="s">
@@ -4622,7 +4622,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="149" t="s">
+      <c r="C7" s="147" t="s">
         <v>296</v>
       </c>
       <c r="G7" t="s">
@@ -4636,7 +4636,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="149" t="s">
+      <c r="C8" s="147" t="s">
         <v>297</v>
       </c>
       <c r="G8" s="18" t="s">
@@ -5241,7 +5241,7 @@
       <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="148" t="s">
+      <c r="I1" s="146" t="s">
         <v>682</v>
       </c>
       <c r="J1" s="11" t="s">
@@ -7709,15 +7709,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="150" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   14-06-2021 -  0:22:41.17
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="701">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>CP/RemoveNodeFromBST.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/CustomPriorityQueue.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4530,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4706,28 +4709,37 @@
         <v>303</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>12</v>
       </c>
       <c r="C15" s="116" t="s">
         <v>304</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="B16" s="104" t="s">
+        <v>597</v>
+      </c>
+      <c r="C16" s="115" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>14</v>
+      </c>
+      <c r="B17" s="104" t="s">
+        <v>597</v>
       </c>
       <c r="C17" s="117" t="s">
         <v>306</v>
@@ -4743,7 +4755,8 @@
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
     <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java"/>
     <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java"/>
-    <hyperlink ref="J14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java"/>
+    <hyperlink ref="J15" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java"/>
+    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   14-06-2021 -  0:33:47.09
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="702">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2483,6 +2483,9 @@
   </si>
   <si>
     <t>CP/CustomPriorityQueue.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/MergeKSortedList.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4533,8 +4536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4700,6 +4703,9 @@
       <c r="C13" s="137" t="s">
         <v>302</v>
       </c>
+      <c r="J13" s="21" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -4757,6 +4763,7 @@
     <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java"/>
     <hyperlink ref="J15" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java"/>
     <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java"/>
+    <hyperlink ref="J13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2021 -  1:35:06.90
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="707">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2486,6 +2486,24 @@
   </si>
   <si>
     <t>CP/MergeKSortedList.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>this is basically dfc recursion</t>
+  </si>
+  <si>
+    <t>vertices as current level
+neighbour as next level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notice that isme baxktrackign bhi ho rha he while dry run
+generic tree jaise solve ho rha he jisme base case nhi lagti, and jitne no of edges he utna hi call ho  rha he 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norml level option se recursion ho rha he </t>
+  </si>
+  <si>
+    <t>need to do sumit sir video</t>
   </si>
 </sst>
 </file>
@@ -2896,7 +2914,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3246,13 +3264,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
@@ -3274,15 +3286,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="6" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3303,6 +3306,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3701,10 +3710,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="144" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="149"/>
+      <c r="G2" s="144"/>
       <c r="J2" s="104" t="s">
         <v>327</v>
       </c>
@@ -3850,7 +3859,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3865,7 +3874,9 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="C1"/>
+      <c r="C1" s="25" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2"/>
@@ -4087,7 +4098,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="135" t="s">
         <v>272</v>
       </c>
       <c r="D13" t="s">
@@ -4275,7 +4286,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="145" t="s">
+      <c r="C23" s="140" t="s">
         <v>282</v>
       </c>
       <c r="D23" t="s">
@@ -4288,9 +4299,9 @@
         <v>678</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="135" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="134"/>
-      <c r="C37" s="136" t="s">
+    <row r="37" spans="1:3" s="133" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="132"/>
+      <c r="C37" s="134" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4333,7 +4344,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4347,7 +4358,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1"/>
+      <c r="C1" s="25" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2"/>
@@ -4413,7 +4426,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="143" t="s">
         <v>285</v>
       </c>
       <c r="D6" t="s">
@@ -4427,7 +4440,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="143" t="s">
         <v>286</v>
       </c>
       <c r="D7" t="s">
@@ -4441,7 +4454,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="148" t="s">
+      <c r="C8" s="143" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -4452,7 +4465,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="148" t="s">
+      <c r="C9" s="143" t="s">
         <v>288</v>
       </c>
       <c r="D9" t="s">
@@ -4466,7 +4479,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="148" t="s">
+      <c r="C10" s="143" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
@@ -4480,7 +4493,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="148" t="s">
+      <c r="C11" s="143" t="s">
         <v>290</v>
       </c>
       <c r="D11" t="s">
@@ -4494,7 +4507,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="148" t="s">
+      <c r="C12" s="143" t="s">
         <v>291</v>
       </c>
       <c r="D12" t="s">
@@ -4536,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4552,6 +4565,9 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
+      <c r="C1" s="25" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
@@ -4595,8 +4611,11 @@
       <c r="B4" s="104" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="147" t="s">
+      <c r="C4" s="142" t="s">
         <v>293</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>687</v>
@@ -4606,8 +4625,11 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="142" t="s">
         <v>294</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>688</v>
@@ -4617,8 +4639,11 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="142" t="s">
         <v>295</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>685</v>
@@ -4628,8 +4653,11 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="147" t="s">
+      <c r="C7" s="142" t="s">
         <v>296</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>681</v>
@@ -4642,8 +4670,11 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="147" t="s">
+      <c r="C8" s="142" t="s">
         <v>297</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>684</v>
@@ -4662,6 +4693,9 @@
       <c r="C9" s="130" t="s">
         <v>298</v>
       </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -4670,6 +4704,9 @@
       <c r="C10" s="113" t="s">
         <v>299</v>
       </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
       <c r="J10" s="16" t="s">
         <v>690</v>
       </c>
@@ -4681,6 +4718,9 @@
       <c r="C11" s="113" t="s">
         <v>300</v>
       </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
       <c r="J11" s="16" t="s">
         <v>691</v>
       </c>
@@ -4692,6 +4732,9 @@
       <c r="C12" s="113" t="s">
         <v>301</v>
       </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
       <c r="J12" s="16" t="s">
         <v>692</v>
       </c>
@@ -4700,8 +4743,11 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="135" t="s">
         <v>302</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
       </c>
       <c r="J13" s="21" t="s">
         <v>701</v>
@@ -4714,6 +4760,9 @@
       <c r="C14" s="115" t="s">
         <v>303</v>
       </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
       <c r="J14" s="16" t="s">
         <v>700</v>
       </c>
@@ -4724,6 +4773,9 @@
       </c>
       <c r="C15" s="116" t="s">
         <v>304</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>693</v>
@@ -4774,7 +4826,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,24 +4887,39 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
+      <c r="C4" s="104" t="s">
+        <v>597</v>
+      </c>
       <c r="D4" s="93" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>2</v>
       </c>
       <c r="D5" s="93" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>702</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
       <c r="D6" s="93" t="s">
         <v>310</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="I6" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5261,7 +5328,7 @@
       <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="146" t="s">
+      <c r="I1" s="141" t="s">
         <v>682</v>
       </c>
       <c r="J1" s="11" t="s">
@@ -6260,8 +6327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6407,7 +6474,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="146" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -6430,7 +6497,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="C10" s="131" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="23" t="s">
@@ -6450,7 +6517,7 @@
       <c r="B11" s="80" t="s">
         <v>647</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="131" t="s">
         <v>168</v>
       </c>
       <c r="D11" s="78" t="s">
@@ -6470,7 +6537,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="C12" s="132" t="s">
+      <c r="C12" s="131" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -6493,7 +6560,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="147" t="s">
         <v>144</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -6519,7 +6586,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="136" t="s">
         <v>149</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -6548,7 +6615,7 @@
       <c r="B15" s="80" t="s">
         <v>478</v>
       </c>
-      <c r="C15" s="139" t="s">
+      <c r="C15" s="137" t="s">
         <v>151</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -6574,7 +6641,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="C16" s="140" t="s">
+      <c r="C16" s="138" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -6594,10 +6661,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="144">
+      <c r="A17" s="139">
         <v>12</v>
       </c>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="146" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -6620,7 +6687,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="C18" s="142" t="s">
+      <c r="C18" s="118" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -6643,7 +6710,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="C19" s="142" t="s">
+      <c r="C19" s="118" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -6666,7 +6733,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="C20" s="142" t="s">
+      <c r="C20" s="118" t="s">
         <v>162</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -6686,7 +6753,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="118" t="s">
         <v>163</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -6706,7 +6773,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="C22" s="143" t="s">
+      <c r="C22" s="147" t="s">
         <v>166</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -7729,15 +7796,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="145" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8479,7 +8546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -9352,8 +9419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9368,7 +9435,9 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="C1"/>
+      <c r="C1" t="s">
+        <v>706</v>
+      </c>
       <c r="G1" s="104" t="s">
         <v>596</v>
       </c>

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2021 -  2:12:26.88
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="713">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2504,6 +2504,24 @@
   </si>
   <si>
     <t>need to do sumit sir video</t>
+  </si>
+  <si>
+    <t>CP/HasPath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PrintAllPath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>stack size max =10000</t>
+  </si>
+  <si>
+    <t>if we get the problem with stack &gt;10000 which can be presnt in graph problems</t>
+  </si>
+  <si>
+    <t>then use the sstack using linked list</t>
+  </si>
+  <si>
+    <t>linked lis.remove</t>
   </si>
 </sst>
 </file>
@@ -2914,7 +2932,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3147,9 +3165,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="11" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3359,7 +3374,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>186051</xdr:rowOff>
+      <xdr:rowOff>176526</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3692,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3710,14 +3725,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="144" t="s">
+      <c r="F2" s="143" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="144"/>
-      <c r="J2" s="104" t="s">
+      <c r="G2" s="143"/>
+      <c r="J2" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="K2" s="104"/>
+      <c r="K2" s="103"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3800,27 +3815,55 @@
       <c r="A13" t="s">
         <v>609</v>
       </c>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="127" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E18" s="12"/>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>711</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="98" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="18" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
         <v>611</v>
       </c>
@@ -3847,10 +3890,11 @@
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" display="https://www.geeksforgeeks.org/java-tricks-competitive-programming-java-8/"/>
     <hyperlink ref="J5" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/"/>
+    <hyperlink ref="C23" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -3915,10 +3959,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="125" t="s">
         <v>263</v>
       </c>
       <c r="E4" s="5">
@@ -3935,10 +3979,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="124" t="s">
         <v>264</v>
       </c>
       <c r="E5" s="5">
@@ -3955,10 +3999,10 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="124" t="s">
         <v>265</v>
       </c>
       <c r="E6" s="5">
@@ -3975,7 +4019,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="124" t="s">
         <v>266</v>
       </c>
       <c r="D7" t="s">
@@ -3995,10 +4039,10 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="129" t="s">
+      <c r="B8" s="128" t="s">
         <v>597</v>
       </c>
-      <c r="C8" s="125" t="s">
+      <c r="C8" s="124" t="s">
         <v>267</v>
       </c>
       <c r="D8" t="s">
@@ -4018,7 +4062,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="124" t="s">
         <v>268</v>
       </c>
       <c r="D9" t="s">
@@ -4038,7 +4082,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="127" t="s">
+      <c r="C10" s="126" t="s">
         <v>269</v>
       </c>
       <c r="D10" t="s">
@@ -4058,7 +4102,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="129" t="s">
         <v>270</v>
       </c>
       <c r="D11" t="s">
@@ -4078,7 +4122,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="112" t="s">
         <v>271</v>
       </c>
       <c r="D12" t="s">
@@ -4098,7 +4142,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="134" t="s">
         <v>272</v>
       </c>
       <c r="D13" t="s">
@@ -4252,7 +4296,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="113" t="s">
+      <c r="C21" s="112" t="s">
         <v>280</v>
       </c>
       <c r="D21" t="s">
@@ -4269,7 +4313,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="112" t="s">
         <v>281</v>
       </c>
       <c r="D22" t="s">
@@ -4286,7 +4330,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="140" t="s">
+      <c r="C23" s="139" t="s">
         <v>282</v>
       </c>
       <c r="D23" t="s">
@@ -4299,9 +4343,9 @@
         <v>678</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="133" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="132"/>
-      <c r="C37" s="134" t="s">
+    <row r="37" spans="1:3" s="132" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="131"/>
+      <c r="C37" s="133" t="s">
         <v>507</v>
       </c>
     </row>
@@ -4343,8 +4387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,10 +4442,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>679</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="93" t="s">
         <v>283</v>
       </c>
       <c r="D4" t="s">
@@ -4412,10 +4456,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="93" t="s">
         <v>284</v>
       </c>
       <c r="D5" t="s">
@@ -4426,7 +4470,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="143" t="s">
+      <c r="C6" s="142" t="s">
         <v>285</v>
       </c>
       <c r="D6" t="s">
@@ -4440,7 +4484,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="142" t="s">
         <v>286</v>
       </c>
       <c r="D7" t="s">
@@ -4454,7 +4498,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="142" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -4465,7 +4509,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="143" t="s">
+      <c r="C9" s="142" t="s">
         <v>288</v>
       </c>
       <c r="D9" t="s">
@@ -4479,7 +4523,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="142" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
@@ -4493,7 +4537,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="143" t="s">
+      <c r="C11" s="142" t="s">
         <v>290</v>
       </c>
       <c r="D11" t="s">
@@ -4507,7 +4551,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="143" t="s">
+      <c r="C12" s="142" t="s">
         <v>291</v>
       </c>
       <c r="D12" t="s">
@@ -4521,10 +4565,10 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C13" s="94" t="s">
+      <c r="C13" s="93" t="s">
         <v>292</v>
       </c>
       <c r="D13" t="s">
@@ -4550,7 +4594,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4608,10 +4652,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="141" t="s">
         <v>293</v>
       </c>
       <c r="E4" t="s">
@@ -4625,7 +4669,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="141" t="s">
         <v>294</v>
       </c>
       <c r="E5" t="s">
@@ -4639,7 +4683,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="141" t="s">
         <v>295</v>
       </c>
       <c r="E6" t="s">
@@ -4653,7 +4697,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="141" t="s">
         <v>296</v>
       </c>
       <c r="E7" t="s">
@@ -4670,7 +4714,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="142" t="s">
+      <c r="C8" s="141" t="s">
         <v>297</v>
       </c>
       <c r="E8" t="s">
@@ -4687,10 +4731,10 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="129" t="s">
         <v>298</v>
       </c>
       <c r="E9" t="s">
@@ -4701,7 +4745,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="113" t="s">
+      <c r="C10" s="112" t="s">
         <v>299</v>
       </c>
       <c r="E10" t="s">
@@ -4715,7 +4759,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="112" t="s">
         <v>300</v>
       </c>
       <c r="E11" t="s">
@@ -4729,7 +4773,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="112" t="s">
         <v>301</v>
       </c>
       <c r="E12" t="s">
@@ -4743,7 +4787,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="134" t="s">
         <v>302</v>
       </c>
       <c r="E13" t="s">
@@ -4757,7 +4801,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="115" t="s">
+      <c r="C14" s="114" t="s">
         <v>303</v>
       </c>
       <c r="E14" t="s">
@@ -4771,7 +4815,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="115" t="s">
         <v>304</v>
       </c>
       <c r="E15" t="s">
@@ -4785,10 +4829,10 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="114" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4796,10 +4840,10 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="116" t="s">
         <v>306</v>
       </c>
     </row>
@@ -4823,226 +4867,233 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
-    <col min="4" max="4" width="51.140625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.85546875" customWidth="1"/>
-    <col min="9" max="9" width="44.7109375" customWidth="1"/>
-    <col min="10" max="10" width="47.28515625" customWidth="1"/>
-    <col min="11" max="11" width="46" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.85546875" customWidth="1"/>
+    <col min="8" max="8" width="44.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>0</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>488</v>
       </c>
+      <c r="G3" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="J3" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>597</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="C4" s="92" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="C5" s="129" t="s">
         <v>309</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
         <v>702</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="J5" s="16" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="112" t="s">
         <v>310</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>704</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="J6" s="16" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="C7" s="112" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="C8" s="112" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="C9" s="112" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="C10" s="112" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="C11" s="112" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="C12" s="112" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="C13" s="139" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="C14" s="114" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="81" t="s">
+      <c r="C15" s="115" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="C16" s="115" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="C17" s="115" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="81" t="s">
+      <c r="C18" s="115" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="81" t="s">
+      <c r="C19" s="115" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="81" t="s">
+      <c r="C20" s="115" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="81" t="s">
+      <c r="C21" s="116" t="s">
         <v>308</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J5" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HasPath.java"/>
+    <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5193,7 +5244,7 @@
       <c r="F9" s="25" t="s">
         <v>494</v>
       </c>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="87" t="s">
         <v>496</v>
       </c>
       <c r="H9" s="10"/>
@@ -5328,7 +5379,7 @@
       <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="141" t="s">
+      <c r="I1" s="140" t="s">
         <v>682</v>
       </c>
       <c r="J1" s="11" t="s">
@@ -6402,7 +6453,7 @@
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="114" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -6428,7 +6479,7 @@
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -6454,7 +6505,7 @@
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="116" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -6474,7 +6525,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="146" t="s">
+      <c r="C9" s="145" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -6497,7 +6548,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="131" t="s">
+      <c r="C10" s="130" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="23" t="s">
@@ -6517,7 +6568,7 @@
       <c r="B11" s="80" t="s">
         <v>647</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="130" t="s">
         <v>168</v>
       </c>
       <c r="D11" s="78" t="s">
@@ -6537,7 +6588,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="C12" s="131" t="s">
+      <c r="C12" s="130" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -6560,7 +6611,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="147" t="s">
+      <c r="C13" s="146" t="s">
         <v>144</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -6586,7 +6637,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="C14" s="136" t="s">
+      <c r="C14" s="135" t="s">
         <v>149</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -6615,7 +6666,7 @@
       <c r="B15" s="80" t="s">
         <v>478</v>
       </c>
-      <c r="C15" s="137" t="s">
+      <c r="C15" s="136" t="s">
         <v>151</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -6641,7 +6692,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="137" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -6661,10 +6712,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="139">
+      <c r="A17" s="138">
         <v>12</v>
       </c>
-      <c r="C17" s="146" t="s">
+      <c r="C17" s="145" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -6687,7 +6738,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="C18" s="118" t="s">
+      <c r="C18" s="117" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -6710,7 +6761,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="117" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -6733,7 +6784,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="C20" s="118" t="s">
+      <c r="C20" s="117" t="s">
         <v>162</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -6753,7 +6804,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="C21" s="118" t="s">
+      <c r="C21" s="117" t="s">
         <v>163</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -6773,7 +6824,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="C22" s="147" t="s">
+      <c r="C22" s="146" t="s">
         <v>166</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -6793,7 +6844,7 @@
       <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="81" t="s">
         <v>174</v>
       </c>
       <c r="G23" s="15" t="s">
@@ -6804,7 +6855,7 @@
       <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="C24" s="82" t="s">
+      <c r="C24" s="81" t="s">
         <v>175</v>
       </c>
     </row>
@@ -6888,7 +6939,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="119" t="s">
         <v>575</v>
       </c>
       <c r="C2" s="16"/>
@@ -7796,15 +7847,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="144" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8119,7 +8170,7 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="82" t="s">
         <v>178</v>
       </c>
       <c r="E4" t="s">
@@ -8133,7 +8184,7 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>179</v>
       </c>
       <c r="E5" t="s">
@@ -8147,7 +8198,7 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>180</v>
       </c>
       <c r="E6" t="s">
@@ -8161,7 +8212,7 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>181</v>
       </c>
       <c r="E7" t="s">
@@ -8175,7 +8226,7 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="82" t="s">
         <v>182</v>
       </c>
       <c r="E8" t="s">
@@ -8189,7 +8240,7 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="82" t="s">
         <v>183</v>
       </c>
       <c r="E9" t="s">
@@ -8203,7 +8254,7 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="83" t="s">
         <v>184</v>
       </c>
       <c r="E10" t="s">
@@ -8217,7 +8268,7 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="83" t="s">
         <v>185</v>
       </c>
       <c r="E11" t="s">
@@ -8231,7 +8282,7 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="D12" s="84" t="s">
+      <c r="D12" s="83" t="s">
         <v>186</v>
       </c>
       <c r="E12" t="s">
@@ -8245,7 +8296,7 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="83" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
@@ -8259,7 +8310,7 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="84" t="s">
+      <c r="D14" s="83" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
@@ -8273,7 +8324,7 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D15" s="83" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
@@ -8287,7 +8338,7 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="97" t="s">
         <v>190</v>
       </c>
       <c r="E16" t="s">
@@ -8301,7 +8352,7 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="98" t="s">
+      <c r="D17" s="97" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
@@ -8315,7 +8366,7 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="97" t="s">
         <v>192</v>
       </c>
       <c r="E18" t="s">
@@ -8329,7 +8380,7 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="97" t="s">
         <v>193</v>
       </c>
       <c r="E19" t="s">
@@ -8343,7 +8394,7 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="86" t="s">
+      <c r="D20" s="85" t="s">
         <v>194</v>
       </c>
       <c r="E20" t="s">
@@ -8357,7 +8408,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="86" t="s">
+      <c r="D21" s="85" t="s">
         <v>195</v>
       </c>
       <c r="E21" t="s">
@@ -8371,7 +8422,7 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="85" t="s">
         <v>196</v>
       </c>
       <c r="E22" t="s">
@@ -8385,7 +8436,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="85" t="s">
         <v>197</v>
       </c>
       <c r="E23" t="s">
@@ -8399,7 +8450,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="86" t="s">
         <v>198</v>
       </c>
       <c r="E24" t="s">
@@ -8413,7 +8464,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="87" t="s">
+      <c r="D25" s="86" t="s">
         <v>199</v>
       </c>
       <c r="E25" t="s">
@@ -8427,7 +8478,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>200</v>
       </c>
       <c r="E26" t="s">
@@ -8441,7 +8492,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>201</v>
       </c>
       <c r="E27" t="s">
@@ -8455,7 +8506,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="85" t="s">
+      <c r="D28" s="84" t="s">
         <v>202</v>
       </c>
       <c r="E28" t="s">
@@ -8469,7 +8520,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="84" t="s">
         <v>203</v>
       </c>
       <c r="E29" t="s">
@@ -8483,7 +8534,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="84" t="s">
         <v>204</v>
       </c>
       <c r="E30" t="s">
@@ -8497,7 +8548,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="85" t="s">
+      <c r="D31" s="84" t="s">
         <v>205</v>
       </c>
       <c r="E31" t="s">
@@ -8511,7 +8562,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="85" t="s">
+      <c r="D32" s="84" t="s">
         <v>206</v>
       </c>
       <c r="G32" s="29">
@@ -8522,7 +8573,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="85" t="s">
+      <c r="D33" s="84" t="s">
         <v>207</v>
       </c>
       <c r="G33" s="29">
@@ -8547,7 +8598,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8566,7 +8617,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="100" t="s">
         <v>544</v>
       </c>
       <c r="E1" s="5">
@@ -8576,32 +8627,32 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="102" t="s">
+      <c r="D2" s="101" t="s">
         <v>545</v>
       </c>
-      <c r="E2" s="102" t="s">
+      <c r="E2" s="101" t="s">
         <v>546</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="D3" s="101"/>
+      <c r="D3" s="100"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="D4" s="101"/>
+      <c r="D4" s="100"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="D5" s="101"/>
+      <c r="D5" s="100"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="D6" s="101"/>
+      <c r="D6" s="100"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8648,7 +8699,7 @@
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="95" t="s">
+      <c r="D9" s="94" t="s">
         <v>240</v>
       </c>
       <c r="E9" t="s">
@@ -8668,7 +8719,7 @@
       <c r="A10" s="29">
         <v>2</v>
       </c>
-      <c r="D10" s="96" t="s">
+      <c r="D10" s="95" t="s">
         <v>241</v>
       </c>
       <c r="E10" t="s">
@@ -8688,7 +8739,7 @@
       <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="95" t="s">
         <v>242</v>
       </c>
       <c r="E11" t="s">
@@ -8708,7 +8759,7 @@
       <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="95" t="s">
         <v>243</v>
       </c>
       <c r="E12" t="s">
@@ -8728,7 +8779,7 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>244</v>
       </c>
       <c r="E13" t="s">
@@ -8748,7 +8799,7 @@
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="95" t="s">
         <v>245</v>
       </c>
       <c r="E14" t="s">
@@ -8768,7 +8819,7 @@
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="D15" s="96" t="s">
+      <c r="D15" s="95" t="s">
         <v>246</v>
       </c>
       <c r="E15" t="s">
@@ -8788,7 +8839,7 @@
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="96" t="s">
+      <c r="D16" s="95" t="s">
         <v>247</v>
       </c>
       <c r="E16" t="s">
@@ -8808,7 +8859,7 @@
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="D17" s="96" t="s">
+      <c r="D17" s="95" t="s">
         <v>248</v>
       </c>
       <c r="E17" t="s">
@@ -8834,7 +8885,7 @@
       <c r="A18" s="29">
         <v>10</v>
       </c>
-      <c r="D18" s="97" t="s">
+      <c r="D18" s="96" t="s">
         <v>249</v>
       </c>
       <c r="E18" t="s">
@@ -8857,7 +8908,7 @@
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="98" t="s">
         <v>250</v>
       </c>
       <c r="E19" t="s">
@@ -8949,7 +9000,7 @@
       <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D23" s="99" t="s">
+      <c r="D23" s="98" t="s">
         <v>254</v>
       </c>
       <c r="E23" t="s">
@@ -9081,7 +9132,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="119" t="s">
+      <c r="D29" s="118" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -9101,7 +9152,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="106" t="s">
+      <c r="D30" s="105" t="s">
         <v>260</v>
       </c>
       <c r="E30" t="s">
@@ -9124,7 +9175,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="104" t="s">
         <v>261</v>
       </c>
       <c r="E31" t="s">
@@ -9153,7 +9204,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="105" t="s">
+      <c r="D32" s="104" t="s">
         <v>262</v>
       </c>
       <c r="E32" t="s">
@@ -9179,7 +9230,7 @@
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="107" t="s">
+      <c r="D33" s="106" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -9205,7 +9256,7 @@
       <c r="C34" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="99" t="s">
         <v>538</v>
       </c>
       <c r="E34" t="s">
@@ -9227,12 +9278,12 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:11" s="90" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A36" s="89"/>
-      <c r="D36" s="91" t="s">
+    <row r="36" spans="1:11" s="89" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="88"/>
+      <c r="D36" s="90" t="s">
         <v>507</v>
       </c>
-      <c r="G36" s="92"/>
+      <c r="G36" s="91"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
@@ -9419,7 +9470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -9438,7 +9489,7 @@
       <c r="C1" t="s">
         <v>706</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="103" t="s">
         <v>596</v>
       </c>
     </row>
@@ -9485,13 +9536,13 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="103" t="s">
         <v>566</v>
       </c>
-      <c r="C4" s="111" t="s">
+      <c r="C4" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="103"/>
+      <c r="F4" s="102"/>
       <c r="J4" s="16" t="s">
         <v>554</v>
       </c>
@@ -9500,13 +9551,13 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="103" t="s">
         <v>566</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="111" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="103"/>
+      <c r="F5" s="102"/>
       <c r="J5" s="16" t="s">
         <v>554</v>
       </c>
@@ -9515,16 +9566,16 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="113" t="s">
+      <c r="C6" s="112" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="103">
+      <c r="F6" s="102">
         <v>3</v>
       </c>
-      <c r="G6" s="108" t="s">
+      <c r="G6" s="107" t="s">
         <v>560</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -9541,13 +9592,13 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="112" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="103">
+      <c r="F7" s="102">
         <v>3</v>
       </c>
       <c r="G7" t="s">
@@ -9564,13 +9615,13 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="113" t="s">
+      <c r="C8" s="112" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="103">
+      <c r="F8" s="102">
         <v>3</v>
       </c>
       <c r="G8" t="s">
@@ -9587,13 +9638,13 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="112" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="103">
+      <c r="F9" s="102">
         <v>3</v>
       </c>
       <c r="G9" t="s">
@@ -9610,16 +9661,16 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="C10" s="96" t="s">
+      <c r="C10" s="95" t="s">
         <v>217</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="103">
+      <c r="F10" s="102">
         <v>3</v>
       </c>
-      <c r="G10" s="110" t="s">
+      <c r="G10" s="109" t="s">
         <v>496</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -9636,16 +9687,16 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="C11" s="112" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="103">
+      <c r="F11" s="102">
         <v>3</v>
       </c>
-      <c r="G11" s="109" t="s">
+      <c r="G11" s="108" t="s">
         <v>567</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -9665,13 +9716,13 @@
       <c r="B12" t="s">
         <v>541</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="112" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="103">
+      <c r="F12" s="102">
         <v>3</v>
       </c>
       <c r="G12" t="s">
@@ -9691,13 +9742,13 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="113" t="s">
+      <c r="C13" s="112" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="103">
+      <c r="F13" s="102">
         <v>3</v>
       </c>
       <c r="G13" t="s">
@@ -9714,13 +9765,13 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="103" t="s">
         <v>566</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="113" t="s">
         <v>221</v>
       </c>
-      <c r="F14" s="103">
+      <c r="F14" s="102">
         <v>3</v>
       </c>
       <c r="G14" s="18"/>
@@ -9732,13 +9783,13 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="114" t="s">
         <v>222</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="103">
+      <c r="F15" s="102">
         <v>3</v>
       </c>
       <c r="J15" s="16" t="s">
@@ -9749,13 +9800,13 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="115" t="s">
         <v>223</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="103">
+      <c r="F16" s="102">
         <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
@@ -9766,13 +9817,13 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="115" t="s">
         <v>224</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="103">
+      <c r="F17" s="102">
         <v>3</v>
       </c>
       <c r="J17" s="16" t="s">
@@ -9783,13 +9834,13 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="115" t="s">
         <v>225</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="103">
+      <c r="F18" s="102">
         <v>3</v>
       </c>
       <c r="J18" s="16" t="s">
@@ -9800,13 +9851,13 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="126" t="s">
+      <c r="C19" s="125" t="s">
         <v>578</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="103">
+      <c r="F19" s="102">
         <v>3</v>
       </c>
       <c r="G19" t="s">
@@ -9820,13 +9871,13 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="125" t="s">
+      <c r="C20" s="124" t="s">
         <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="103">
+      <c r="F20" s="102">
         <v>3</v>
       </c>
       <c r="G20" t="s">
@@ -9840,13 +9891,13 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="125" t="s">
+      <c r="C21" s="124" t="s">
         <v>227</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="103">
+      <c r="F21" s="102">
         <v>3</v>
       </c>
       <c r="G21" t="s">
@@ -9860,13 +9911,13 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="127" t="s">
+      <c r="C22" s="126" t="s">
         <v>228</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="103">
+      <c r="F22" s="102">
         <v>3</v>
       </c>
       <c r="G22" t="s">
@@ -9883,13 +9934,13 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="116" t="s">
+      <c r="C23" s="115" t="s">
         <v>229</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="103">
+      <c r="F23" s="102">
         <v>3</v>
       </c>
       <c r="G23" t="s">
@@ -9906,13 +9957,13 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="116" t="s">
+      <c r="C24" s="115" t="s">
         <v>230</v>
       </c>
       <c r="E24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="103">
+      <c r="F24" s="102">
         <v>3</v>
       </c>
       <c r="G24" t="s">
@@ -9926,13 +9977,13 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="117" t="s">
+      <c r="C25" s="116" t="s">
         <v>231</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="103">
+      <c r="F25" s="102">
         <v>3</v>
       </c>
       <c r="G25" t="s">
@@ -9946,13 +9997,13 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="118" t="s">
+      <c r="C26" s="117" t="s">
         <v>232</v>
       </c>
       <c r="E26" t="s">
         <v>639</v>
       </c>
-      <c r="F26" s="103">
+      <c r="F26" s="102">
         <v>3</v>
       </c>
       <c r="G26" t="s">
@@ -9969,13 +10020,13 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="118" t="s">
+      <c r="C27" s="117" t="s">
         <v>233</v>
       </c>
       <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="103">
+      <c r="F27" s="102">
         <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
@@ -9992,13 +10043,13 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="117" t="s">
         <v>234</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="103">
+      <c r="F28" s="102">
         <v>3</v>
       </c>
       <c r="G28" s="18" t="s">
@@ -10012,13 +10063,13 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="118" t="s">
+      <c r="C29" s="117" t="s">
         <v>235</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="103">
+      <c r="F29" s="102">
         <v>3</v>
       </c>
       <c r="G29" t="s">
@@ -10032,13 +10083,13 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="117" t="s">
         <v>236</v>
       </c>
       <c r="E30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="103">
+      <c r="F30" s="102">
         <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
@@ -10052,13 +10103,13 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="118" t="s">
+      <c r="C31" s="117" t="s">
         <v>237</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>637</v>
       </c>
-      <c r="F31" s="103">
+      <c r="F31" s="102">
         <v>3</v>
       </c>
       <c r="G31" s="18" t="s">
@@ -10075,13 +10126,13 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C32" s="117" t="s">
         <v>238</v>
       </c>
       <c r="E32" t="s">
         <v>638</v>
       </c>
-      <c r="F32" s="103">
+      <c r="F32" s="102">
         <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
@@ -10098,16 +10149,16 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="103" t="s">
         <v>566</v>
       </c>
-      <c r="C33" s="124" t="s">
+      <c r="C33" s="123" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="122" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="121"/>
-      <c r="C45" s="123" t="s">
+    <row r="45" spans="1:3" s="121" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="120"/>
+      <c r="C45" s="122" t="s">
         <v>577</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2021 - 14:13:34.96
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="714">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2523,12 +2523,15 @@
   <si>
     <t>linked lis.remove</t>
   </si>
+  <si>
+    <t>then you can have max n*(n-1)/2 edge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2659,6 +2662,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -2932,7 +2941,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3328,6 +3337,7 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3707,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4867,10 +4877,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5089,12 +5099,23 @@
         <v>308</v>
       </c>
     </row>
+    <row r="27" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="C27" s="147" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="C28" s="147" t="s">
+        <v>713</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HasPath.java"/>
     <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2021 - 23:38:37.90
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="716">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2525,6 +2525,12 @@
   </si>
   <si>
     <t>then you can have max n*(n-1)/2 edge</t>
+  </si>
+  <si>
+    <t>pq on student class, need to impleemtn comparable</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -3325,19 +3331,19 @@
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" xfId="16" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="10" builtinId="30"/>
@@ -3735,10 +3741,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="146" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="143"/>
+      <c r="G2" s="146"/>
       <c r="J2" s="103" t="s">
         <v>327</v>
       </c>
@@ -4601,10 +4607,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4846,7 +4852,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -4855,6 +4861,14 @@
       </c>
       <c r="C17" s="116" t="s">
         <v>306</v>
+      </c>
+      <c r="G17" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>715</v>
       </c>
     </row>
   </sheetData>
@@ -4879,7 +4893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27:C28"/>
     </sheetView>
   </sheetViews>
@@ -5100,12 +5114,12 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
-      <c r="C27" s="147" t="s">
+      <c r="C27" s="145" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
-      <c r="C28" s="147" t="s">
+      <c r="C28" s="145" t="s">
         <v>713</v>
       </c>
     </row>
@@ -6546,7 +6560,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="145" t="s">
+      <c r="C9" s="143" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -6632,7 +6646,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="146" t="s">
+      <c r="C13" s="144" t="s">
         <v>144</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -6736,7 +6750,7 @@
       <c r="A17" s="138">
         <v>12</v>
       </c>
-      <c r="C17" s="145" t="s">
+      <c r="C17" s="143" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -6845,7 +6859,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="C22" s="146" t="s">
+      <c r="C22" s="144" t="s">
         <v>166</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -7868,15 +7882,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="147" t="s">
         <v>348</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="144"/>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
-      <c r="F2" s="144"/>
-      <c r="G2" s="144"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   20-06-2021 - 21:18:27.13
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="734">
   <si>
     <t>TOPIC</t>
   </si>
@@ -1114,12 +1114,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Spread Of Infection </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shortest Path In Weights </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Minimum Wire Required To Connect All Pcs </t>
   </si>
   <si>
     <t xml:space="preserve"> Order Of Compilation </t>
@@ -2532,12 +2526,72 @@
   <si>
     <t>\</t>
   </si>
+  <si>
+    <t>graph3</t>
+  </si>
+  <si>
+    <t>graph4</t>
+  </si>
+  <si>
+    <t>graph5</t>
+  </si>
+  <si>
+    <t>graph1</t>
+  </si>
+  <si>
+    <t>graph2</t>
+  </si>
+  <si>
+    <t>rotten oranges , fire in city</t>
+  </si>
+  <si>
+    <t>bfs +pq</t>
+  </si>
+  <si>
+    <t>bpf+pq</t>
+  </si>
+  <si>
+    <t>prims algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Minimum Wire Required To Connect All Pcs (prims algo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shortest Path In Weights (dijkstra)</t>
+  </si>
+  <si>
+    <t>dijkstra,single src shortest path to all vertices</t>
+  </si>
+  <si>
+    <t>will not work for negative wgts,because it greedly finds the min</t>
+  </si>
+  <si>
+    <t>leet 207- course scheduling</t>
+  </si>
+  <si>
+    <t>399. Evaluate Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotten oranges </t>
+  </si>
+  <si>
+    <t>fire in city</t>
+  </si>
+  <si>
+    <t>directed cycle</t>
+  </si>
+  <si>
+    <t>solve color problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solve using dfs, hashmap generic graph </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2673,6 +2727,12 @@
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2947,7 +3007,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3338,6 +3398,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3741,12 +3805,12 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="146" t="s">
+      <c r="F2" s="148" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="146"/>
+      <c r="G2" s="148"/>
       <c r="J2" s="103" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K2" s="103"/>
     </row>
@@ -3764,15 +3828,15 @@
         <v>48</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -3780,7 +3844,7 @@
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>127</v>
@@ -3792,12 +3856,12 @@
         <v>97</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>124</v>
@@ -3816,23 +3880,23 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B13" s="127" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -3843,20 +3907,20 @@
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -3866,37 +3930,37 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C27" s="18" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N30" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N32" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -3935,7 +3999,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" s="25" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3956,7 +4020,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>38</v>
@@ -3976,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C4" s="125" t="s">
         <v>263</v>
@@ -3988,7 +4052,7 @@
         <v>100</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3996,7 +4060,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C5" s="124" t="s">
         <v>264</v>
@@ -4008,7 +4072,7 @@
         <v>100</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4016,7 +4080,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C6" s="124" t="s">
         <v>265</v>
@@ -4028,7 +4092,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,7 +4112,7 @@
         <v>100</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4056,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="128" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C8" s="124" t="s">
         <v>267</v>
@@ -4071,7 +4135,7 @@
         <v>100</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4091,7 +4155,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4111,7 +4175,7 @@
         <v>100</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4131,7 +4195,7 @@
         <v>100</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4151,7 +4215,7 @@
         <v>100</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4168,10 +4232,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4188,10 +4252,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4208,10 +4272,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4228,7 +4292,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4245,13 +4309,13 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -4268,7 +4332,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -4285,10 +4349,10 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4305,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4322,7 +4386,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4339,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4356,18 +4420,18 @@
         <v>0</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="132" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="131"/>
       <c r="C37" s="133" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C38" s="16" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>
@@ -4419,7 +4483,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" s="25" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,7 +4503,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>38</v>
@@ -4459,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C4" s="93" t="s">
         <v>283</v>
@@ -4473,7 +4537,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C5" s="93" t="s">
         <v>284</v>
@@ -4493,7 +4557,7 @@
         <v>34</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4507,7 +4571,7 @@
         <v>34</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4518,7 +4582,7 @@
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4532,7 +4596,7 @@
         <v>34</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4546,7 +4610,7 @@
         <v>34</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -4560,7 +4624,7 @@
         <v>34</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -4574,7 +4638,7 @@
         <v>34</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4582,7 +4646,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C13" s="93" t="s">
         <v>292</v>
@@ -4609,7 +4673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -4626,7 +4690,7 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" s="25" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4649,7 +4713,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>38</v>
@@ -4669,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C4" s="141" t="s">
         <v>293</v>
@@ -4678,7 +4742,7 @@
         <v>34</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4692,7 +4756,7 @@
         <v>34</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4706,7 +4770,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4720,10 +4784,10 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4737,10 +4801,10 @@
         <v>34</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -4748,7 +4812,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C9" s="129" t="s">
         <v>298</v>
@@ -4768,7 +4832,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4782,7 +4846,7 @@
         <v>34</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4796,7 +4860,7 @@
         <v>34</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4810,7 +4874,7 @@
         <v>34</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4824,7 +4888,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4838,7 +4902,7 @@
         <v>34</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -4846,7 +4910,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C16" s="114" t="s">
         <v>305</v>
@@ -4857,18 +4921,18 @@
         <v>14</v>
       </c>
       <c r="B17" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C17" s="116" t="s">
         <v>306</v>
       </c>
       <c r="G17" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -4891,10 +4955,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,7 +4997,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>38</v>
@@ -4953,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C4" s="92" t="s">
         <v>307</v>
@@ -4963,88 +5027,139 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>717</v>
+      </c>
       <c r="C5" s="129" t="s">
         <v>309</v>
       </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>717</v>
+      </c>
       <c r="C6" s="112" t="s">
         <v>310</v>
       </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
       <c r="G6" s="18" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="H6" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>718</v>
+      </c>
       <c r="C7" s="112" t="s">
         <v>311</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>718</v>
+      </c>
       <c r="C8" s="112" t="s">
         <v>312</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>718</v>
+      </c>
       <c r="C9" s="112" t="s">
         <v>313</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>718</v>
+      </c>
       <c r="C10" s="112" t="s">
         <v>314</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>8</v>
       </c>
+      <c r="B11" s="103" t="s">
+        <v>714</v>
+      </c>
       <c r="C11" s="112" t="s">
         <v>315</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
       </c>
+      <c r="B12" s="103" t="s">
+        <v>714</v>
+      </c>
       <c r="C12" s="112" t="s">
         <v>316</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>10</v>
       </c>
+      <c r="B13" s="103" t="s">
+        <v>714</v>
+      </c>
       <c r="C13" s="139" t="s">
         <v>317</v>
       </c>
@@ -5053,59 +5168,110 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
+      <c r="B14" s="103" t="s">
+        <v>714</v>
+      </c>
       <c r="C14" s="114" t="s">
         <v>318</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>12</v>
       </c>
+      <c r="B15" s="103" t="s">
+        <v>715</v>
+      </c>
       <c r="C15" s="115" t="s">
         <v>319</v>
+      </c>
+      <c r="G15" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>13</v>
       </c>
+      <c r="B16" s="103" t="s">
+        <v>715</v>
+      </c>
       <c r="C16" s="115" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
+      <c r="B17" s="103" t="s">
+        <v>715</v>
+      </c>
       <c r="C17" s="115" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>15</v>
       </c>
+      <c r="B18" s="146" t="s">
+        <v>716</v>
+      </c>
       <c r="C18" s="115" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+      <c r="G18" t="s">
+        <v>720</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>725</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
+      <c r="B19" s="146" t="s">
+        <v>716</v>
+      </c>
       <c r="C19" s="115" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>723</v>
+      </c>
+      <c r="G19" t="s">
+        <v>721</v>
+      </c>
+      <c r="H19" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
+      <c r="B20" s="146" t="s">
+        <v>716</v>
+      </c>
       <c r="C20" s="115" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+      <c r="G20" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -5113,14 +5279,34 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21.75" x14ac:dyDescent="0.3">
       <c r="C27" s="145" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="21.75" x14ac:dyDescent="0.3">
-      <c r="C28" s="145" t="s">
-        <v>713</v>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C28" s="147" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="25" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" customFormat="1" ht="21.75" x14ac:dyDescent="0.3">
+      <c r="C35" s="145" t="s">
+        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -5156,16 +5342,16 @@
         <v>51</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -5182,13 +5368,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="16" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5196,21 +5382,21 @@
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="16" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="10" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J6" s="10"/>
     </row>
@@ -5219,11 +5405,11 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -5232,7 +5418,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="10"/>
       <c r="I7" s="16" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -5241,24 +5427,24 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="79" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J8" s="10"/>
     </row>
@@ -5267,56 +5453,56 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="G9" s="87" t="s">
         <v>494</v>
-      </c>
-      <c r="G9" s="87" t="s">
-        <v>496</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="16" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D10" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="G10" t="s">
+        <v>494</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>495</v>
-      </c>
-      <c r="G10" t="s">
-        <v>496</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C11" t="s">
         <v>208</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="F11" t="s">
+        <v>527</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>528</v>
-      </c>
-      <c r="F11" t="s">
-        <v>529</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5389,7 +5575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -5415,10 +5601,10 @@
         <v>115</v>
       </c>
       <c r="I1" s="140" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5445,7 +5631,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>38</v>
@@ -5773,10 +5959,10 @@
         <v>100</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>98</v>
@@ -5805,7 +5991,7 @@
         <v>100</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -5831,7 +6017,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5857,10 +6043,10 @@
         <v>100</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5889,7 +6075,7 @@
         <v>108</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -5915,7 +6101,7 @@
         <v>100</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5941,7 +6127,7 @@
         <v>100</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5967,7 +6153,7 @@
         <v>100</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5993,7 +6179,7 @@
         <v>100</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -6025,7 +6211,7 @@
         <v>102</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -6057,7 +6243,7 @@
         <v>106</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6086,7 +6272,7 @@
         <v>111</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6115,7 +6301,7 @@
         <v>109</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -6147,7 +6333,7 @@
         <v>112</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -6176,7 +6362,7 @@
         <v>117</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6208,7 +6394,7 @@
         <v>118</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6240,7 +6426,7 @@
         <v>103</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -6272,7 +6458,7 @@
         <v>129</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="177" customHeight="1" x14ac:dyDescent="0.25">
@@ -6304,7 +6490,7 @@
         <v>128</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
@@ -6318,7 +6504,7 @@
         <v>137</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6350,7 +6536,7 @@
         <v>135</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6437,7 +6623,7 @@
         <v>116</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I1" s="17"/>
     </row>
@@ -6462,7 +6648,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F3" s="27" t="s">
         <v>38</v>
@@ -6479,7 +6665,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I4" s="16"/>
     </row>
@@ -6507,7 +6693,7 @@
         <v>105</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6533,7 +6719,7 @@
         <v>71</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6553,7 +6739,7 @@
         <v>67</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6576,7 +6762,7 @@
         <v>146</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -6601,7 +6787,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="80" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C11" s="130" t="s">
         <v>168</v>
@@ -6613,10 +6799,10 @@
         <v>2</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -6633,13 +6819,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>145</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6656,7 +6842,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>148</v>
@@ -6665,7 +6851,7 @@
         <v>147</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -6688,10 +6874,10 @@
         <v>169</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6699,7 +6885,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="80" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C15" s="136" t="s">
         <v>151</v>
@@ -6711,16 +6897,16 @@
         <v>2</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>152</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6743,7 +6929,7 @@
         <v>155</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6766,7 +6952,7 @@
         <v>165</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -6789,7 +6975,7 @@
         <v>158</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -6812,7 +6998,7 @@
         <v>171</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -6832,7 +7018,7 @@
         <v>164</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6852,7 +7038,7 @@
         <v>167</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6872,7 +7058,7 @@
         <v>173</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6883,7 +7069,7 @@
         <v>174</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6965,17 +7151,17 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2" s="119" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C2" s="16"/>
       <c r="G2" s="16"/>
@@ -6984,7 +7170,7 @@
     <row r="3" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
       <c r="B3" s="38" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -7008,7 +7194,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -7040,13 +7226,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>329</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -7066,13 +7252,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>334</v>
-      </c>
       <c r="I6" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -7080,7 +7266,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>33</v>
@@ -7092,13 +7278,13 @@
         <v>5</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -7118,13 +7304,13 @@
         <v>5</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7144,10 +7330,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7167,10 +7353,10 @@
         <v>5</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -7190,16 +7376,16 @@
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -7219,13 +7405,13 @@
         <v>3</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7245,13 +7431,13 @@
         <v>3</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7271,13 +7457,13 @@
         <v>3</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -7297,13 +7483,13 @@
         <v>3</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -7323,10 +7509,10 @@
         <v>3</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7346,10 +7532,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7369,10 +7555,10 @@
         <v>3</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -7392,7 +7578,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7412,16 +7598,16 @@
         <v>3</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7441,10 +7627,10 @@
         <v>3</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -7459,7 +7645,7 @@
     <row r="33" spans="1:9" s="37" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
       <c r="B33" s="38" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -7474,7 +7660,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>208</v>
@@ -7486,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I34" s="31"/>
     </row>
@@ -7495,7 +7681,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>208</v>
@@ -7507,10 +7693,10 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I35" s="31"/>
     </row>
@@ -7519,7 +7705,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>33</v>
@@ -7531,7 +7717,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I36" s="31"/>
     </row>
@@ -7540,10 +7726,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>34</v>
@@ -7552,10 +7738,10 @@
         <v>0</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H37" s="59"/>
       <c r="I37" s="31"/>
@@ -7565,10 +7751,10 @@
         <v>5</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>34</v>
@@ -7577,7 +7763,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H38" s="59"/>
       <c r="I38" s="31"/>
@@ -7587,10 +7773,10 @@
         <v>6</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>34</v>
@@ -7599,10 +7785,10 @@
         <v>0</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I39" s="31"/>
     </row>
@@ -7611,7 +7797,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>208</v>
@@ -7623,7 +7809,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I40" s="31"/>
     </row>
@@ -7632,10 +7818,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>34</v>
@@ -7644,10 +7830,10 @@
         <v>0</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I41" s="31"/>
     </row>
@@ -7656,10 +7842,10 @@
         <v>9</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>34</v>
@@ -7668,10 +7854,10 @@
         <v>0</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I42" s="31"/>
     </row>
@@ -7680,7 +7866,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>208</v>
@@ -7692,10 +7878,10 @@
         <v>0</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I43" s="31"/>
     </row>
@@ -7704,7 +7890,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>208</v>
@@ -7716,13 +7902,13 @@
         <v>0</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I44" s="31"/>
     </row>
@@ -7731,7 +7917,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>208</v>
@@ -7743,13 +7929,13 @@
         <v>0</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I45" s="21"/>
     </row>
@@ -7758,7 +7944,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>33</v>
@@ -7770,10 +7956,10 @@
         <v>0</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I46" s="16"/>
     </row>
@@ -7782,30 +7968,30 @@
         <v>14</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="16" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="16" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="16" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -7877,20 +8063,20 @@
         <v>116</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="147" t="s">
-        <v>348</v>
-      </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="A2" s="149" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7907,7 +8093,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>38</v>
@@ -7927,7 +8113,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>33</v>
@@ -7939,12 +8125,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
       <c r="I4" s="16" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -7961,7 +8147,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
       <c r="I5" s="16" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -7984,7 +8170,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8007,7 +8193,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="16" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -8030,7 +8216,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
       <c r="I8" s="16" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8053,7 +8239,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
       <c r="I9" s="16" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8074,11 +8260,11 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="77" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8086,36 +8272,36 @@
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="74" t="s">
+        <v>406</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>408</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -8186,7 +8372,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H3" s="27" t="s">
         <v>38</v>
@@ -8617,7 +8803,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -8653,7 +8839,7 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="D1" s="100" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E1" s="5">
         <v>0</v>
@@ -8663,10 +8849,10 @@
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="D2" s="101" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E2" s="101" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G2"/>
     </row>
@@ -8710,7 +8896,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>38</v>
@@ -8727,7 +8913,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8747,7 +8933,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8767,7 +8953,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -8787,7 +8973,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8807,7 +8993,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8827,7 +9013,7 @@
         <v>3</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8847,7 +9033,7 @@
         <v>3</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8867,7 +9053,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8887,7 +9073,7 @@
         <v>3</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -8907,13 +9093,13 @@
         <v>3</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8933,10 +9119,10 @@
         <v>3</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -8956,10 +9142,10 @@
         <v>3</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -8979,10 +9165,10 @@
         <v>3</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -9002,10 +9188,10 @@
         <v>3</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9025,10 +9211,10 @@
         <v>3</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -9048,16 +9234,16 @@
         <v>3</v>
       </c>
       <c r="H23" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="I23" t="s">
         <v>498</v>
       </c>
-      <c r="I23" t="s">
-        <v>500</v>
-      </c>
       <c r="J23" s="18" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -9077,7 +9263,7 @@
         <v>3</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -9097,10 +9283,10 @@
         <v>3</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -9120,7 +9306,7 @@
         <v>3</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -9140,7 +9326,7 @@
         <v>3</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -9160,7 +9346,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9180,7 +9366,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -9200,10 +9386,10 @@
         <v>3</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -9223,16 +9409,16 @@
         <v>3</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -9252,13 +9438,13 @@
         <v>3</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9278,10 +9464,10 @@
         <v>3</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9289,10 +9475,10 @@
         <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D34" s="99" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
@@ -9304,10 +9490,10 @@
         <v>3</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -9316,13 +9502,13 @@
     <row r="36" spans="1:11" s="89" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A36" s="88"/>
       <c r="D36" s="90" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G36" s="91"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
@@ -9333,12 +9519,12 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D39" s="16" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D40" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F40" t="s">
         <v>34</v>
@@ -9349,7 +9535,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D41" s="16" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F41" t="s">
         <v>34</v>
@@ -9360,7 +9546,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D42" s="16" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F42" t="s">
         <v>34</v>
@@ -9371,7 +9557,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D43" s="16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F43" t="s">
         <v>34</v>
@@ -9380,13 +9566,13 @@
         <v>0</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="K43" s="16"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D44" s="16" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F44" t="s">
         <v>34</v>
@@ -9397,7 +9583,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D45" s="16" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F45" t="s">
         <v>34</v>
@@ -9408,7 +9594,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D46" s="16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F46" t="s">
         <v>34</v>
@@ -9419,10 +9605,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G47" s="5">
         <v>0</v>
@@ -9430,7 +9616,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D48" s="16" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F48" t="s">
         <v>34</v>
@@ -9441,7 +9627,7 @@
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D49" s="16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F49" t="s">
         <v>34</v>
@@ -9522,17 +9708,17 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="C1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G1" s="103" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="C2"/>
       <c r="G2" s="18" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="22" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9552,7 +9738,7 @@
         <v>30</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G3" s="27" t="s">
         <v>38</v>
@@ -9572,14 +9758,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="103" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C4" s="110" t="s">
         <v>211</v>
       </c>
       <c r="F4" s="102"/>
       <c r="J4" s="16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9587,14 +9773,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="103" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C5" s="111" t="s">
         <v>212</v>
       </c>
       <c r="F5" s="102"/>
       <c r="J5" s="16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9611,16 +9797,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="107" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9637,13 +9823,13 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -9660,13 +9846,13 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9683,13 +9869,13 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9706,16 +9892,16 @@
         <v>3</v>
       </c>
       <c r="G10" s="109" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I10" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9732,16 +9918,16 @@
         <v>3</v>
       </c>
       <c r="G11" s="108" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -9749,7 +9935,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C12" s="112" t="s">
         <v>219</v>
@@ -9761,16 +9947,16 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
+        <v>566</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>570</v>
-      </c>
       <c r="I12" s="10" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -9787,13 +9973,13 @@
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9801,7 +9987,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="103" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C14" s="113" t="s">
         <v>221</v>
@@ -9811,7 +9997,7 @@
       </c>
       <c r="G14" s="18"/>
       <c r="J14" s="16" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -9828,7 +10014,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -9845,7 +10031,7 @@
         <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -9862,7 +10048,7 @@
         <v>3</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9879,7 +10065,7 @@
         <v>3</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -9887,7 +10073,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="125" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
@@ -9896,10 +10082,10 @@
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -9916,10 +10102,10 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -9936,10 +10122,10 @@
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9956,13 +10142,13 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
+        <v>599</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>601</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>603</v>
-      </c>
       <c r="J22" s="16" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -9979,13 +10165,13 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -10002,10 +10188,10 @@
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10022,10 +10208,10 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -10036,19 +10222,19 @@
         <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F26" s="102">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H26" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10065,13 +10251,13 @@
         <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -10088,10 +10274,10 @@
         <v>3</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -10108,10 +10294,10 @@
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -10128,10 +10314,10 @@
         <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -10142,19 +10328,19 @@
         <v>237</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F31" s="102">
         <v>3</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -10165,19 +10351,19 @@
         <v>238</v>
       </c>
       <c r="E32" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F32" s="102">
         <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10185,7 +10371,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="103" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C33" s="123" t="s">
         <v>239</v>
@@ -10194,27 +10380,27 @@
     <row r="45" spans="1:3" s="121" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A45" s="120"/>
       <c r="C45" s="122" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="16" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="16" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code on timestamp:   20-06-2021 - 21:27:53.65
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="736">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2585,6 +2585,12 @@
   </si>
   <si>
     <t xml:space="preserve">solve using dfs, hashmap generic graph </t>
+  </si>
+  <si>
+    <t>CP/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/GetConnectedComponent.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4957,8 +4963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,6 +5088,9 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
+      <c r="J7" s="16" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
@@ -5095,6 +5104,9 @@
       </c>
       <c r="D8" t="s">
         <v>34</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5313,9 +5325,11 @@
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HasPath.java"/>
     <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java"/>
+    <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java"/>
+    <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   20-06-2021 - 21:40:35.84
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="737">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2591,6 +2591,9 @@
   </si>
   <si>
     <t>CP/GetConnectedComponent.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IsGraphConnected.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4964,7 +4967,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5122,6 +5125,9 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
+      <c r="J9" s="16" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
@@ -5327,9 +5333,10 @@
     <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java"/>
     <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java"/>
     <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java"/>
+    <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   20-06-2021 - 21:50:20.11
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="738">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2594,6 +2594,9 @@
   </si>
   <si>
     <t>CP/IsGraphConnected.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/NumberOfIsland.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4967,7 +4970,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,6 +5145,9 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
+      <c r="J10" s="16" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
@@ -5334,9 +5340,10 @@
     <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java"/>
     <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java"/>
     <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java"/>
+    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/NumberOfIsland.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   20-06-2021 - 22:12:29.78
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="739">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2597,6 +2597,9 @@
   </si>
   <si>
     <t>CP/NumberOfIsland.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/PerfectFriends.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4969,8 +4972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5162,6 +5165,9 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
+      <c r="J11" s="16" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
@@ -5341,9 +5347,10 @@
     <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java"/>
     <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java"/>
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/NumberOfIsland.java"/>
+    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PerfectFriends.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  0:04:44.55
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="741">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2600,6 +2600,12 @@
   </si>
   <si>
     <t>CP/PerfectFriends.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/HamiltonianPathAndCycle.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/KnightsTour.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4972,8 +4978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5182,6 +5188,9 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
+      <c r="J12" s="16" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
@@ -5192,6 +5201,9 @@
       </c>
       <c r="C13" s="139" t="s">
         <v>317</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5348,9 +5360,11 @@
     <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java"/>
     <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/NumberOfIsland.java"/>
     <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PerfectFriends.java"/>
+    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HamiltonianPathAndCycle.java"/>
+    <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  0:24:19.60
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="742">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2606,6 +2606,9 @@
   </si>
   <si>
     <t>CP/KnightsTour.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/BFS.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4979,7 +4982,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5219,6 +5222,9 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
+      <c r="J14" s="16" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
@@ -5362,9 +5368,10 @@
     <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PerfectFriends.java"/>
     <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HamiltonianPathAndCycle.java"/>
     <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java"/>
+    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/BFS.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  0:46:48.45
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="743">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2609,6 +2609,9 @@
   </si>
   <si>
     <t>CP/BFS.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IsGraphCyclic.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4982,7 +4985,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5239,6 +5242,9 @@
       <c r="G15" t="s">
         <v>733</v>
       </c>
+      <c r="J15" s="16" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
@@ -5369,9 +5375,10 @@
     <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HamiltonianPathAndCycle.java"/>
     <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java"/>
     <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/BFS.java"/>
+    <hyperlink ref="J15" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphCyclic.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  1:22:41.71
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="745">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2612,6 +2612,12 @@
   </si>
   <si>
     <t>CP/IsGraphCyclic.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IsGraphBipartite.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/SpreadOfInfection.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4985,7 +4991,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5259,8 +5265,11 @@
       <c r="G16" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="16" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>14</v>
       </c>
@@ -5273,8 +5282,11 @@
       <c r="G17" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="16" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>15</v>
       </c>
@@ -5294,7 +5306,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>16</v>
       </c>
@@ -5311,7 +5323,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>17</v>
       </c>
@@ -5325,7 +5337,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>18</v>
       </c>
@@ -5333,27 +5345,27 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="21.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
       <c r="C27" s="145" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C28" s="147" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="25" t="s">
         <v>731</v>
       </c>
@@ -5376,9 +5388,11 @@
     <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java"/>
     <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/BFS.java"/>
     <hyperlink ref="J15" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphCyclic.java"/>
+    <hyperlink ref="J16" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphBipartite.java"/>
+    <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  1:55:59.55
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="746">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2618,6 +2618,9 @@
   </si>
   <si>
     <t>CP/SpreadOfInfection.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Dijkstra.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4991,7 +4994,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5305,6 +5308,9 @@
       <c r="I18" s="29" t="s">
         <v>726</v>
       </c>
+      <c r="J18" s="16" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
@@ -5390,9 +5396,10 @@
     <hyperlink ref="J15" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphCyclic.java"/>
     <hyperlink ref="J16" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphBipartite.java"/>
     <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java"/>
+    <hyperlink ref="J18" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Dijkstra.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   21-06-2021 -  2:55:34.36
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="747">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2621,6 +2621,9 @@
   </si>
   <si>
     <t>CP/Dijkstra.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/Prims.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4994,7 +4997,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,6 +5331,9 @@
       <c r="H19" t="s">
         <v>722</v>
       </c>
+      <c r="J19" s="16" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
@@ -5397,9 +5403,10 @@
     <hyperlink ref="J16" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphBipartite.java"/>
     <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java"/>
     <hyperlink ref="J18" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Dijkstra.java"/>
+    <hyperlink ref="J19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Prims.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   23-06-2021 -  2:27:48.35
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="748">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2624,6 +2624,9 @@
   </si>
   <si>
     <t>CP/Prims.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>graph6</t>
   </si>
 </sst>
 </file>
@@ -4996,8 +4999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5352,6 +5355,9 @@
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
         <v>18</v>
+      </c>
+      <c r="B21" s="146" t="s">
+        <v>747</v>
       </c>
       <c r="C21" s="116" t="s">
         <v>308</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   24-06-2021 - 23:00:16.14
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="751">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2628,12 +2628,205 @@
   <si>
     <t>graph6</t>
   </si>
+  <si>
+    <r>
+      <t>    ll x1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFD971F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> n) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> n) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> n;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    ll y1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> ((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFD971F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> m) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> m) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> m;</t>
+    </r>
+  </si>
+  <si>
+    <t>circular trver in maze</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2776,6 +2969,24 @@
       <color rgb="FF212121"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF92672"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFD971F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3049,7 +3260,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3449,6 +3660,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3829,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,7 +4189,20 @@
         <v>710</v>
       </c>
     </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="150" t="s">
+        <v>748</v>
+      </c>
+    </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="150" t="s">
+        <v>749</v>
+      </c>
       <c r="N30" t="s">
         <v>613</v>
       </c>
@@ -4999,8 +5226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5356,7 +5583,7 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="B21" s="146" t="s">
+      <c r="B21" s="103" t="s">
         <v>747</v>
       </c>
       <c r="C21" s="116" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   26-06-2021 -  0:14:45.92
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="756">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2820,6 +2820,21 @@
   </si>
   <si>
     <t>circular trver in maze</t>
+  </si>
+  <si>
+    <t>Detect cycle in a directed graph | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>use bfs and replace queue with stack</t>
+  </si>
+  <si>
+    <t>topological sort, dfs with stpush at post order</t>
+  </si>
+  <si>
+    <t>CP/OrderOfcompilation.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t>CP/IterativeDFS.java at main · spartan4cs/CP (github.com)</t>
   </si>
 </sst>
 </file>
@@ -4043,7 +4058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -5226,8 +5241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5578,6 +5593,12 @@
       <c r="G20" t="s">
         <v>727</v>
       </c>
+      <c r="H20" t="s">
+        <v>753</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29">
@@ -5588,6 +5609,17 @@
       </c>
       <c r="C21" s="116" t="s">
         <v>308</v>
+      </c>
+      <c r="G21" t="s">
+        <v>752</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="16" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -5637,9 +5669,12 @@
     <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java"/>
     <hyperlink ref="J18" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Dijkstra.java"/>
     <hyperlink ref="J19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Prims.java"/>
+    <hyperlink ref="C22" r:id="rId16" display="https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1"/>
+    <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/OrderOfcompilation.java"/>
+    <hyperlink ref="J21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IterativeDFS.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code on timestamp:   26-06-2021 -  1:50:40.45
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="757">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2835,6 +2835,9 @@
   </si>
   <si>
     <t>CP/IterativeDFS.java at main · spartan4cs/CP (github.com)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">printing in reverse preorder </t>
   </si>
 </sst>
 </file>
@@ -5242,7 +5245,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5612,6 +5615,9 @@
       </c>
       <c r="G21" t="s">
         <v>752</v>
+      </c>
+      <c r="H21" t="s">
+        <v>756</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>755</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   27-06-2021 -  0:54:09.29
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="757">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2569,16 +2569,7 @@
     <t>leet 207- course scheduling</t>
   </si>
   <si>
-    <t>399. Evaluate Division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rotten oranges </t>
-  </si>
-  <si>
     <t>fire in city</t>
-  </si>
-  <si>
-    <t>directed cycle</t>
   </si>
   <si>
     <t>solve color problem</t>
@@ -2839,12 +2830,21 @@
   <si>
     <t xml:space="preserve">printing in reverse preorder </t>
   </si>
+  <si>
+    <t>Rotting Oranges - LeetCode</t>
+  </si>
+  <si>
+    <t>Evaluate Division - LeetCode</t>
+  </si>
+  <si>
+    <t>Course Schedule - LeetCode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2980,12 +2980,6 @@
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF212121"/>
-      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
     <font>
@@ -3278,7 +3272,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3670,16 +3664,13 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4079,10 +4070,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="148" t="s">
+      <c r="F2" s="147" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="148"/>
+      <c r="G2" s="147"/>
       <c r="J2" s="103" t="s">
         <v>325</v>
       </c>
@@ -4209,17 +4200,17 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="150" t="s">
-        <v>748</v>
+      <c r="B29" s="149" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="150" t="s">
-        <v>749</v>
+      <c r="B30" s="149" t="s">
+        <v>746</v>
       </c>
       <c r="N30" t="s">
         <v>613</v>
@@ -5244,8 +5235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5370,7 +5361,7 @@
         <v>34</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5387,7 +5378,7 @@
         <v>34</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5404,7 +5395,7 @@
         <v>34</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5421,7 +5412,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5438,7 +5429,7 @@
         <v>34</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5455,7 +5446,7 @@
         <v>34</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5469,7 +5460,7 @@
         <v>317</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5486,7 +5477,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5500,10 +5491,10 @@
         <v>319</v>
       </c>
       <c r="G15" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5517,10 +5508,10 @@
         <v>320</v>
       </c>
       <c r="G16" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5537,7 +5528,7 @@
         <v>719</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5560,7 +5551,7 @@
         <v>726</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -5580,7 +5571,7 @@
         <v>722</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5597,10 +5588,10 @@
         <v>727</v>
       </c>
       <c r="H20" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5608,49 +5599,44 @@
         <v>18</v>
       </c>
       <c r="B21" s="103" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C21" s="116" t="s">
         <v>308</v>
       </c>
       <c r="G21" t="s">
+        <v>749</v>
+      </c>
+      <c r="H21" t="s">
+        <v>753</v>
+      </c>
+      <c r="J21" s="16" t="s">
         <v>752</v>
-      </c>
-      <c r="H21" t="s">
-        <v>756</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="16" t="s">
-        <v>751</v>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="16" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="16" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>729</v>
+      <c r="C25" s="16" t="s">
+        <v>756</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
       <c r="C27" s="145" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C28" s="147" t="s">
         <v>728</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="25" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="35" spans="3:3" customFormat="1" ht="21.75" x14ac:dyDescent="0.3">
@@ -5678,9 +5664,12 @@
     <hyperlink ref="C22" r:id="rId16" display="https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1"/>
     <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/OrderOfcompilation.java"/>
     <hyperlink ref="J21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IterativeDFS.java"/>
+    <hyperlink ref="C23" r:id="rId19" display="https://leetcode.com/problems/rotting-oranges/"/>
+    <hyperlink ref="C24" r:id="rId20" display="https://leetcode.com/problems/evaluate-division/"/>
+    <hyperlink ref="C25" r:id="rId21" display="https://leetcode.com/problems/course-schedule/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -8433,15 +8422,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="148" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated code on timestamp:   27-06-2021 - 19:23:30.48
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="761">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2838,6 +2838,18 @@
   </si>
   <si>
     <t>Course Schedule - LeetCode</t>
+  </si>
+  <si>
+    <t>dp1</t>
+  </si>
+  <si>
+    <t>dp2</t>
+  </si>
+  <si>
+    <t>dp3</t>
+  </si>
+  <si>
+    <t>dp4</t>
   </si>
 </sst>
 </file>
@@ -5235,8 +5247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8685,8 +8697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8745,6 +8757,9 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>757</v>
+      </c>
       <c r="D4" s="82" t="s">
         <v>178</v>
       </c>
@@ -8759,6 +8774,9 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>757</v>
+      </c>
       <c r="D5" s="82" t="s">
         <v>179</v>
       </c>
@@ -8773,6 +8791,9 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>757</v>
+      </c>
       <c r="D6" s="82" t="s">
         <v>180</v>
       </c>
@@ -8787,6 +8808,9 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>758</v>
+      </c>
       <c r="D7" s="82" t="s">
         <v>181</v>
       </c>
@@ -8801,6 +8825,9 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>758</v>
+      </c>
       <c r="D8" s="82" t="s">
         <v>182</v>
       </c>
@@ -8815,6 +8842,9 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>759</v>
+      </c>
       <c r="D9" s="82" t="s">
         <v>183</v>
       </c>
@@ -8829,6 +8859,9 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
+      <c r="B10" s="103" t="s">
+        <v>759</v>
+      </c>
       <c r="D10" s="83" t="s">
         <v>184</v>
       </c>
@@ -8843,6 +8876,9 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
+      <c r="B11" s="103" t="s">
+        <v>760</v>
+      </c>
       <c r="D11" s="83" t="s">
         <v>185</v>
       </c>
@@ -8856,6 +8892,9 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>9</v>
+      </c>
+      <c r="B12" s="103" t="s">
+        <v>760</v>
       </c>
       <c r="D12" s="83" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   03-07-2021 - 22:06:55.26
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -22,6 +22,7 @@
     <sheet name="Graph" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="769">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2850,6 +2851,30 @@
   </si>
   <si>
     <t>dp4</t>
+  </si>
+  <si>
+    <t>dp5</t>
+  </si>
+  <si>
+    <t>sun morning</t>
+  </si>
+  <si>
+    <t>sum eve</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>dp6</t>
+  </si>
+  <si>
+    <t>dp7</t>
+  </si>
+  <si>
+    <t>dp8</t>
+  </si>
+  <si>
+    <t>dp9</t>
   </si>
 </sst>
 </file>
@@ -3284,7 +3309,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3522,9 +3547,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="8" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
@@ -3676,14 +3698,27 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -4082,14 +4117,14 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="152" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="147"/>
-      <c r="J2" s="103" t="s">
+      <c r="G2" s="152"/>
+      <c r="J2" s="102" t="s">
         <v>325</v>
       </c>
-      <c r="K2" s="103"/>
+      <c r="K2" s="102"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -4172,7 +4207,7 @@
       <c r="A13" t="s">
         <v>607</v>
       </c>
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="126" t="s">
         <v>605</v>
       </c>
     </row>
@@ -4201,7 +4236,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="97" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4216,12 +4251,12 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="149" t="s">
+      <c r="B29" s="146" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="149" t="s">
+      <c r="B30" s="146" t="s">
         <v>746</v>
       </c>
       <c r="N30" t="s">
@@ -4329,10 +4364,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="124" t="s">
         <v>263</v>
       </c>
       <c r="E4" s="5">
@@ -4349,10 +4384,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="123" t="s">
         <v>264</v>
       </c>
       <c r="E5" s="5">
@@ -4369,10 +4404,10 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="123" t="s">
         <v>265</v>
       </c>
       <c r="E6" s="5">
@@ -4389,7 +4424,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="123" t="s">
         <v>266</v>
       </c>
       <c r="D7" t="s">
@@ -4409,10 +4444,10 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="127" t="s">
         <v>595</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="123" t="s">
         <v>267</v>
       </c>
       <c r="D8" t="s">
@@ -4432,7 +4467,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="124" t="s">
+      <c r="C9" s="123" t="s">
         <v>268</v>
       </c>
       <c r="D9" t="s">
@@ -4452,7 +4487,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="126" t="s">
+      <c r="C10" s="125" t="s">
         <v>269</v>
       </c>
       <c r="D10" t="s">
@@ -4472,7 +4507,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="129" t="s">
+      <c r="C11" s="128" t="s">
         <v>270</v>
       </c>
       <c r="D11" t="s">
@@ -4492,7 +4527,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="111" t="s">
         <v>271</v>
       </c>
       <c r="D12" t="s">
@@ -4512,7 +4547,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="133" t="s">
         <v>272</v>
       </c>
       <c r="D13" t="s">
@@ -4666,7 +4701,7 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="112" t="s">
+      <c r="C21" s="111" t="s">
         <v>280</v>
       </c>
       <c r="D21" t="s">
@@ -4683,7 +4718,7 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="112" t="s">
+      <c r="C22" s="111" t="s">
         <v>281</v>
       </c>
       <c r="D22" t="s">
@@ -4700,7 +4735,7 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="139" t="s">
+      <c r="C23" s="138" t="s">
         <v>282</v>
       </c>
       <c r="D23" t="s">
@@ -4713,9 +4748,9 @@
         <v>676</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="132" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="131"/>
-      <c r="C37" s="133" t="s">
+    <row r="37" spans="1:3" s="131" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="130"/>
+      <c r="C37" s="132" t="s">
         <v>505</v>
       </c>
     </row>
@@ -4812,10 +4847,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>677</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="92" t="s">
         <v>283</v>
       </c>
       <c r="D4" t="s">
@@ -4826,10 +4861,10 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="92" t="s">
         <v>284</v>
       </c>
       <c r="D5" t="s">
@@ -4840,7 +4875,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="141" t="s">
         <v>285</v>
       </c>
       <c r="D6" t="s">
@@ -4854,7 +4889,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="141" t="s">
         <v>286</v>
       </c>
       <c r="D7" t="s">
@@ -4868,7 +4903,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="142" t="s">
+      <c r="C8" s="141" t="s">
         <v>287</v>
       </c>
       <c r="I8" s="16" t="s">
@@ -4879,7 +4914,7 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="142" t="s">
+      <c r="C9" s="141" t="s">
         <v>288</v>
       </c>
       <c r="D9" t="s">
@@ -4893,7 +4928,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="142" t="s">
+      <c r="C10" s="141" t="s">
         <v>289</v>
       </c>
       <c r="D10" t="s">
@@ -4907,7 +4942,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="142" t="s">
+      <c r="C11" s="141" t="s">
         <v>290</v>
       </c>
       <c r="D11" t="s">
@@ -4921,7 +4956,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="142" t="s">
+      <c r="C12" s="141" t="s">
         <v>291</v>
       </c>
       <c r="D12" t="s">
@@ -4935,10 +4970,10 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="92" t="s">
         <v>292</v>
       </c>
       <c r="D13" t="s">
@@ -5022,10 +5057,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="140" t="s">
         <v>293</v>
       </c>
       <c r="E4" t="s">
@@ -5039,7 +5074,7 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="141" t="s">
+      <c r="C5" s="140" t="s">
         <v>294</v>
       </c>
       <c r="E5" t="s">
@@ -5053,7 +5088,7 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="141" t="s">
+      <c r="C6" s="140" t="s">
         <v>295</v>
       </c>
       <c r="E6" t="s">
@@ -5067,7 +5102,7 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="141" t="s">
+      <c r="C7" s="140" t="s">
         <v>296</v>
       </c>
       <c r="E7" t="s">
@@ -5084,7 +5119,7 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="141" t="s">
+      <c r="C8" s="140" t="s">
         <v>297</v>
       </c>
       <c r="E8" t="s">
@@ -5101,10 +5136,10 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C9" s="129" t="s">
+      <c r="C9" s="128" t="s">
         <v>298</v>
       </c>
       <c r="E9" t="s">
@@ -5115,7 +5150,7 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="111" t="s">
         <v>299</v>
       </c>
       <c r="E10" t="s">
@@ -5129,7 +5164,7 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="111" t="s">
         <v>300</v>
       </c>
       <c r="E11" t="s">
@@ -5143,7 +5178,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="111" t="s">
         <v>301</v>
       </c>
       <c r="E12" t="s">
@@ -5157,7 +5192,7 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="133" t="s">
         <v>302</v>
       </c>
       <c r="E13" t="s">
@@ -5171,7 +5206,7 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="113" t="s">
         <v>303</v>
       </c>
       <c r="E14" t="s">
@@ -5185,7 +5220,7 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="114" t="s">
         <v>304</v>
       </c>
       <c r="E15" t="s">
@@ -5199,10 +5234,10 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C16" s="114" t="s">
+      <c r="C16" s="113" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5210,10 +5245,10 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="115" t="s">
         <v>306</v>
       </c>
       <c r="G17" t="s">
@@ -5306,10 +5341,10 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>595</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="91" t="s">
         <v>307</v>
       </c>
     </row>
@@ -5320,7 +5355,7 @@
       <c r="B5" t="s">
         <v>717</v>
       </c>
-      <c r="C5" s="129" t="s">
+      <c r="C5" s="128" t="s">
         <v>309</v>
       </c>
       <c r="D5" t="s">
@@ -5343,7 +5378,7 @@
       <c r="B6" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="111" t="s">
         <v>310</v>
       </c>
       <c r="D6" t="s">
@@ -5366,7 +5401,7 @@
       <c r="B7" t="s">
         <v>718</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="111" t="s">
         <v>311</v>
       </c>
       <c r="D7" t="s">
@@ -5383,7 +5418,7 @@
       <c r="B8" t="s">
         <v>718</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="111" t="s">
         <v>312</v>
       </c>
       <c r="D8" t="s">
@@ -5400,7 +5435,7 @@
       <c r="B9" t="s">
         <v>718</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="111" t="s">
         <v>313</v>
       </c>
       <c r="D9" t="s">
@@ -5417,7 +5452,7 @@
       <c r="B10" t="s">
         <v>718</v>
       </c>
-      <c r="C10" s="112" t="s">
+      <c r="C10" s="111" t="s">
         <v>314</v>
       </c>
       <c r="D10" t="s">
@@ -5431,10 +5466,10 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="102" t="s">
         <v>714</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="111" t="s">
         <v>315</v>
       </c>
       <c r="D11" t="s">
@@ -5448,10 +5483,10 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="102" t="s">
         <v>714</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="111" t="s">
         <v>316</v>
       </c>
       <c r="D12" t="s">
@@ -5465,10 +5500,10 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="102" t="s">
         <v>714</v>
       </c>
-      <c r="C13" s="139" t="s">
+      <c r="C13" s="138" t="s">
         <v>317</v>
       </c>
       <c r="J13" s="16" t="s">
@@ -5479,10 +5514,10 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="102" t="s">
         <v>714</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="113" t="s">
         <v>318</v>
       </c>
       <c r="D14" t="s">
@@ -5496,10 +5531,10 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="102" t="s">
         <v>715</v>
       </c>
-      <c r="C15" s="115" t="s">
+      <c r="C15" s="114" t="s">
         <v>319</v>
       </c>
       <c r="G15" t="s">
@@ -5513,10 +5548,10 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="102" t="s">
         <v>715</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="114" t="s">
         <v>320</v>
       </c>
       <c r="G16" t="s">
@@ -5530,10 +5565,10 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="102" t="s">
         <v>715</v>
       </c>
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="114" t="s">
         <v>321</v>
       </c>
       <c r="G17" t="s">
@@ -5547,10 +5582,10 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="145" t="s">
         <v>716</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="114" t="s">
         <v>724</v>
       </c>
       <c r="G18" t="s">
@@ -5570,10 +5605,10 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="B19" s="146" t="s">
+      <c r="B19" s="145" t="s">
         <v>716</v>
       </c>
-      <c r="C19" s="115" t="s">
+      <c r="C19" s="114" t="s">
         <v>723</v>
       </c>
       <c r="G19" t="s">
@@ -5590,10 +5625,10 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="145" t="s">
         <v>716</v>
       </c>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="114" t="s">
         <v>322</v>
       </c>
       <c r="G20" t="s">
@@ -5610,10 +5645,10 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="102" t="s">
         <v>744</v>
       </c>
-      <c r="C21" s="116" t="s">
+      <c r="C21" s="115" t="s">
         <v>308</v>
       </c>
       <c r="G21" t="s">
@@ -5647,12 +5682,12 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
-      <c r="C27" s="145" t="s">
+      <c r="C27" s="144" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="35" spans="3:3" customFormat="1" ht="21.75" x14ac:dyDescent="0.3">
-      <c r="C35" s="145" t="s">
+      <c r="C35" s="144" t="s">
         <v>711</v>
       </c>
     </row>
@@ -5831,7 +5866,7 @@
       <c r="F9" s="25" t="s">
         <v>492</v>
       </c>
-      <c r="G9" s="87" t="s">
+      <c r="G9" s="86" t="s">
         <v>494</v>
       </c>
       <c r="H9" s="10"/>
@@ -5966,7 +6001,7 @@
       <c r="E1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="140" t="s">
+      <c r="I1" s="139" t="s">
         <v>680</v>
       </c>
       <c r="J1" s="11" t="s">
@@ -7040,7 +7075,7 @@
       <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="114" t="s">
+      <c r="C6" s="113" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -7066,7 +7101,7 @@
       <c r="A7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="114" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -7092,7 +7127,7 @@
       <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="115" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -7112,7 +7147,7 @@
       <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="143" t="s">
+      <c r="C9" s="142" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -7135,7 +7170,7 @@
       <c r="A10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="130" t="s">
+      <c r="C10" s="129" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="23" t="s">
@@ -7155,7 +7190,7 @@
       <c r="B11" s="80" t="s">
         <v>645</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="129" t="s">
         <v>168</v>
       </c>
       <c r="D11" s="78" t="s">
@@ -7175,7 +7210,7 @@
       <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="129" t="s">
         <v>140</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -7198,7 +7233,7 @@
       <c r="A13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="144" t="s">
+      <c r="C13" s="143" t="s">
         <v>144</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -7224,7 +7259,7 @@
       <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="C14" s="135" t="s">
+      <c r="C14" s="134" t="s">
         <v>149</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -7253,7 +7288,7 @@
       <c r="B15" s="80" t="s">
         <v>476</v>
       </c>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="135" t="s">
         <v>151</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -7279,7 +7314,7 @@
       <c r="A16" s="13">
         <v>11</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="C16" s="136" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -7299,10 +7334,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="138">
+      <c r="A17" s="137">
         <v>12</v>
       </c>
-      <c r="C17" s="143" t="s">
+      <c r="C17" s="142" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -7325,7 +7360,7 @@
       <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="C18" s="117" t="s">
+      <c r="C18" s="116" t="s">
         <v>157</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -7348,7 +7383,7 @@
       <c r="A19" s="13">
         <v>14</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="116" t="s">
         <v>159</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -7371,7 +7406,7 @@
       <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="C20" s="117" t="s">
+      <c r="C20" s="116" t="s">
         <v>162</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -7391,7 +7426,7 @@
       <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="C21" s="117" t="s">
+      <c r="C21" s="116" t="s">
         <v>163</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -7411,7 +7446,7 @@
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="C22" s="144" t="s">
+      <c r="C22" s="143" t="s">
         <v>166</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -7526,7 +7561,7 @@
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="118" t="s">
         <v>573</v>
       </c>
       <c r="C2" s="16"/>
@@ -8434,15 +8469,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="148" t="s">
+      <c r="A2" s="153" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8697,13 +8732,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="29"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="7" max="7" width="24.7109375" style="29" customWidth="1"/>
     <col min="8" max="8" width="51.85546875" customWidth="1"/>
@@ -8735,7 +8771,7 @@
         <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>30</v>
+        <v>764</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>486</v>
@@ -8766,6 +8802,9 @@
       <c r="E4" t="s">
         <v>33</v>
       </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="29">
         <v>0</v>
       </c>
@@ -8783,6 +8822,9 @@
       <c r="E5" t="s">
         <v>33</v>
       </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" s="29">
         <v>0</v>
       </c>
@@ -8800,6 +8842,9 @@
       <c r="E6" t="s">
         <v>33</v>
       </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
       <c r="G6" s="29">
         <v>0</v>
       </c>
@@ -8817,6 +8862,9 @@
       <c r="E7" t="s">
         <v>33</v>
       </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
       <c r="G7" s="29">
         <v>0</v>
       </c>
@@ -8834,11 +8882,14 @@
       <c r="E8" t="s">
         <v>33</v>
       </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
       <c r="G8" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>6</v>
       </c>
@@ -8850,6 +8901,9 @@
       </c>
       <c r="E9" t="s">
         <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
       </c>
       <c r="G9" s="29">
         <v>0</v>
@@ -8859,10 +8913,10 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="102" t="s">
         <v>759</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="150" t="s">
         <v>184</v>
       </c>
       <c r="E10" t="s">
@@ -8876,10 +8930,13 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="102" t="s">
         <v>760</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="C11" t="s">
+        <v>762</v>
+      </c>
+      <c r="D11" s="151" t="s">
         <v>185</v>
       </c>
       <c r="E11" t="s">
@@ -8893,10 +8950,13 @@
       <c r="A12" s="29">
         <v>9</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="102" t="s">
         <v>760</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="C12" t="s">
+        <v>762</v>
+      </c>
+      <c r="D12" s="151" t="s">
         <v>186</v>
       </c>
       <c r="E12" t="s">
@@ -8910,11 +8970,20 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="B13" s="149" t="s">
+        <v>761</v>
+      </c>
+      <c r="C13" t="s">
+        <v>763</v>
+      </c>
+      <c r="D13" s="147" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
       </c>
       <c r="G13" s="29">
         <v>0</v>
@@ -8924,25 +8993,43 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="B14" s="149" t="s">
+        <v>761</v>
+      </c>
+      <c r="C14" t="s">
+        <v>763</v>
+      </c>
+      <c r="D14" s="147" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
       </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="29">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="B15" s="149" t="s">
+        <v>761</v>
+      </c>
+      <c r="C15" t="s">
+        <v>763</v>
+      </c>
+      <c r="D15" s="148" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
+      </c>
+      <c r="F15" t="s">
+        <v>34</v>
       </c>
       <c r="G15" s="29">
         <v>0</v>
@@ -8952,7 +9039,10 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="B16" s="102" t="s">
+        <v>765</v>
+      </c>
+      <c r="D16" s="96" t="s">
         <v>190</v>
       </c>
       <c r="E16" t="s">
@@ -8966,7 +9056,10 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="B17" s="102" t="s">
+        <v>765</v>
+      </c>
+      <c r="D17" s="96" t="s">
         <v>191</v>
       </c>
       <c r="E17" t="s">
@@ -8980,7 +9073,10 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="D18" s="97" t="s">
+      <c r="B18" s="102" t="s">
+        <v>765</v>
+      </c>
+      <c r="D18" s="96" t="s">
         <v>192</v>
       </c>
       <c r="E18" t="s">
@@ -8994,7 +9090,10 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="D19" s="97" t="s">
+      <c r="B19" s="102" t="s">
+        <v>766</v>
+      </c>
+      <c r="D19" s="96" t="s">
         <v>193</v>
       </c>
       <c r="E19" t="s">
@@ -9008,7 +9107,10 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="D20" s="85" t="s">
+      <c r="B20" s="102" t="s">
+        <v>766</v>
+      </c>
+      <c r="D20" s="84" t="s">
         <v>194</v>
       </c>
       <c r="E20" t="s">
@@ -9022,7 +9124,10 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="D21" s="85" t="s">
+      <c r="B21" s="102" t="s">
+        <v>766</v>
+      </c>
+      <c r="D21" s="84" t="s">
         <v>195</v>
       </c>
       <c r="E21" t="s">
@@ -9036,7 +9141,10 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="D22" s="85" t="s">
+      <c r="B22" s="102" t="s">
+        <v>766</v>
+      </c>
+      <c r="D22" s="84" t="s">
         <v>196</v>
       </c>
       <c r="E22" t="s">
@@ -9050,7 +9158,10 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="D23" s="85" t="s">
+      <c r="B23" s="149" t="s">
+        <v>767</v>
+      </c>
+      <c r="D23" s="84" t="s">
         <v>197</v>
       </c>
       <c r="E23" t="s">
@@ -9064,7 +9175,10 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="B24" s="149" t="s">
+        <v>767</v>
+      </c>
+      <c r="D24" s="85" t="s">
         <v>198</v>
       </c>
       <c r="E24" t="s">
@@ -9078,7 +9192,10 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="D25" s="86" t="s">
+      <c r="B25" s="149" t="s">
+        <v>767</v>
+      </c>
+      <c r="D25" s="85" t="s">
         <v>199</v>
       </c>
       <c r="E25" t="s">
@@ -9092,7 +9209,10 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="B26" s="149" t="s">
+        <v>768</v>
+      </c>
+      <c r="D26" s="85" t="s">
         <v>200</v>
       </c>
       <c r="E26" t="s">
@@ -9106,7 +9226,10 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="B27" s="149" t="s">
+        <v>768</v>
+      </c>
+      <c r="D27" s="85" t="s">
         <v>201</v>
       </c>
       <c r="E27" t="s">
@@ -9120,7 +9243,10 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="D28" s="84" t="s">
+      <c r="B28" s="149" t="s">
+        <v>768</v>
+      </c>
+      <c r="D28" s="83" t="s">
         <v>202</v>
       </c>
       <c r="E28" t="s">
@@ -9134,7 +9260,10 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="D29" s="84" t="s">
+      <c r="B29" s="149" t="s">
+        <v>768</v>
+      </c>
+      <c r="D29" s="83" t="s">
         <v>203</v>
       </c>
       <c r="E29" t="s">
@@ -9148,7 +9277,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="D30" s="84" t="s">
+      <c r="D30" s="83" t="s">
         <v>204</v>
       </c>
       <c r="E30" t="s">
@@ -9162,7 +9291,7 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="D31" s="84" t="s">
+      <c r="D31" s="83" t="s">
         <v>205</v>
       </c>
       <c r="E31" t="s">
@@ -9176,7 +9305,7 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" s="83" t="s">
         <v>206</v>
       </c>
       <c r="G32" s="29">
@@ -9187,7 +9316,7 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="D33" s="84" t="s">
+      <c r="D33" s="83" t="s">
         <v>207</v>
       </c>
       <c r="G33" s="29">
@@ -9231,7 +9360,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="99" t="s">
         <v>542</v>
       </c>
       <c r="E1" s="5">
@@ -9241,32 +9370,32 @@
     </row>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="100" t="s">
         <v>543</v>
       </c>
-      <c r="E2" s="101" t="s">
+      <c r="E2" s="100" t="s">
         <v>544</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="D3" s="100"/>
+      <c r="D3" s="99"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4"/>
-      <c r="D4" s="100"/>
+      <c r="D4" s="99"/>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5"/>
-      <c r="D5" s="100"/>
+      <c r="D5" s="99"/>
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="D6" s="100"/>
+      <c r="D6" s="99"/>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" s="22" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9313,7 +9442,7 @@
       <c r="A9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="93" t="s">
         <v>240</v>
       </c>
       <c r="E9" t="s">
@@ -9333,7 +9462,7 @@
       <c r="A10" s="29">
         <v>2</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="D10" s="94" t="s">
         <v>241</v>
       </c>
       <c r="E10" t="s">
@@ -9353,7 +9482,7 @@
       <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="D11" s="95" t="s">
+      <c r="D11" s="94" t="s">
         <v>242</v>
       </c>
       <c r="E11" t="s">
@@ -9373,7 +9502,7 @@
       <c r="A12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="94" t="s">
         <v>243</v>
       </c>
       <c r="E12" t="s">
@@ -9393,7 +9522,7 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="94" t="s">
         <v>244</v>
       </c>
       <c r="E13" t="s">
@@ -9413,7 +9542,7 @@
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="94" t="s">
         <v>245</v>
       </c>
       <c r="E14" t="s">
@@ -9433,7 +9562,7 @@
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="94" t="s">
         <v>246</v>
       </c>
       <c r="E15" t="s">
@@ -9453,7 +9582,7 @@
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="D16" s="95" t="s">
+      <c r="D16" s="94" t="s">
         <v>247</v>
       </c>
       <c r="E16" t="s">
@@ -9473,7 +9602,7 @@
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="D17" s="95" t="s">
+      <c r="D17" s="94" t="s">
         <v>248</v>
       </c>
       <c r="E17" t="s">
@@ -9499,7 +9628,7 @@
       <c r="A18" s="29">
         <v>10</v>
       </c>
-      <c r="D18" s="96" t="s">
+      <c r="D18" s="95" t="s">
         <v>249</v>
       </c>
       <c r="E18" t="s">
@@ -9522,7 +9651,7 @@
       <c r="A19" s="29">
         <v>11</v>
       </c>
-      <c r="D19" s="98" t="s">
+      <c r="D19" s="97" t="s">
         <v>250</v>
       </c>
       <c r="E19" t="s">
@@ -9614,7 +9743,7 @@
       <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D23" s="98" t="s">
+      <c r="D23" s="97" t="s">
         <v>254</v>
       </c>
       <c r="E23" t="s">
@@ -9746,7 +9875,7 @@
       <c r="A29" s="29">
         <v>21</v>
       </c>
-      <c r="D29" s="118" t="s">
+      <c r="D29" s="117" t="s">
         <v>259</v>
       </c>
       <c r="E29" t="s">
@@ -9766,7 +9895,7 @@
       <c r="A30" s="29">
         <v>22</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="104" t="s">
         <v>260</v>
       </c>
       <c r="E30" t="s">
@@ -9789,7 +9918,7 @@
       <c r="A31" s="29">
         <v>23</v>
       </c>
-      <c r="D31" s="104" t="s">
+      <c r="D31" s="103" t="s">
         <v>261</v>
       </c>
       <c r="E31" t="s">
@@ -9818,7 +9947,7 @@
       <c r="A32" s="29">
         <v>24</v>
       </c>
-      <c r="D32" s="104" t="s">
+      <c r="D32" s="103" t="s">
         <v>262</v>
       </c>
       <c r="E32" t="s">
@@ -9844,7 +9973,7 @@
       <c r="A33" s="29">
         <v>25</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D33" s="105" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="s">
@@ -9870,7 +9999,7 @@
       <c r="C34" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="98" t="s">
         <v>536</v>
       </c>
       <c r="E34" t="s">
@@ -9892,12 +10021,12 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:11" s="89" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A36" s="88"/>
-      <c r="D36" s="90" t="s">
+    <row r="36" spans="1:11" s="88" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="87"/>
+      <c r="D36" s="89" t="s">
         <v>505</v>
       </c>
-      <c r="G36" s="91"/>
+      <c r="G36" s="90"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D38" s="16" t="s">
@@ -10103,7 +10232,7 @@
       <c r="C1" t="s">
         <v>704</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="102" t="s">
         <v>594</v>
       </c>
     </row>
@@ -10150,13 +10279,13 @@
       <c r="A4" s="29">
         <v>1</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>564</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="F4" s="102"/>
+      <c r="F4" s="101"/>
       <c r="J4" s="16" t="s">
         <v>552</v>
       </c>
@@ -10165,13 +10294,13 @@
       <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
         <v>564</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="110" t="s">
         <v>212</v>
       </c>
-      <c r="F5" s="102"/>
+      <c r="F5" s="101"/>
       <c r="J5" s="16" t="s">
         <v>552</v>
       </c>
@@ -10180,16 +10309,16 @@
       <c r="A6" s="29">
         <v>3</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="111" t="s">
         <v>213</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="102">
+      <c r="F6" s="101">
         <v>3</v>
       </c>
-      <c r="G6" s="107" t="s">
+      <c r="G6" s="106" t="s">
         <v>558</v>
       </c>
       <c r="H6" s="10" t="s">
@@ -10206,13 +10335,13 @@
       <c r="A7" s="29">
         <v>4</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="111" t="s">
         <v>214</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="102">
+      <c r="F7" s="101">
         <v>3</v>
       </c>
       <c r="G7" t="s">
@@ -10229,13 +10358,13 @@
       <c r="A8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="111" t="s">
         <v>215</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="102">
+      <c r="F8" s="101">
         <v>3</v>
       </c>
       <c r="G8" t="s">
@@ -10252,13 +10381,13 @@
       <c r="A9" s="29">
         <v>6</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="111" t="s">
         <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="102">
+      <c r="F9" s="101">
         <v>3</v>
       </c>
       <c r="G9" t="s">
@@ -10275,16 +10404,16 @@
       <c r="A10" s="29">
         <v>7</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="94" t="s">
         <v>217</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="102">
+      <c r="F10" s="101">
         <v>3</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="108" t="s">
         <v>494</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -10301,16 +10430,16 @@
       <c r="A11" s="29">
         <v>8</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="111" t="s">
         <v>218</v>
       </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="102">
+      <c r="F11" s="101">
         <v>3</v>
       </c>
-      <c r="G11" s="108" t="s">
+      <c r="G11" s="107" t="s">
         <v>565</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -10330,13 +10459,13 @@
       <c r="B12" t="s">
         <v>539</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="111" t="s">
         <v>219</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="101">
         <v>3</v>
       </c>
       <c r="G12" t="s">
@@ -10356,13 +10485,13 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="112" t="s">
+      <c r="C13" s="111" t="s">
         <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="102">
+      <c r="F13" s="101">
         <v>3</v>
       </c>
       <c r="G13" t="s">
@@ -10379,13 +10508,13 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="102" t="s">
         <v>564</v>
       </c>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="112" t="s">
         <v>221</v>
       </c>
-      <c r="F14" s="102">
+      <c r="F14" s="101">
         <v>3</v>
       </c>
       <c r="G14" s="18"/>
@@ -10397,13 +10526,13 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="C15" s="114" t="s">
+      <c r="C15" s="113" t="s">
         <v>222</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="102">
+      <c r="F15" s="101">
         <v>3</v>
       </c>
       <c r="J15" s="16" t="s">
@@ -10414,13 +10543,13 @@
       <c r="A16" s="29">
         <v>13</v>
       </c>
-      <c r="C16" s="115" t="s">
+      <c r="C16" s="114" t="s">
         <v>223</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="102">
+      <c r="F16" s="101">
         <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
@@ -10431,13 +10560,13 @@
       <c r="A17" s="29">
         <v>14</v>
       </c>
-      <c r="C17" s="115" t="s">
+      <c r="C17" s="114" t="s">
         <v>224</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="102">
+      <c r="F17" s="101">
         <v>3</v>
       </c>
       <c r="J17" s="16" t="s">
@@ -10448,13 +10577,13 @@
       <c r="A18" s="29">
         <v>15</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="114" t="s">
         <v>225</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="102">
+      <c r="F18" s="101">
         <v>3</v>
       </c>
       <c r="J18" s="16" t="s">
@@ -10465,13 +10594,13 @@
       <c r="A19" s="29">
         <v>16</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="124" t="s">
         <v>576</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="102">
+      <c r="F19" s="101">
         <v>3</v>
       </c>
       <c r="G19" t="s">
@@ -10485,13 +10614,13 @@
       <c r="A20" s="29">
         <v>17</v>
       </c>
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="123" t="s">
         <v>226</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="102">
+      <c r="F20" s="101">
         <v>3</v>
       </c>
       <c r="G20" t="s">
@@ -10505,13 +10634,13 @@
       <c r="A21" s="29">
         <v>18</v>
       </c>
-      <c r="C21" s="124" t="s">
+      <c r="C21" s="123" t="s">
         <v>227</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="102">
+      <c r="F21" s="101">
         <v>3</v>
       </c>
       <c r="G21" t="s">
@@ -10525,13 +10654,13 @@
       <c r="A22" s="29">
         <v>19</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="125" t="s">
         <v>228</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="102">
+      <c r="F22" s="101">
         <v>3</v>
       </c>
       <c r="G22" t="s">
@@ -10548,13 +10677,13 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="C23" s="115" t="s">
+      <c r="C23" s="114" t="s">
         <v>229</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="102">
+      <c r="F23" s="101">
         <v>3</v>
       </c>
       <c r="G23" t="s">
@@ -10571,13 +10700,13 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="C24" s="115" t="s">
+      <c r="C24" s="114" t="s">
         <v>230</v>
       </c>
       <c r="E24" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="102">
+      <c r="F24" s="101">
         <v>3</v>
       </c>
       <c r="G24" t="s">
@@ -10591,13 +10720,13 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="C25" s="116" t="s">
+      <c r="C25" s="115" t="s">
         <v>231</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="102">
+      <c r="F25" s="101">
         <v>3</v>
       </c>
       <c r="G25" t="s">
@@ -10611,13 +10740,13 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="C26" s="117" t="s">
+      <c r="C26" s="116" t="s">
         <v>232</v>
       </c>
       <c r="E26" t="s">
         <v>637</v>
       </c>
-      <c r="F26" s="102">
+      <c r="F26" s="101">
         <v>3</v>
       </c>
       <c r="G26" t="s">
@@ -10634,13 +10763,13 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="C27" s="117" t="s">
+      <c r="C27" s="116" t="s">
         <v>233</v>
       </c>
       <c r="E27" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="102">
+      <c r="F27" s="101">
         <v>3</v>
       </c>
       <c r="G27" s="18" t="s">
@@ -10657,13 +10786,13 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="116" t="s">
         <v>234</v>
       </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="102">
+      <c r="F28" s="101">
         <v>3</v>
       </c>
       <c r="G28" s="18" t="s">
@@ -10677,13 +10806,13 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="C29" s="117" t="s">
+      <c r="C29" s="116" t="s">
         <v>235</v>
       </c>
       <c r="E29" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="102">
+      <c r="F29" s="101">
         <v>3</v>
       </c>
       <c r="G29" t="s">
@@ -10697,13 +10826,13 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="C30" s="117" t="s">
+      <c r="C30" s="116" t="s">
         <v>236</v>
       </c>
       <c r="E30" t="s">
         <v>34</v>
       </c>
-      <c r="F30" s="102">
+      <c r="F30" s="101">
         <v>3</v>
       </c>
       <c r="G30" s="18" t="s">
@@ -10717,13 +10846,13 @@
       <c r="A31" s="29">
         <v>28</v>
       </c>
-      <c r="C31" s="117" t="s">
+      <c r="C31" s="116" t="s">
         <v>237</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>635</v>
       </c>
-      <c r="F31" s="102">
+      <c r="F31" s="101">
         <v>3</v>
       </c>
       <c r="G31" s="18" t="s">
@@ -10740,13 +10869,13 @@
       <c r="A32" s="29">
         <v>29</v>
       </c>
-      <c r="C32" s="117" t="s">
+      <c r="C32" s="116" t="s">
         <v>238</v>
       </c>
       <c r="E32" t="s">
         <v>636</v>
       </c>
-      <c r="F32" s="102">
+      <c r="F32" s="101">
         <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
@@ -10763,16 +10892,16 @@
       <c r="A33" s="29">
         <v>30</v>
       </c>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="102" t="s">
         <v>564</v>
       </c>
-      <c r="C33" s="123" t="s">
+      <c r="C33" s="122" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="121" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="120"/>
-      <c r="C45" s="122" t="s">
+    <row r="45" spans="1:3" s="120" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="119"/>
+      <c r="C45" s="121" t="s">
         <v>575</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code on timestamp:   04-07-2021 - 14:00:30.29
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="769">
   <si>
     <t>TOPIC</t>
   </si>
@@ -8733,7 +8733,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9276,6 +9276,9 @@
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>27</v>
+      </c>
+      <c r="B30" s="149" t="s">
+        <v>768</v>
       </c>
       <c r="D30" s="83" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
Updated code on timestamp:   08-07-2021 -  1:56:35.01
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -8732,8 +8732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9110,7 +9110,7 @@
       <c r="B20" s="102" t="s">
         <v>766</v>
       </c>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="96" t="s">
         <v>194</v>
       </c>
       <c r="E20" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   08-07-2021 -  2:42:05.12
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -3309,7 +3309,7 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3701,24 +3701,21 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -4117,10 +4114,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="152" t="s">
+      <c r="F2" s="148" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="152"/>
+      <c r="G2" s="148"/>
       <c r="J2" s="102" t="s">
         <v>325</v>
       </c>
@@ -8469,15 +8466,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="149" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
+      <c r="B2" s="149"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8733,7 +8730,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D10" sqref="D10:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8970,13 +8967,13 @@
       <c r="A13" s="29">
         <v>10</v>
       </c>
-      <c r="B13" s="149" t="s">
+      <c r="B13" s="147" t="s">
         <v>761</v>
       </c>
       <c r="C13" t="s">
         <v>763</v>
       </c>
-      <c r="D13" s="147" t="s">
+      <c r="D13" s="151" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
@@ -8993,13 +8990,13 @@
       <c r="A14" s="29">
         <v>11</v>
       </c>
-      <c r="B14" s="149" t="s">
+      <c r="B14" s="147" t="s">
         <v>761</v>
       </c>
       <c r="C14" t="s">
         <v>763</v>
       </c>
-      <c r="D14" s="147" t="s">
+      <c r="D14" s="151" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
@@ -9016,13 +9013,13 @@
       <c r="A15" s="29">
         <v>12</v>
       </c>
-      <c r="B15" s="149" t="s">
+      <c r="B15" s="147" t="s">
         <v>761</v>
       </c>
       <c r="C15" t="s">
         <v>763</v>
       </c>
-      <c r="D15" s="148" t="s">
+      <c r="D15" s="152" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
@@ -9158,7 +9155,7 @@
       <c r="A23" s="29">
         <v>20</v>
       </c>
-      <c r="B23" s="149" t="s">
+      <c r="B23" s="147" t="s">
         <v>767</v>
       </c>
       <c r="D23" s="84" t="s">
@@ -9175,7 +9172,7 @@
       <c r="A24" s="29">
         <v>21</v>
       </c>
-      <c r="B24" s="149" t="s">
+      <c r="B24" s="147" t="s">
         <v>767</v>
       </c>
       <c r="D24" s="85" t="s">
@@ -9192,7 +9189,7 @@
       <c r="A25" s="29">
         <v>22</v>
       </c>
-      <c r="B25" s="149" t="s">
+      <c r="B25" s="147" t="s">
         <v>767</v>
       </c>
       <c r="D25" s="85" t="s">
@@ -9209,7 +9206,7 @@
       <c r="A26" s="29">
         <v>23</v>
       </c>
-      <c r="B26" s="149" t="s">
+      <c r="B26" s="147" t="s">
         <v>768</v>
       </c>
       <c r="D26" s="85" t="s">
@@ -9226,7 +9223,7 @@
       <c r="A27" s="29">
         <v>24</v>
       </c>
-      <c r="B27" s="149" t="s">
+      <c r="B27" s="147" t="s">
         <v>768</v>
       </c>
       <c r="D27" s="85" t="s">
@@ -9243,7 +9240,7 @@
       <c r="A28" s="29">
         <v>25</v>
       </c>
-      <c r="B28" s="149" t="s">
+      <c r="B28" s="147" t="s">
         <v>768</v>
       </c>
       <c r="D28" s="83" t="s">
@@ -9260,7 +9257,7 @@
       <c r="A29" s="29">
         <v>26</v>
       </c>
-      <c r="B29" s="149" t="s">
+      <c r="B29" s="147" t="s">
         <v>768</v>
       </c>
       <c r="D29" s="83" t="s">
@@ -9277,7 +9274,7 @@
       <c r="A30" s="29">
         <v>27</v>
       </c>
-      <c r="B30" s="149" t="s">
+      <c r="B30" s="147" t="s">
         <v>768</v>
       </c>
       <c r="D30" s="83" t="s">

</xml_diff>

<commit_message>
Updated code on timestamp:   23-09-2021 - 15:08:16.28
</commit_message>
<xml_diff>
--- a/QuestionList_Level1.xlsx
+++ b/QuestionList_Level1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714E0C11-ED01-40A1-8FEC-54AAE080CCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9090" tabRatio="852" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="852" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="11" r:id="rId1"/>
@@ -22,7 +23,6 @@
     <sheet name="Graph" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="769">
   <si>
     <t>TOPIC</t>
   </si>
@@ -2880,7 +2880,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3702,20 +3702,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3767,7 +3767,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3805,7 +3811,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4093,11 +4105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4114,10 +4126,10 @@
       <c r="C2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="148" t="s">
+      <c r="F2" s="151" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="148"/>
+      <c r="G2" s="151"/>
       <c r="J2" s="102" t="s">
         <v>325</v>
       </c>
@@ -4290,9 +4302,9 @@
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" display="https://www.geeksforgeeks.org/java-tricks-competitive-programming-java-8/"/>
-    <hyperlink ref="J5" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/"/>
-    <hyperlink ref="C23" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
+    <hyperlink ref="J3" r:id="rId1" display="https://www.geeksforgeeks.org/java-tricks-competitive-programming-java-8/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J5" r:id="rId2" display="https://www.geeksforgeeks.org/fast-io-in-java-in-competitive-programming/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C23" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -4301,7 +4313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4758,27 +4770,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C38" r:id="rId1" display="https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/"/>
-    <hyperlink ref="I4" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
-    <hyperlink ref="I6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
-    <hyperlink ref="I5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java"/>
-    <hyperlink ref="I7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java"/>
-    <hyperlink ref="I9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java"/>
-    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java"/>
-    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java"/>
-    <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java"/>
-    <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java"/>
-    <hyperlink ref="I14" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java"/>
-    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java"/>
-    <hyperlink ref="I15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java"/>
-    <hyperlink ref="I16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java"/>
-    <hyperlink ref="I19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java"/>
-    <hyperlink ref="I18" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java"/>
-    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java"/>
-    <hyperlink ref="I21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java"/>
-    <hyperlink ref="I22" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java"/>
-    <hyperlink ref="I23" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java"/>
-    <hyperlink ref="I13" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java"/>
+    <hyperlink ref="C38" r:id="rId1" display="https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="I6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/BinaryTreeConstruction.java" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/SizeMinMaxHgt.java" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="I9" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LevelOrderTraversal.java" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/Traversal.java" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IterativePrePostInOrderinBT.java" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="I11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/NodeToRootPath.java" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="I12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKlevelDown.java" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="I14" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RootToleafPathSumInRange.java" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
+    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintSingleChildNode.java" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
+    <hyperlink ref="I15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformNormalToLeftClone.java" xr:uid="{00000000-0004-0000-0900-00000C000000}"/>
+    <hyperlink ref="I16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TransformLeftCloneToNormal.java" xr:uid="{00000000-0004-0000-0900-00000D000000}"/>
+    <hyperlink ref="I19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/DiameterOfBT.java" xr:uid="{00000000-0004-0000-0900-00000E000000}"/>
+    <hyperlink ref="I18" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/RemoveLeaves.java" xr:uid="{00000000-0004-0000-0900-00000F000000}"/>
+    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/TiltABT.java" xr:uid="{00000000-0004-0000-0900-000010000000}"/>
+    <hyperlink ref="I21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBinarySearchTree.java" xr:uid="{00000000-0004-0000-0900-000011000000}"/>
+    <hyperlink ref="I22" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/IsBalancesBST.java" xr:uid="{00000000-0004-0000-0900-000012000000}"/>
+    <hyperlink ref="I23" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/LargestBSTSubtree.java" xr:uid="{00000000-0004-0000-0900-000013000000}"/>
+    <hyperlink ref="I13" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/7.BinaryTree/PrintKDistanceAwaynode.java" xr:uid="{00000000-0004-0000-0900-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
@@ -4786,10 +4798,10 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
@@ -4979,20 +4991,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/AddNodeToBST.java"/>
-    <hyperlink ref="I10" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/LcaInBST.java"/>
-    <hyperlink ref="I9" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/ReplaceNodeSumOfLargerValue.java"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/SizeMinMaxFindSum.java"/>
-    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/PrintInRangeInBST.java"/>
-    <hyperlink ref="I8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/RemoveNodeFromBST.java"/>
-    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/TargetSumPair.java"/>
+    <hyperlink ref="I7" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/AddNodeToBST.java" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="I10" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/LcaInBST.java" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="I9" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/ReplaceNodeSumOfLargerValue.java" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/SizeMinMaxFindSum.java" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/PrintInRangeInBST.java" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="I8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/RemoveNodeFromBST.java" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/8.BST/TargetSumPair.java" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5259,24 +5271,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java"/>
-    <hyperlink ref="J7" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java"/>
-    <hyperlink ref="J4" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java"/>
-    <hyperlink ref="J5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java"/>
-    <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java"/>
-    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java"/>
-    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java"/>
-    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java"/>
-    <hyperlink ref="J15" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java"/>
-    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java"/>
-    <hyperlink ref="J13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java"/>
+    <hyperlink ref="J6" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements.java" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="J7" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GetCommonElements2.java" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HashMapUsage.java" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="J5" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/HighestFrequencyCharacter.java" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="J8" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/LongestConsecutiveSequenceOfElements.java" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
+    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/KLargestElement.java" xr:uid="{00000000-0004-0000-0B00-000005000000}"/>
+    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/SortKUnSorted.java" xr:uid="{00000000-0004-0000-0B00-000006000000}"/>
+    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MedianPriorityQ.java" xr:uid="{00000000-0004-0000-0B00-000007000000}"/>
+    <hyperlink ref="J15" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/GenericHM.java" xr:uid="{00000000-0004-0000-0B00-000008000000}"/>
+    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/CustomPriorityQueue.java" xr:uid="{00000000-0004-0000-0B00-000009000000}"/>
+    <hyperlink ref="J13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/9.HashMapAndHeap/MergeKSortedList.java" xr:uid="{00000000-0004-0000-0B00-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5690,27 +5702,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HasPath.java"/>
-    <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java"/>
-    <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java"/>
-    <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java"/>
-    <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java"/>
-    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/NumberOfIsland.java"/>
-    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PerfectFriends.java"/>
-    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HamiltonianPathAndCycle.java"/>
-    <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java"/>
-    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/BFS.java"/>
-    <hyperlink ref="J15" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphCyclic.java"/>
-    <hyperlink ref="J16" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphBipartite.java"/>
-    <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java"/>
-    <hyperlink ref="J18" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Dijkstra.java"/>
-    <hyperlink ref="J19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Prims.java"/>
-    <hyperlink ref="C22" r:id="rId16" display="https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1"/>
-    <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/OrderOfcompilation.java"/>
-    <hyperlink ref="J21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IterativeDFS.java"/>
-    <hyperlink ref="C23" r:id="rId19" display="https://leetcode.com/problems/rotting-oranges/"/>
-    <hyperlink ref="C24" r:id="rId20" display="https://leetcode.com/problems/evaluate-division/"/>
-    <hyperlink ref="C25" r:id="rId21" display="https://leetcode.com/problems/course-schedule/"/>
+    <hyperlink ref="J5" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HasPath.java" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="J6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PrintAllPath.java" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="J7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Multisolver_Smallest_Longest_Ceil_Floor_KthlargestPath.java" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="J8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/GetConnectedComponent.java" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
+    <hyperlink ref="J9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphConnected.java" xr:uid="{00000000-0004-0000-0C00-000004000000}"/>
+    <hyperlink ref="J10" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/NumberOfIsland.java" xr:uid="{00000000-0004-0000-0C00-000005000000}"/>
+    <hyperlink ref="J11" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/PerfectFriends.java" xr:uid="{00000000-0004-0000-0C00-000006000000}"/>
+    <hyperlink ref="J12" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/HamiltonianPathAndCycle.java" xr:uid="{00000000-0004-0000-0C00-000007000000}"/>
+    <hyperlink ref="J13" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightsTour.java" xr:uid="{00000000-0004-0000-0C00-000008000000}"/>
+    <hyperlink ref="J14" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/BFS.java" xr:uid="{00000000-0004-0000-0C00-000009000000}"/>
+    <hyperlink ref="J15" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphCyclic.java" xr:uid="{00000000-0004-0000-0C00-00000A000000}"/>
+    <hyperlink ref="J16" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IsGraphBipartite.java" xr:uid="{00000000-0004-0000-0C00-00000B000000}"/>
+    <hyperlink ref="J17" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/SpreadOfInfection.java" xr:uid="{00000000-0004-0000-0C00-00000C000000}"/>
+    <hyperlink ref="J18" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Dijkstra.java" xr:uid="{00000000-0004-0000-0C00-00000D000000}"/>
+    <hyperlink ref="J19" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/Prims.java" xr:uid="{00000000-0004-0000-0C00-00000E000000}"/>
+    <hyperlink ref="C22" r:id="rId16" display="https://practice.geeksforgeeks.org/problems/detect-cycle-in-a-directed-graph/1" xr:uid="{00000000-0004-0000-0C00-00000F000000}"/>
+    <hyperlink ref="J20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/OrderOfcompilation.java" xr:uid="{00000000-0004-0000-0C00-000010000000}"/>
+    <hyperlink ref="J21" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/10.Graph/IterativeDFS.java" xr:uid="{00000000-0004-0000-0C00-000011000000}"/>
+    <hyperlink ref="C23" r:id="rId19" display="https://leetcode.com/problems/rotting-oranges/" xr:uid="{00000000-0004-0000-0C00-000012000000}"/>
+    <hyperlink ref="C24" r:id="rId20" display="https://leetcode.com/problems/evaluate-division/" xr:uid="{00000000-0004-0000-0C00-000013000000}"/>
+    <hyperlink ref="C25" r:id="rId21" display="https://leetcode.com/problems/course-schedule/" xr:uid="{00000000-0004-0000-0C00-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
@@ -5718,7 +5730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5950,19 +5962,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://leetcode.com/problems/maximum-distance-between-a-pair-of-values/"/>
-    <hyperlink ref="D7" r:id="rId2" display="https://www.hackerrank.com/challenges/recursive-digit-sum/problem?h_l=interview&amp;playlist_slugs%5B%5D=interview-preparation-kit&amp;playlist_slugs%5B%5D=recursion-backtracking"/>
-    <hyperlink ref="I7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/HackerRankRecursiveDigit_sum.java"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.java"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.txt"/>
-    <hyperlink ref="D8" r:id="rId6" display="https://www.hackerrank.com/contests/tsp1tsp2-test1/challenges/pep-combination-sum/problem"/>
-    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/HackerRankCombinationSum.java"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://leetcode.com/problems/longest-string-chain/"/>
-    <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_longest_string_chain_Recursive_approach.java"/>
-    <hyperlink ref="D10" r:id="rId10" display="https://leetcode.com/problems/coin-change/"/>
-    <hyperlink ref="I10" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_coinchange.java"/>
-    <hyperlink ref="D11" r:id="rId12" display="https://leetcode.com/problems/find-and-replace-pattern/"/>
-    <hyperlink ref="I11" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/3.leetcode-premium-master/LeetCode/Leet_890.java"/>
+    <hyperlink ref="D5" r:id="rId1" display="https://leetcode.com/problems/maximum-distance-between-a-pair-of-values/" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId2" display="https://www.hackerrank.com/challenges/recursive-digit-sum/problem?h_l=interview&amp;playlist_slugs%5B%5D=interview-preparation-kit&amp;playlist_slugs%5B%5D=recursion-backtracking" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/HackerRankRecursiveDigit_sum.java" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.java" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/PinBall.txt" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://www.hackerrank.com/contests/tsp1tsp2-test1/challenges/pep-combination-sum/problem" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/HackerRankCombinationSum.java" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" display="https://leetcode.com/problems/longest-string-chain/" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_longest_string_chain_Recursive_approach.java" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D10" r:id="rId10" display="https://leetcode.com/problems/coin-change/" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I10" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/Leet_coinchange.java" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D11" r:id="rId12" display="https://leetcode.com/problems/find-and-replace-pattern/" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I11" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/3.leetcode-premium-master/LeetCode/Leet_890.java" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -5970,11 +5982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6196,6 +6208,9 @@
       <c r="D9" s="41" t="s">
         <v>81</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G9" s="2">
         <v>2</v>
       </c>
@@ -6286,9 +6301,6 @@
       <c r="E12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G12" s="2">
         <v>2</v>
       </c>
@@ -6315,9 +6327,6 @@
       <c r="E13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G13" s="2">
         <v>2</v>
       </c>
@@ -6347,9 +6356,6 @@
       <c r="E14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
@@ -6379,9 +6385,6 @@
       <c r="E15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" s="2">
         <v>2</v>
       </c>
@@ -6405,9 +6408,6 @@
       <c r="E16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
@@ -6431,9 +6431,6 @@
       <c r="E17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" s="2">
         <v>2</v>
       </c>
@@ -6460,9 +6457,6 @@
       <c r="E18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G18" s="2">
         <v>0</v>
       </c>
@@ -6489,9 +6483,6 @@
       <c r="E19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G19" s="2">
         <v>0</v>
       </c>
@@ -6515,9 +6506,6 @@
       <c r="E20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G20" s="2">
         <v>0</v>
       </c>
@@ -6541,9 +6529,6 @@
       <c r="E21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G21" s="2">
         <v>0</v>
       </c>
@@ -6567,9 +6552,6 @@
       <c r="E22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G22" s="2">
         <v>0</v>
       </c>
@@ -6593,9 +6575,6 @@
       <c r="E23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G23" s="2">
         <v>0</v>
       </c>
@@ -6625,9 +6604,6 @@
       <c r="E24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G24" s="2">
         <v>0</v>
       </c>
@@ -6657,9 +6633,6 @@
       <c r="E25" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G25" s="2">
         <v>1</v>
       </c>
@@ -6686,9 +6659,6 @@
       <c r="E26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G26" s="2">
         <v>1</v>
       </c>
@@ -6715,9 +6685,6 @@
       <c r="E27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" s="2">
         <v>1</v>
       </c>
@@ -6747,9 +6714,6 @@
       <c r="E28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G28" s="2">
         <v>1</v>
       </c>
@@ -6776,9 +6740,6 @@
       <c r="E29" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G29" s="2">
         <v>1</v>
       </c>
@@ -6808,9 +6769,6 @@
       <c r="E30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" s="2">
         <v>3</v>
       </c>
@@ -6840,9 +6798,6 @@
       <c r="E31" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G31" s="2">
         <v>3</v>
       </c>
@@ -6872,9 +6827,6 @@
       <c r="E32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G32" s="2">
         <v>2</v>
       </c>
@@ -6918,9 +6870,6 @@
       <c r="E34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G34" s="2">
         <v>2</v>
       </c>
@@ -6955,38 +6904,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Recursion.pdf"/>
-    <hyperlink ref="K4" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintDecreasing.java"/>
-    <hyperlink ref="K5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintIncreasing.java"/>
-    <hyperlink ref="K6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintIncreasingDecreasing.java"/>
-    <hyperlink ref="K7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/Factorial.java"/>
-    <hyperlink ref="K8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PowerLinear.java"/>
-    <hyperlink ref="K9" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PowerLog.java"/>
-    <hyperlink ref="K10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintZigZag.java"/>
-    <hyperlink ref="K11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/TowerOfHanoi.java"/>
-    <hyperlink ref="K12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/DisplayArr.java"/>
-    <hyperlink ref="K13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/DisplayReverse.java"/>
-    <hyperlink ref="K14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/MaxOfArr.java"/>
-    <hyperlink ref="K15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/FirstIndex.java"/>
-    <hyperlink ref="K16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/LastIndex.java"/>
-    <hyperlink ref="K17" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/AllIndices.java"/>
-    <hyperlink ref="K30" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/FloodFill.java"/>
-    <hyperlink ref="K34" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightTraversal.java"/>
-    <hyperlink ref="K33" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenOptionLevelApproach.java"/>
-    <hyperlink ref="K32" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenSubsetApproach.java"/>
-    <hyperlink ref="K31" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/TargetSumSubset.java"/>
-    <hyperlink ref="K29" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintEncodings.java"/>
-    <hyperlink ref="K24" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintKPC.java"/>
-    <hyperlink ref="K25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintStairPath.java"/>
-    <hyperlink ref="K26" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePath.java"/>
-    <hyperlink ref="K27" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePathWithJumps.java"/>
-    <hyperlink ref="K28" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintPermutation.java"/>
-    <hyperlink ref="K23" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintSubsequences.java"/>
-    <hyperlink ref="K21" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazePath.java"/>
-    <hyperlink ref="K22" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazepathJumps.java"/>
-    <hyperlink ref="K20" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetStairPaths.java"/>
-    <hyperlink ref="K18" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetSubsequence.java"/>
-    <hyperlink ref="K19" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/kpc.java"/>
+    <hyperlink ref="E1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Recursion.pdf" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="K4" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintDecreasing.java" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="K5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintIncreasing.java" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="K6" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintIncreasingDecreasing.java" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="K7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/Factorial.java" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="K8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PowerLinear.java" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="K9" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PowerLog.java" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="K10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/PrintZigZag.java" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="K11" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/intro/TowerOfHanoi.java" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="K12" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/DisplayArr.java" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="K13" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/DisplayReverse.java" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="K14" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/MaxOfArr.java" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="K15" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/FirstIndex.java" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="K16" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/LastIndex.java" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="K17" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion in arrrays/AllIndices.java" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="K30" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/FloodFill.java" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="K34" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/KnightTraversal.java" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="K33" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenOptionLevelApproach.java" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="K32" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/NQueenSubsetApproach.java" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="K31" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with backtracking/TargetSumSubset.java" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="K29" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintEncodings.java" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="K24" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintKPC.java" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="K25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintStairPath.java" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="K26" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePath.java" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="K27" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintMazePathWithJumps.java" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="K28" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintPermutation.java" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="K23" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/PrintSubsequences.java" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="K21" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazePath.java" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="K22" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetMazepathJumps.java" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="K20" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetStairPaths.java" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="K18" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/GetSubsequence.java" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="K19" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/2.Recursion And Backtracking/recursion with arraylist/kpc.java" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId33"/>
@@ -6994,10 +6943,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -7499,23 +7448,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf"/>
-    <hyperlink ref="I6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java"/>
-    <hyperlink ref="I7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java"/>
-    <hyperlink ref="I8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java"/>
-    <hyperlink ref="I9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java"/>
-    <hyperlink ref="I11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java"/>
-    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java"/>
-    <hyperlink ref="I13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java"/>
-    <hyperlink ref="I14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java"/>
-    <hyperlink ref="I15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java"/>
-    <hyperlink ref="I16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java"/>
-    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java"/>
-    <hyperlink ref="I18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java"/>
-    <hyperlink ref="I19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java"/>
-    <hyperlink ref="I21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java"/>
-    <hyperlink ref="I22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java"/>
-    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Searching%26Sorting.pdf" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sort01.java" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/Sorto12.java" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="I8" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeTwoSortedArr.java" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="I9" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/MergeSort.java" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="I11" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SeiveOfErathothenes.java" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="I12" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PartitionOfArray.java" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="I13" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSort.java" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="I14" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/QuickSelect.java" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="I15" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/TargetSumPair.java" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="I16" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/PivotInSortedAndRotatedArray.java" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="I17" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BubbleSort.java" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="I18" r:id="rId13" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/SelectionSort.java" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="I19" r:id="rId14" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/InsertionSort.java" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="I21" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSort.java" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="I22" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/CountSortStability.java" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="I20" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/3.TimeComplexity/BaseCountSort.java" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>
@@ -7523,11 +7472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7617,9 +7566,6 @@
       <c r="C5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="2">
         <v>5</v>
       </c>
@@ -7643,9 +7589,6 @@
       <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="2">
         <v>5</v>
       </c>
@@ -7669,9 +7612,6 @@
       <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
@@ -7695,9 +7635,6 @@
       <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="2">
         <v>5</v>
       </c>
@@ -7721,9 +7658,6 @@
       <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -7744,9 +7678,7 @@
       <c r="C10" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="69" t="s">
-        <v>34</v>
-      </c>
+      <c r="D10" s="69"/>
       <c r="E10" s="70">
         <v>5</v>
       </c>
@@ -7767,9 +7699,6 @@
       <c r="C11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
@@ -7796,9 +7725,6 @@
       <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E12" s="2">
         <v>3</v>
       </c>
@@ -7822,9 +7748,6 @@
       <c r="C13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E13" s="2">
         <v>3</v>
       </c>
@@ -7848,9 +7771,7 @@
       <c r="C14" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="69" t="s">
-        <v>34</v>
-      </c>
+      <c r="D14" s="69"/>
       <c r="E14" s="70">
         <v>3</v>
       </c>
@@ -7874,9 +7795,6 @@
       <c r="C15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E15" s="2">
         <v>3</v>
       </c>
@@ -7900,9 +7818,6 @@
       <c r="C16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E16" s="2">
         <v>3</v>
       </c>
@@ -7923,9 +7838,6 @@
       <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E17" s="2">
         <v>3</v>
       </c>
@@ -7946,9 +7858,6 @@
       <c r="C18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" s="2">
         <v>3</v>
       </c>
@@ -7969,9 +7878,6 @@
       <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" s="2">
         <v>3</v>
       </c>
@@ -7989,9 +7895,6 @@
       <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E20" s="2">
         <v>3</v>
       </c>
@@ -8018,9 +7921,7 @@
       <c r="C21" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="66" t="s">
-        <v>34</v>
-      </c>
+      <c r="D21" s="66"/>
       <c r="E21" s="67">
         <v>3</v>
       </c>
@@ -8394,44 +8295,44 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf"/>
-    <hyperlink ref="B34" r:id="rId2" display="https://leetcode.com/problems/daily-temperatures/"/>
-    <hyperlink ref="B35" r:id="rId3" display="https://leetcode.com/problems/next-greater-element-ii/"/>
-    <hyperlink ref="B36" r:id="rId4" display="https://leetcode.com/problems/next-greater-element-i/"/>
-    <hyperlink ref="B37" r:id="rId5" display="https://leetcode.com/problems/maximal-rectangle/"/>
-    <hyperlink ref="B38" r:id="rId6" display="https://leetcode.com/problems/maximal-rectangle/"/>
-    <hyperlink ref="B39" r:id="rId7" display="https://leetcode.com/problems/sliding-window-maximum/submissions/"/>
-    <hyperlink ref="B41" r:id="rId8" display="https://leetcode.com/problems/basic-calculator/"/>
-    <hyperlink ref="B40" r:id="rId9" display="https://leetcode.com/problems/basic-calculator-ii/"/>
-    <hyperlink ref="B42" r:id="rId10" display="https://leetcode.com/problems/longest-valid-parentheses/"/>
-    <hyperlink ref="B43" r:id="rId11" display="https://leetcode.com/problems/container-with-most-water/"/>
-    <hyperlink ref="B44" r:id="rId12" display="https://leetcode.com/problems/simplify-path/"/>
-    <hyperlink ref="B45" r:id="rId13" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string-ii/"/>
-    <hyperlink ref="B46" r:id="rId14" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/"/>
-    <hyperlink ref="B47" r:id="rId15" display="https://leetcode.com/problems/maximum-frequency-stack/"/>
-    <hyperlink ref="H20" r:id="rId16" display="https://leetcode.com/problems/min-stack/"/>
-    <hyperlink ref="B48" r:id="rId17" display="https://leetcode.com/problems/trapping-rain-water/"/>
-    <hyperlink ref="B49" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/"/>
-    <hyperlink ref="G1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues"/>
-    <hyperlink ref="I5" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java"/>
-    <hyperlink ref="I8" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java"/>
-    <hyperlink ref="I9" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java"/>
-    <hyperlink ref="I10" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java"/>
-    <hyperlink ref="I6" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java"/>
-    <hyperlink ref="I15" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java"/>
-    <hyperlink ref="I16" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java"/>
-    <hyperlink ref="I13" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java"/>
-    <hyperlink ref="I14" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java"/>
-    <hyperlink ref="I11" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java"/>
-    <hyperlink ref="I12" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java"/>
-    <hyperlink ref="I17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java"/>
-    <hyperlink ref="I18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java"/>
-    <hyperlink ref="I19" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java"/>
-    <hyperlink ref="I20" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java"/>
-    <hyperlink ref="I21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java"/>
-    <hyperlink ref="B50" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/"/>
-    <hyperlink ref="I7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java"/>
-    <hyperlink ref="B51" r:id="rId38" display="https://leetcode.com/problems/validate-stack-sequences/"/>
+    <hyperlink ref="C1" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B34" r:id="rId2" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="B35" r:id="rId3" display="https://leetcode.com/problems/next-greater-element-ii/" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B36" r:id="rId4" display="https://leetcode.com/problems/next-greater-element-i/" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="B37" r:id="rId5" display="https://leetcode.com/problems/maximal-rectangle/" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="B38" r:id="rId6" display="https://leetcode.com/problems/maximal-rectangle/" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="B39" r:id="rId7" display="https://leetcode.com/problems/sliding-window-maximum/submissions/" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="B41" r:id="rId8" display="https://leetcode.com/problems/basic-calculator/" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="B40" r:id="rId9" display="https://leetcode.com/problems/basic-calculator-ii/" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="B42" r:id="rId10" display="https://leetcode.com/problems/longest-valid-parentheses/" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="B43" r:id="rId11" display="https://leetcode.com/problems/container-with-most-water/" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="B44" r:id="rId12" display="https://leetcode.com/problems/simplify-path/" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="B45" r:id="rId13" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string-ii/" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="B46" r:id="rId14" display="https://leetcode.com/problems/remove-all-adjacent-duplicates-in-string/" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="B47" r:id="rId15" display="https://leetcode.com/problems/maximum-frequency-stack/" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="H20" r:id="rId16" display="https://leetcode.com/problems/min-stack/" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="B48" r:id="rId17" display="https://leetcode.com/problems/trapping-rain-water/" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="B49" r:id="rId18" display="https://leetcode.com/problems/merge-intervals/" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="G1" r:id="rId19" display="https://github.com/spartan4cs/CP/tree/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="I5" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Duplicatebracket.java" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="I8" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/StockSpan.java" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="I9" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/LargestAreaHistogram.java" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="I10" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/SlidingWindowMax.java" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="I6" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/BalancedBracket.java" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="I15" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/CelebrityProblem.java" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="I16" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Merge_Overlapping_Interval.java" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="I13" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PostFixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="I14" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/PrefixEvaluationConversion.java" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="I11" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixEvaluation.java" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="I12" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/InfixConversion.java" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="I17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Smallest_Number_Following_Pattern.java" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="I18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NormalStack.java" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="I19" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/DynamicStack.java" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="I20" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStack.java" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="I21" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/MinimumStackConstantSpace.java" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="B50" r:id="rId36" display="https://leetcode.com/problems/valid-parentheses/" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="I7" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/NGETR.java" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="B51" r:id="rId38" display="https://leetcode.com/problems/validate-stack-sequences/" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId39"/>
@@ -8439,11 +8340,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="D4" sqref="D4:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8466,15 +8367,15 @@
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:9" s="72" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="152" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
       <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8516,9 +8417,7 @@
       <c r="C4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="2">
         <v>0</v>
       </c>
@@ -8558,9 +8457,7 @@
       <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="2">
         <v>0</v>
       </c>
@@ -8581,9 +8478,7 @@
       <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="2">
         <v>0</v>
       </c>
@@ -8604,9 +8499,7 @@
       <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="2">
         <v>0</v>
       </c>
@@ -8627,9 +8520,7 @@
       <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="2">
         <v>0</v>
       </c>
@@ -8650,9 +8541,7 @@
       <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="2">
         <v>0</v>
       </c>
@@ -8675,9 +8564,7 @@
       <c r="C11" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="74" t="s">
         <v>406</v>
@@ -8707,29 +8594,29 @@
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="https://auth.geeksforgeeks.org/?to=https%3A%2F%2Fpractice.geeksforgeeks.org%2Fproblems%2Fgenerate-binary-numbers-1587115620%2F1"/>
-    <hyperlink ref="C1" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java"/>
-    <hyperlink ref="I4" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java"/>
-    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java"/>
-    <hyperlink ref="I7" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java"/>
-    <hyperlink ref="I6" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java"/>
-    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java"/>
-    <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java"/>
-    <hyperlink ref="I8" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java"/>
-    <hyperlink ref="G10" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.geeksforgeeks.org/kth-smallestlargest-element-unsorted-array/"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://practice.geeksforgeeks.org/problems/minimize-the-heights3351/1"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://auth.geeksforgeeks.org/?to=https%3A%2F%2Fpractice.geeksforgeeks.org%2Fproblems%2Fgenerate-binary-numbers-1587115620%2F1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/Stacks and queues.pdf" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="I5" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/DynamicQueue.java" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="I4" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/NormalQueue.java" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/1.  Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/GFG_GenerateBinaryNumber.java" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PopEfficient.java" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="I6" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/QueueToStackAdapter_PushEfficient.java" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="I10" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/TwoStackInArray.java" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="I9" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackToQueueAdapter_RemoveEfficient.java" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="I8" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/4.StacksAnd Queues/Queue/StackTOQueueAdapter_AddEfficient.java" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="G10" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.geeksforgeeks.org/kth-smallestlargest-element-unsorted-array/" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://practice.geeksforgeeks.org/problems/minimize-the-heights3351/1" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D15"/>
     </sheetView>
   </sheetViews>
@@ -8913,7 +8800,7 @@
       <c r="B10" s="102" t="s">
         <v>759</v>
       </c>
-      <c r="D10" s="150" t="s">
+      <c r="D10" s="148" t="s">
         <v>184</v>
       </c>
       <c r="E10" t="s">
@@ -8933,7 +8820,7 @@
       <c r="C11" t="s">
         <v>762</v>
       </c>
-      <c r="D11" s="151" t="s">
+      <c r="D11" s="149" t="s">
         <v>185</v>
       </c>
       <c r="E11" t="s">
@@ -8953,7 +8840,7 @@
       <c r="C12" t="s">
         <v>762</v>
       </c>
-      <c r="D12" s="151" t="s">
+      <c r="D12" s="149" t="s">
         <v>186</v>
       </c>
       <c r="E12" t="s">
@@ -8973,7 +8860,7 @@
       <c r="C13" t="s">
         <v>763</v>
       </c>
-      <c r="D13" s="151" t="s">
+      <c r="D13" s="149" t="s">
         <v>187</v>
       </c>
       <c r="E13" t="s">
@@ -8996,7 +8883,7 @@
       <c r="C14" t="s">
         <v>763</v>
       </c>
-      <c r="D14" s="151" t="s">
+      <c r="D14" s="149" t="s">
         <v>188</v>
       </c>
       <c r="E14" t="s">
@@ -9019,7 +8906,7 @@
       <c r="C15" t="s">
         <v>763</v>
       </c>
-      <c r="D15" s="152" t="s">
+      <c r="D15" s="150" t="s">
         <v>189</v>
       </c>
       <c r="E15" t="s">
@@ -9330,18 +9217,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/longest-string-chain/"/>
+    <hyperlink ref="D38" r:id="rId1" display="https://leetcode.com/problems/longest-string-chain/" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9448,9 +9335,6 @@
       <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
       <c r="G9" s="5">
         <v>3</v>
       </c>
@@ -9468,9 +9352,6 @@
       <c r="E10" t="s">
         <v>33</v>
       </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
       <c r="G10" s="5">
         <v>3</v>
       </c>
@@ -9488,9 +9369,6 @@
       <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
       <c r="G11" s="5">
         <v>3</v>
       </c>
@@ -9508,9 +9386,6 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
-        <v>34</v>
-      </c>
       <c r="G12" s="5">
         <v>3</v>
       </c>
@@ -9528,9 +9403,6 @@
       <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" t="s">
-        <v>34</v>
-      </c>
       <c r="G13" s="5">
         <v>3</v>
       </c>
@@ -9548,9 +9420,6 @@
       <c r="E14" t="s">
         <v>33</v>
       </c>
-      <c r="F14" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="5">
         <v>3</v>
       </c>
@@ -9568,9 +9437,6 @@
       <c r="E15" t="s">
         <v>33</v>
       </c>
-      <c r="F15" t="s">
-        <v>34</v>
-      </c>
       <c r="G15" s="5">
         <v>3</v>
       </c>
@@ -9588,9 +9454,6 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
       <c r="G16" s="5">
         <v>3</v>
       </c>
@@ -9608,9 +9471,6 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" s="5">
         <v>3</v>
       </c>
@@ -9634,9 +9494,6 @@
       <c r="E18" t="s">
         <v>33</v>
       </c>
-      <c r="F18" t="s">
-        <v>34</v>
-      </c>
       <c r="G18" s="5">
         <v>3</v>
       </c>
@@ -9657,9 +9514,6 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" t="s">
-        <v>34</v>
-      </c>
       <c r="G19" s="5">
         <v>3</v>
       </c>
@@ -9680,9 +9534,6 @@
       <c r="E20" t="s">
         <v>33</v>
       </c>
-      <c r="F20" t="s">
-        <v>34</v>
-      </c>
       <c r="G20" s="5">
         <v>3</v>
       </c>
@@ -9703,9 +9554,6 @@
       <c r="E21" t="s">
         <v>33</v>
       </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
       <c r="G21" s="5">
         <v>3</v>
       </c>
@@ -9726,9 +9574,6 @@
       <c r="E22" t="s">
         <v>33</v>
       </c>
-      <c r="F22" t="s">
-        <v>34</v>
-      </c>
       <c r="G22" s="5">
         <v>3</v>
       </c>
@@ -9749,9 +9594,6 @@
       <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="F23" t="s">
-        <v>34</v>
-      </c>
       <c r="G23" s="5">
         <v>3</v>
       </c>
@@ -9778,9 +9620,6 @@
       <c r="E24" t="s">
         <v>33</v>
       </c>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
       <c r="G24" s="5">
         <v>3</v>
       </c>
@@ -9798,9 +9637,6 @@
       <c r="E25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" t="s">
-        <v>34</v>
-      </c>
       <c r="G25" s="5">
         <v>3</v>
       </c>
@@ -9821,9 +9657,6 @@
       <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="F26" t="s">
-        <v>34</v>
-      </c>
       <c r="G26" s="5">
         <v>3</v>
       </c>
@@ -9841,9 +9674,6 @@
       <c r="E27" t="s">
         <v>33</v>
       </c>
-      <c r="F27" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" s="5">
         <v>3</v>
       </c>
@@ -9861,9 +9691,6 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" t="s">
-        <v>34</v>
-      </c>
       <c r="G28" s="5">
         <v>3</v>
       </c>
@@ -9881,9 +9708,6 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29" t="s">
-        <v>34</v>
-      </c>
       <c r="G29" s="5">
         <v>3</v>
       </c>
@@ -9901,9 +9725,6 @@
       <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" s="5">
         <v>3</v>
       </c>
@@ -9924,9 +9745,6 @@
       <c r="E31" t="s">
         <v>33</v>
       </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
       <c r="G31" s="5">
         <v>3</v>
       </c>
@@ -9953,9 +9771,6 @@
       <c r="E32" t="s">
         <v>33</v>
       </c>
-      <c r="F32" t="s">
-        <v>34</v>
-      </c>
       <c r="G32" s="5">
         <v>3</v>
       </c>
@@ -9979,9 +9794,6 @@
       <c r="E33" t="s">
         <v>33</v>
       </c>
-      <c r="F33" t="s">
-        <v>34</v>
-      </c>
       <c r="G33" s="5">
         <v>3</v>
       </c>
@@ -10004,9 +9816,6 @@
       </c>
       <c r="E34" t="s">
         <v>33</v>
-      </c>
-      <c r="F34" t="s">
-        <v>34</v>
       </c>
       <c r="G34" s="5">
         <v>3</v>
@@ -10160,49 +9969,49 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K9" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K10" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K11" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K12" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K13" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K14" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K15" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="K16" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java"/>
-    <hyperlink ref="H23" r:id="rId10" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
-    <hyperlink ref="K23" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java"/>
-    <hyperlink ref="K24" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java"/>
-    <hyperlink ref="H25" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D47" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/"/>
-    <hyperlink ref="I17" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D44" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/"/>
-    <hyperlink ref="D40" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/"/>
-    <hyperlink ref="D38" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/"/>
-    <hyperlink ref="D42" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/"/>
-    <hyperlink ref="D43" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/"/>
-    <hyperlink ref="D46" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/"/>
-    <hyperlink ref="D41" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/"/>
-    <hyperlink ref="D45" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/"/>
-    <hyperlink ref="H43" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs"/>
-    <hyperlink ref="K26" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java"/>
-    <hyperlink ref="K25" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java"/>
-    <hyperlink ref="K19" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java"/>
-    <hyperlink ref="K20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java"/>
-    <hyperlink ref="K21" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java"/>
-    <hyperlink ref="K22" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java"/>
-    <hyperlink ref="K17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java"/>
-    <hyperlink ref="K18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java"/>
-    <hyperlink ref="K27" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java"/>
-    <hyperlink ref="K28" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java"/>
-    <hyperlink ref="K29" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java"/>
-    <hyperlink ref="K30" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java"/>
-    <hyperlink ref="K31" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java"/>
-    <hyperlink ref="D49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/"/>
-    <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/"/>
-    <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/"/>
-    <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java"/>
-    <hyperlink ref="K33" r:id="rId42" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java"/>
-    <hyperlink ref="K34" r:id="rId43" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java"/>
+    <hyperlink ref="K8" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="K9" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="K10" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="K11" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="K12" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="K13" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="K14" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="K15" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="K16" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinkListCreationDemo.java" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="H23" r:id="rId10" display="https://leetcode.com/problems/merge-two-sorted-lists/" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="K23" r:id="rId11" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Leet_mergeTwoSorterLinklist.java" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
+    <hyperlink ref="K24" r:id="rId12" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistMergeSort.java" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
+    <hyperlink ref="H25" r:id="rId13" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{00000000-0004-0000-0700-00000C000000}"/>
+    <hyperlink ref="D47" r:id="rId14" display="https://leetcode.com/problems/remove-duplicates-from-an-unsorted-linked-list/" xr:uid="{00000000-0004-0000-0700-00000D000000}"/>
+    <hyperlink ref="I17" r:id="rId15" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{00000000-0004-0000-0700-00000E000000}"/>
+    <hyperlink ref="D44" r:id="rId16" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/" xr:uid="{00000000-0004-0000-0700-00000F000000}"/>
+    <hyperlink ref="D40" r:id="rId17" display="https://leetcode.com/problems/merge-two-sorted-lists/" xr:uid="{00000000-0004-0000-0700-000010000000}"/>
+    <hyperlink ref="D38" r:id="rId18" display="https://leetcode.com/problems/reverse-linked-list/" xr:uid="{00000000-0004-0000-0700-000011000000}"/>
+    <hyperlink ref="D42" r:id="rId19" display="https://leetcode.com/problems/linked-list-cycle/" xr:uid="{00000000-0004-0000-0700-000012000000}"/>
+    <hyperlink ref="D43" r:id="rId20" display="https://leetcode.com/problems/linked-list-cycle-ii/" xr:uid="{00000000-0004-0000-0700-000013000000}"/>
+    <hyperlink ref="D46" r:id="rId21" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/" xr:uid="{00000000-0004-0000-0700-000014000000}"/>
+    <hyperlink ref="D41" r:id="rId22" display="https://leetcode.com/problems/palindrome-linked-list/" xr:uid="{00000000-0004-0000-0700-000015000000}"/>
+    <hyperlink ref="D45" r:id="rId23" display="https://leetcode.com/problems/add-two-numbers/" xr:uid="{00000000-0004-0000-0700-000016000000}"/>
+    <hyperlink ref="H43" r:id="rId24" display="https://www.youtube.com/watch?v=dpqpgnTHiLs" xr:uid="{00000000-0004-0000-0700-000017000000}"/>
+    <hyperlink ref="K26" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/OddEvenLinklist.java" xr:uid="{00000000-0004-0000-0700-000018000000}"/>
+    <hyperlink ref="K25" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/RemoveDuplicatesFromSortedLL.java" xr:uid="{00000000-0004-0000-0700-000019000000}"/>
+    <hyperlink ref="K19" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Linklist_To_Stack_Adapter.java" xr:uid="{00000000-0004-0000-0700-00001A000000}"/>
+    <hyperlink ref="K20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LinklistToQueueAdapter.java" xr:uid="{00000000-0004-0000-0700-00001B000000}"/>
+    <hyperlink ref="K21" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KthNodeFromEndOfLiklist.java" xr:uid="{00000000-0004-0000-0700-00001C000000}"/>
+    <hyperlink ref="K22" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/MidOfLinklist.java" xr:uid="{00000000-0004-0000-0700-00001D000000}"/>
+    <hyperlink ref="K17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Iterative.java" xr:uid="{00000000-0004-0000-0700-00001E000000}"/>
+    <hyperlink ref="K18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLinklist_Pointer.java" xr:uid="{00000000-0004-0000-0700-00001F000000}"/>
+    <hyperlink ref="K27" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/KReverseinLL.java" xr:uid="{00000000-0004-0000-0700-000020000000}"/>
+    <hyperlink ref="K28" r:id="rId34" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/DisplayReverseRecursive.java" xr:uid="{00000000-0004-0000-0700-000021000000}"/>
+    <hyperlink ref="K29" r:id="rId35" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/ReverseLL_Pointer_Recursive.java" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
+    <hyperlink ref="K30" r:id="rId36" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/LL_palindrome_Or_note.java" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
+    <hyperlink ref="K31" r:id="rId37" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/FoldALinkedList.java" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
+    <hyperlink ref="D49" r:id="rId38" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
+    <hyperlink ref="D48" r:id="rId39" display="https://leetcode.com/problems/intersection-of-two-linked-lists/" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
+    <hyperlink ref="D39" r:id="rId40" display="https://leetcode.com/problems/reverse-linked-list-ii/" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
+    <hyperlink ref="K32" r:id="rId41" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/Add2LinkedList.java" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
+    <hyperlink ref="K33" r:id="rId42" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/IntersectionPointOfLL.java" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
+    <hyperlink ref="K34" r:id="rId43" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/5.LinkedList/CopyLLwithRandomnumbers.java" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId44"/>
@@ -10210,7 +10019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -10927,39 +10736,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="J5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="J6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java"/>
-    <hyperlink ref="J9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java"/>
-    <hyperlink ref="J7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java"/>
-    <hyperlink ref="J8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java"/>
-    <hyperlink ref="J10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java"/>
-    <hyperlink ref="J11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java"/>
-    <hyperlink ref="J12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
-    <hyperlink ref="J13" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java"/>
-    <hyperlink ref="C47" r:id="rId11" display="https://leetcode.com/problems/n-ary-tree-level-order-traversal/"/>
-    <hyperlink ref="C48" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-n-ary-tree/"/>
-    <hyperlink ref="C49" r:id="rId13" display="https://leetcode.com/problems/n-ary-tree-preorder-traversal/"/>
-    <hyperlink ref="C50" r:id="rId14" display="https://leetcode.com/problems/n-ary-tree-postorder-traversal/"/>
-    <hyperlink ref="J15" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MirrorAGT.java"/>
-    <hyperlink ref="J27" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/PredessorAndSuccessorElement.java"/>
-    <hyperlink ref="J28" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/CeilAndFloor.java"/>
-    <hyperlink ref="J29" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/KthLargestInGT.java"/>
-    <hyperlink ref="J31" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/DiameterGT.java"/>
-    <hyperlink ref="J26" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Multisolver.java"/>
-    <hyperlink ref="J30" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxSumSubtree.java"/>
-    <hyperlink ref="J32" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/IterativePreorderPostorderGT.java"/>
-    <hyperlink ref="J25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreeSymmetric.java"/>
-    <hyperlink ref="J24" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java"/>
-    <hyperlink ref="J23" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesSimilarInShape.java"/>
-    <hyperlink ref="J22" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Distancebetween2Nodes.java"/>
-    <hyperlink ref="J21" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LowestCommonAncestor.java"/>
-    <hyperlink ref="J20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/NodeToRootPath.java"/>
-    <hyperlink ref="J19" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/FindElementInGenericTree.java"/>
-    <hyperlink ref="J16" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/RemoveLeavesInGT.java"/>
-    <hyperlink ref="J17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java"/>
-    <hyperlink ref="J18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java"/>
-    <hyperlink ref="J14" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java"/>
+    <hyperlink ref="J4" r:id="rId1" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="J5" r:id="rId2" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="J6" r:id="rId3" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/GenericTreeDemo.java" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="J9" r:id="rId4" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/HeightOfTree.java" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="J7" r:id="rId5" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/SizeOfGenericTree.java" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="J8" r:id="rId6" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxAndMinGenericTree.java" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="J10" r:id="rId7" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/TraversalInGenericTree.java" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="J11" r:id="rId8" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderTraversal.java" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="J12" r:id="rId9" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="J13" r:id="rId10" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseZigzag.java" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="C47" r:id="rId11" display="https://leetcode.com/problems/n-ary-tree-level-order-traversal/" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
+    <hyperlink ref="C48" r:id="rId12" display="https://leetcode.com/problems/maximum-depth-of-n-ary-tree/" xr:uid="{00000000-0004-0000-0800-00000B000000}"/>
+    <hyperlink ref="C49" r:id="rId13" display="https://leetcode.com/problems/n-ary-tree-preorder-traversal/" xr:uid="{00000000-0004-0000-0800-00000C000000}"/>
+    <hyperlink ref="C50" r:id="rId14" display="https://leetcode.com/problems/n-ary-tree-postorder-traversal/" xr:uid="{00000000-0004-0000-0800-00000D000000}"/>
+    <hyperlink ref="J15" r:id="rId15" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MirrorAGT.java" xr:uid="{00000000-0004-0000-0800-00000E000000}"/>
+    <hyperlink ref="J27" r:id="rId16" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/PredessorAndSuccessorElement.java" xr:uid="{00000000-0004-0000-0800-00000F000000}"/>
+    <hyperlink ref="J28" r:id="rId17" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/CeilAndFloor.java" xr:uid="{00000000-0004-0000-0800-000010000000}"/>
+    <hyperlink ref="J29" r:id="rId18" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/KthLargestInGT.java" xr:uid="{00000000-0004-0000-0800-000011000000}"/>
+    <hyperlink ref="J31" r:id="rId19" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/DiameterGT.java" xr:uid="{00000000-0004-0000-0800-000012000000}"/>
+    <hyperlink ref="J26" r:id="rId20" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Multisolver.java" xr:uid="{00000000-0004-0000-0800-000013000000}"/>
+    <hyperlink ref="J30" r:id="rId21" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/MaxSumSubtree.java" xr:uid="{00000000-0004-0000-0800-000014000000}"/>
+    <hyperlink ref="J32" r:id="rId22" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/IterativePreorderPostorderGT.java" xr:uid="{00000000-0004-0000-0800-000015000000}"/>
+    <hyperlink ref="J25" r:id="rId23" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreeSymmetric.java" xr:uid="{00000000-0004-0000-0800-000016000000}"/>
+    <hyperlink ref="J24" r:id="rId24" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesMirror.java" xr:uid="{00000000-0004-0000-0800-000017000000}"/>
+    <hyperlink ref="J23" r:id="rId25" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/AreTreesSimilarInShape.java" xr:uid="{00000000-0004-0000-0800-000018000000}"/>
+    <hyperlink ref="J22" r:id="rId26" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/Distancebetween2Nodes.java" xr:uid="{00000000-0004-0000-0800-000019000000}"/>
+    <hyperlink ref="J21" r:id="rId27" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LowestCommonAncestor.java" xr:uid="{00000000-0004-0000-0800-00001A000000}"/>
+    <hyperlink ref="J20" r:id="rId28" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/NodeToRootPath.java" xr:uid="{00000000-0004-0000-0800-00001B000000}"/>
+    <hyperlink ref="J19" r:id="rId29" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/FindElementInGenericTree.java" xr:uid="{00000000-0004-0000-0800-00001C000000}"/>
+    <hyperlink ref="J16" r:id="rId30" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/RemoveLeavesInGT.java" xr:uid="{00000000-0004-0000-0800-00001D000000}"/>
+    <hyperlink ref="J17" r:id="rId31" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java" xr:uid="{00000000-0004-0000-0800-00001E000000}"/>
+    <hyperlink ref="J18" r:id="rId32" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LinearizeGT.java" xr:uid="{00000000-0004-0000-0800-00001F000000}"/>
+    <hyperlink ref="J14" r:id="rId33" display="https://github.com/spartan4cs/CP/blob/main/2.Pepcoding/TSP2/Level1/6.GenericTree/LevelOrderLinewiseTraversal.java" xr:uid="{00000000-0004-0000-0800-000020000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>

</xml_diff>